<commit_message>
Le rapport du 21 Aout 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -28774,10 +28774,10 @@
         </is>
       </c>
       <c r="J507" s="1" t="n">
-        <v>28.083334</v>
+        <v>28.5</v>
       </c>
       <c r="K507" s="1" t="n">
-        <v>547625.0</v>
+        <v>555750.0</v>
       </c>
       <c r="L507" s="1"/>
       <c r="M507" s="1"/>

</xml_diff>

<commit_message>
Rapport du 23 Aout 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -13782,10 +13782,10 @@
         </is>
       </c>
       <c r="J243" s="1" t="n">
-        <v>10.708333</v>
+        <v>13.208333</v>
       </c>
       <c r="K243" s="1" t="n">
-        <v>257000.0</v>
+        <v>317000.0</v>
       </c>
       <c r="L243" s="1"/>
       <c r="M243" s="1"/>
@@ -13830,10 +13830,10 @@
         </is>
       </c>
       <c r="J244" s="1" t="n">
-        <v>8.5</v>
+        <v>10.0</v>
       </c>
       <c r="K244" s="1" t="n">
-        <v>165750.0</v>
+        <v>195000.0</v>
       </c>
       <c r="L244" s="1"/>
       <c r="M244" s="1"/>
@@ -43620,10 +43620,10 @@
         </is>
       </c>
       <c r="J772" s="1" t="n">
-        <v>46.0</v>
+        <v>45.5</v>
       </c>
       <c r="K772" s="1" t="n">
-        <v>471500.0</v>
+        <v>466375.0</v>
       </c>
       <c r="L772" s="1"/>
       <c r="M772" s="1"/>
@@ -43668,10 +43668,10 @@
         </is>
       </c>
       <c r="J773" s="1" t="n">
-        <v>23.5</v>
+        <v>23.0</v>
       </c>
       <c r="K773" s="1" t="n">
-        <v>458250.0</v>
+        <v>448500.0</v>
       </c>
       <c r="L773" s="1"/>
       <c r="M773" s="1"/>
@@ -43860,10 +43860,10 @@
         </is>
       </c>
       <c r="J777" s="1" t="n">
-        <v>19.0</v>
+        <v>17.75</v>
       </c>
       <c r="K777" s="1" t="n">
-        <v>456000.0</v>
+        <v>426000.0</v>
       </c>
       <c r="L777" s="1"/>
       <c r="M777" s="1"/>

</xml_diff>

<commit_message>
Rapport du 01 09
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -10409,10 +10409,10 @@
         </is>
       </c>
       <c r="J173" s="1" t="n">
-        <v>22.75</v>
+        <v>23.25</v>
       </c>
       <c r="K173" s="1" t="n">
-        <v>762125.0</v>
+        <v>778875.0</v>
       </c>
       <c r="L173" s="1"/>
       <c r="M173" s="1"/>
@@ -10505,10 +10505,10 @@
         </is>
       </c>
       <c r="J175" s="1" t="n">
-        <v>18.9</v>
+        <v>19.0</v>
       </c>
       <c r="K175" s="1" t="n">
-        <v>122850.0</v>
+        <v>123500.0</v>
       </c>
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
@@ -10841,10 +10841,10 @@
         </is>
       </c>
       <c r="J182" s="1" t="n">
-        <v>34.375</v>
+        <v>34.791668</v>
       </c>
       <c r="K182" s="1" t="n">
-        <v>601562.5</v>
+        <v>608854.2</v>
       </c>
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>

</xml_diff>

<commit_message>
Rapport du 02 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -5607,10 +5607,10 @@
         </is>
       </c>
       <c r="J98" s="1" t="n">
-        <v>24.166666</v>
+        <v>24.125</v>
       </c>
       <c r="K98" s="1" t="n">
-        <v>580000.0</v>
+        <v>579000.0</v>
       </c>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
@@ -5751,10 +5751,10 @@
         </is>
       </c>
       <c r="J101" s="1" t="n">
-        <v>19.2</v>
+        <v>19.3</v>
       </c>
       <c r="K101" s="1" t="n">
-        <v>235200.0</v>
+        <v>236425.0</v>
       </c>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>

</xml_diff>

<commit_message>
Rapport du 09 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -14925,10 +14925,10 @@
         </is>
       </c>
       <c r="J256" s="1" t="n">
-        <v>18.5</v>
+        <v>33.5</v>
       </c>
       <c r="K256" s="1" t="n">
-        <v>360750.0</v>
+        <v>653250.0</v>
       </c>
       <c r="L256" s="1"/>
       <c r="M256" s="1"/>
@@ -17649,10 +17649,10 @@
         </is>
       </c>
       <c r="J305" s="1" t="n">
-        <v>34.0</v>
+        <v>19.0</v>
       </c>
       <c r="K305" s="1" t="n">
-        <v>663000.0</v>
+        <v>370500.0</v>
       </c>
       <c r="L305" s="1"/>
       <c r="M305" s="1"/>

</xml_diff>

<commit_message>
Rapport du 10 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -7367,10 +7367,10 @@
         </is>
       </c>
       <c r="J125" s="1" t="n">
-        <v>5.2083335</v>
+        <v>5.1666665</v>
       </c>
       <c r="K125" s="1" t="n">
-        <v>91145.836</v>
+        <v>90416.664</v>
       </c>
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>

</xml_diff>

<commit_message>
Rapport du 11 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -34259,10 +34259,10 @@
         </is>
       </c>
       <c r="J593" s="1" t="n">
-        <v>33.5</v>
+        <v>58.5</v>
       </c>
       <c r="K593" s="1" t="n">
-        <v>653250.0</v>
+        <v>1140750.0</v>
       </c>
       <c r="L593" s="1"/>
       <c r="M593" s="1"/>
@@ -36983,10 +36983,10 @@
         </is>
       </c>
       <c r="J642" s="1" t="n">
-        <v>19.0</v>
+        <v>44.0</v>
       </c>
       <c r="K642" s="1" t="n">
-        <v>370500.0</v>
+        <v>858000.0</v>
       </c>
       <c r="L642" s="1"/>
       <c r="M642" s="1"/>

</xml_diff>

<commit_message>
Rapport du 12 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B4641E-1D29-4675-A224-729223DAE26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F738687-93CB-4948-A0E7-A449337998AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5290" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5242" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -278,9 +278,6 @@
   </si>
   <si>
     <t>Ndeye M SY</t>
-  </si>
-  <si>
-    <t>TATA 3</t>
   </si>
 </sst>
 </file>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C34"/>
+    <sheetView tabSelected="1" topLeftCell="F732" workbookViewId="0">
+      <selection activeCell="L743" sqref="L743:M770"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -749,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -793,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
@@ -835,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
@@ -877,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -919,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
@@ -961,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1003,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
@@ -1045,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -1087,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -1129,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -1171,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1213,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
@@ -1255,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
@@ -1297,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -1339,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -1381,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -1423,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -1465,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1507,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
@@ -1549,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -1591,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1633,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1675,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1717,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1759,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1801,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1843,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1885,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
@@ -1927,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -1969,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -2011,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -2053,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -2095,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>17</v>
@@ -20245,9 +20242,7 @@
       <c r="K471" s="1">
         <v>9750</v>
       </c>
-      <c r="L471" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L471" s="1"/>
       <c r="M471" s="1"/>
       <c r="N471" s="1"/>
       <c r="O471" s="1">
@@ -20289,9 +20284,7 @@
       <c r="K472" s="1">
         <v>1225</v>
       </c>
-      <c r="L472" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L472" s="1"/>
       <c r="M472" s="1"/>
       <c r="N472" s="1"/>
       <c r="O472" s="1">
@@ -20333,9 +20326,7 @@
       <c r="K473" s="1">
         <v>6000</v>
       </c>
-      <c r="L473" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L473" s="1"/>
       <c r="M473" s="1"/>
       <c r="N473" s="1"/>
       <c r="O473" s="1">
@@ -20377,9 +20368,7 @@
       <c r="K474" s="1">
         <v>1300</v>
       </c>
-      <c r="L474" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L474" s="1"/>
       <c r="M474" s="1"/>
       <c r="N474" s="1"/>
       <c r="O474" s="1">
@@ -20421,9 +20410,7 @@
       <c r="K475" s="1">
         <v>1225</v>
       </c>
-      <c r="L475" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L475" s="1"/>
       <c r="M475" s="1"/>
       <c r="N475" s="1"/>
       <c r="O475" s="1">
@@ -20465,9 +20452,7 @@
       <c r="K476" s="1">
         <v>6000</v>
       </c>
-      <c r="L476" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L476" s="1"/>
       <c r="M476" s="1"/>
       <c r="N476" s="1"/>
       <c r="O476" s="1">
@@ -20509,9 +20494,7 @@
       <c r="K477" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L477" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L477" s="1"/>
       <c r="M477" s="1"/>
       <c r="N477" s="1"/>
       <c r="O477" s="1">
@@ -20553,9 +20536,7 @@
       <c r="K478" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L478" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L478" s="1"/>
       <c r="M478" s="1"/>
       <c r="N478" s="1"/>
       <c r="O478" s="1">
@@ -20597,9 +20578,7 @@
       <c r="K479" s="1">
         <v>10250</v>
       </c>
-      <c r="L479" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L479" s="1"/>
       <c r="M479" s="1"/>
       <c r="N479" s="1"/>
       <c r="O479" s="1">
@@ -20641,9 +20620,7 @@
       <c r="K480" s="1">
         <v>39000</v>
       </c>
-      <c r="L480" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L480" s="1"/>
       <c r="M480" s="1"/>
       <c r="N480" s="1"/>
       <c r="O480" s="1">
@@ -20685,9 +20662,7 @@
       <c r="K481" s="1">
         <v>1225</v>
       </c>
-      <c r="L481" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L481" s="1"/>
       <c r="M481" s="1"/>
       <c r="N481" s="1"/>
       <c r="O481" s="1">
@@ -20729,9 +20704,7 @@
       <c r="K482" s="1">
         <v>20150</v>
       </c>
-      <c r="L482" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L482" s="1"/>
       <c r="M482" s="1"/>
       <c r="N482" s="1"/>
       <c r="O482" s="1">
@@ -20773,9 +20746,7 @@
       <c r="K483" s="1">
         <v>14375</v>
       </c>
-      <c r="L483" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L483" s="1"/>
       <c r="M483" s="1"/>
       <c r="N483" s="1"/>
       <c r="O483" s="1">
@@ -20817,9 +20788,7 @@
       <c r="K484" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L484" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L484" s="1"/>
       <c r="M484" s="1"/>
       <c r="N484" s="1"/>
       <c r="O484" s="1">
@@ -20861,9 +20830,7 @@
       <c r="K485" s="1">
         <v>10250</v>
       </c>
-      <c r="L485" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L485" s="1"/>
       <c r="M485" s="1"/>
       <c r="N485" s="1"/>
       <c r="O485" s="1">
@@ -20905,9 +20872,7 @@
       <c r="K486" s="1">
         <v>2450</v>
       </c>
-      <c r="L486" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L486" s="1"/>
       <c r="M486" s="1"/>
       <c r="N486" s="1"/>
       <c r="O486" s="1">
@@ -20949,9 +20914,7 @@
       <c r="K487" s="1">
         <v>1000</v>
       </c>
-      <c r="L487" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L487" s="1"/>
       <c r="M487" s="1"/>
       <c r="N487" s="1"/>
       <c r="O487" s="1">
@@ -20993,9 +20956,7 @@
       <c r="K488" s="1">
         <v>7800</v>
       </c>
-      <c r="L488" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L488" s="1"/>
       <c r="M488" s="1"/>
       <c r="N488" s="1"/>
       <c r="O488" s="1">
@@ -21037,9 +20998,7 @@
       <c r="K489" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L489" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L489" s="1"/>
       <c r="M489" s="1"/>
       <c r="N489" s="1"/>
       <c r="O489" s="1">
@@ -21081,9 +21040,7 @@
       <c r="K490" s="1">
         <v>10250</v>
       </c>
-      <c r="L490" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L490" s="1"/>
       <c r="M490" s="1"/>
       <c r="N490" s="1"/>
       <c r="O490" s="1">
@@ -21125,9 +21082,7 @@
       <c r="K491" s="1">
         <v>2450</v>
       </c>
-      <c r="L491" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L491" s="1"/>
       <c r="M491" s="1"/>
       <c r="N491" s="1"/>
       <c r="O491" s="1">
@@ -21169,9 +21124,7 @@
       <c r="K492" s="1">
         <v>2000</v>
       </c>
-      <c r="L492" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L492" s="1"/>
       <c r="M492" s="1"/>
       <c r="N492" s="1"/>
       <c r="O492" s="1">
@@ -21213,9 +21166,7 @@
       <c r="K493" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L493" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L493" s="1"/>
       <c r="M493" s="1"/>
       <c r="N493" s="1"/>
       <c r="O493" s="1">
@@ -21257,9 +21208,7 @@
       <c r="K494" s="1">
         <v>5125</v>
       </c>
-      <c r="L494" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L494" s="1"/>
       <c r="M494" s="1"/>
       <c r="N494" s="1"/>
       <c r="O494" s="1">
@@ -21301,9 +21250,7 @@
       <c r="K495" s="1">
         <v>2450</v>
       </c>
-      <c r="L495" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L495" s="1"/>
       <c r="M495" s="1"/>
       <c r="N495" s="1"/>
       <c r="O495" s="1">
@@ -21345,9 +21292,7 @@
       <c r="K496" s="1">
         <v>6000</v>
       </c>
-      <c r="L496" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L496" s="1"/>
       <c r="M496" s="1"/>
       <c r="N496" s="1"/>
       <c r="O496" s="1">
@@ -21389,9 +21334,7 @@
       <c r="K497" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L497" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L497" s="1"/>
       <c r="M497" s="1"/>
       <c r="N497" s="1"/>
       <c r="O497" s="1">
@@ -21433,9 +21376,7 @@
       <c r="K498" s="1">
         <v>19500</v>
       </c>
-      <c r="L498" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L498" s="1"/>
       <c r="M498" s="1"/>
       <c r="N498" s="1"/>
       <c r="O498" s="1">
@@ -21477,9 +21418,7 @@
       <c r="K499" s="1">
         <v>2000</v>
       </c>
-      <c r="L499" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L499" s="1"/>
       <c r="M499" s="1"/>
       <c r="N499" s="1"/>
       <c r="O499" s="1">
@@ -21521,9 +21460,7 @@
       <c r="K500" s="1">
         <v>33500</v>
       </c>
-      <c r="L500" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L500" s="1"/>
       <c r="M500" s="1"/>
       <c r="N500" s="1"/>
       <c r="O500" s="1">
@@ -21565,9 +21502,7 @@
       <c r="K501" s="1">
         <v>9750</v>
       </c>
-      <c r="L501" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L501" s="1"/>
       <c r="M501" s="1"/>
       <c r="N501" s="1"/>
       <c r="O501" s="1">
@@ -21609,9 +21544,7 @@
       <c r="K502" s="1">
         <v>5000</v>
       </c>
-      <c r="L502" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L502" s="1"/>
       <c r="M502" s="1"/>
       <c r="N502" s="1"/>
       <c r="O502" s="1">
@@ -21653,9 +21586,7 @@
       <c r="K503" s="1">
         <v>50250</v>
       </c>
-      <c r="L503" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L503" s="1"/>
       <c r="M503" s="1"/>
       <c r="N503" s="1"/>
       <c r="O503" s="1">
@@ -21697,9 +21628,7 @@
       <c r="K504" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L504" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L504" s="1"/>
       <c r="M504" s="1"/>
       <c r="N504" s="1"/>
       <c r="O504" s="1">
@@ -21741,9 +21670,7 @@
       <c r="K505" s="1">
         <v>20500</v>
       </c>
-      <c r="L505" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L505" s="1"/>
       <c r="M505" s="1"/>
       <c r="N505" s="1"/>
       <c r="O505" s="1">
@@ -21829,9 +21756,7 @@
       <c r="K507" s="1">
         <v>5125</v>
       </c>
-      <c r="L507" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L507" s="1"/>
       <c r="M507" s="1"/>
       <c r="N507" s="1"/>
       <c r="O507" s="1">
@@ -21873,9 +21798,7 @@
       <c r="K508" s="1">
         <v>6000</v>
       </c>
-      <c r="L508" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L508" s="1"/>
       <c r="M508" s="1"/>
       <c r="N508" s="1"/>
       <c r="O508" s="1">
@@ -21917,9 +21840,7 @@
       <c r="K509" s="1">
         <v>1225</v>
       </c>
-      <c r="L509" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L509" s="1"/>
       <c r="M509" s="1"/>
       <c r="N509" s="1"/>
       <c r="O509" s="1">
@@ -21961,9 +21882,7 @@
       <c r="K510" s="1">
         <v>650</v>
       </c>
-      <c r="L510" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L510" s="1"/>
       <c r="M510" s="1"/>
       <c r="N510" s="1"/>
       <c r="O510" s="1">
@@ -22005,9 +21924,7 @@
       <c r="K511" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L511" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L511" s="1"/>
       <c r="M511" s="1"/>
       <c r="N511" s="1"/>
       <c r="O511" s="1">
@@ -22049,9 +21966,7 @@
       <c r="K512" s="1">
         <v>2875</v>
       </c>
-      <c r="L512" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L512" s="1"/>
       <c r="M512" s="1"/>
       <c r="N512" s="1"/>
       <c r="O512" s="1">
@@ -22093,9 +22008,7 @@
       <c r="K513" s="1">
         <v>9750</v>
       </c>
-      <c r="L513" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L513" s="1"/>
       <c r="M513" s="1"/>
       <c r="N513" s="1"/>
       <c r="O513" s="1">
@@ -22137,9 +22050,7 @@
       <c r="K514" s="1">
         <v>6000</v>
       </c>
-      <c r="L514" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L514" s="1"/>
       <c r="M514" s="1"/>
       <c r="N514" s="1"/>
       <c r="O514" s="1">
@@ -22181,9 +22092,7 @@
       <c r="K515" s="1">
         <v>1225</v>
       </c>
-      <c r="L515" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L515" s="1"/>
       <c r="M515" s="1"/>
       <c r="N515" s="1"/>
       <c r="O515" s="1">
@@ -22225,9 +22134,7 @@
       <c r="K516" s="1">
         <v>650</v>
       </c>
-      <c r="L516" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L516" s="1"/>
       <c r="M516" s="1"/>
       <c r="N516" s="1"/>
       <c r="O516" s="1">
@@ -22269,9 +22176,7 @@
       <c r="K517" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L517" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L517" s="1"/>
       <c r="M517" s="1"/>
       <c r="N517" s="1"/>
       <c r="O517" s="1">
@@ -22313,9 +22218,7 @@
       <c r="K518" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L518" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L518" s="1"/>
       <c r="M518" s="1"/>
       <c r="N518" s="1"/>
       <c r="O518" s="1">
@@ -22357,9 +22260,7 @@
       <c r="K519" s="1">
         <v>6125</v>
       </c>
-      <c r="L519" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L519" s="1"/>
       <c r="M519" s="1"/>
       <c r="N519" s="1"/>
       <c r="O519" s="1">
@@ -22401,9 +22302,7 @@
       <c r="K520" s="1">
         <v>7000</v>
       </c>
-      <c r="L520" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L520" s="1"/>
       <c r="M520" s="1"/>
       <c r="N520" s="1"/>
       <c r="O520" s="1">
@@ -22445,9 +22344,7 @@
       <c r="K521" s="1">
         <v>650</v>
       </c>
-      <c r="L521" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L521" s="1"/>
       <c r="M521" s="1"/>
       <c r="N521" s="1"/>
       <c r="O521" s="1">
@@ -22489,9 +22386,7 @@
       <c r="K522" s="1">
         <v>1458.3334</v>
       </c>
-      <c r="L522" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L522" s="1"/>
       <c r="M522" s="1"/>
       <c r="N522" s="1"/>
       <c r="O522" s="1">
@@ -22533,9 +22428,7 @@
       <c r="K523" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L523" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L523" s="1"/>
       <c r="M523" s="1"/>
       <c r="N523" s="1"/>
       <c r="O523" s="1">
@@ -22577,9 +22470,7 @@
       <c r="K524" s="1">
         <v>19500</v>
       </c>
-      <c r="L524" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L524" s="1"/>
       <c r="M524" s="1"/>
       <c r="N524" s="1"/>
       <c r="O524" s="1">
@@ -22621,9 +22512,7 @@
       <c r="K525" s="1">
         <v>18000</v>
       </c>
-      <c r="L525" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L525" s="1"/>
       <c r="M525" s="1"/>
       <c r="N525" s="1"/>
       <c r="O525" s="1">
@@ -22665,9 +22554,7 @@
       <c r="K526" s="1">
         <v>2450</v>
       </c>
-      <c r="L526" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L526" s="1"/>
       <c r="M526" s="1"/>
       <c r="N526" s="1"/>
       <c r="O526" s="1">
@@ -22709,9 +22596,7 @@
       <c r="K527" s="1">
         <v>1300</v>
       </c>
-      <c r="L527" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L527" s="1"/>
       <c r="M527" s="1"/>
       <c r="N527" s="1"/>
       <c r="O527" s="1">
@@ -22753,9 +22638,7 @@
       <c r="K528" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L528" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L528" s="1"/>
       <c r="M528" s="1"/>
       <c r="N528" s="1"/>
       <c r="O528" s="1">
@@ -22797,9 +22680,7 @@
       <c r="K529" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L529" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L529" s="1"/>
       <c r="M529" s="1"/>
       <c r="N529" s="1"/>
       <c r="O529" s="1">
@@ -22841,9 +22722,7 @@
       <c r="K530" s="1">
         <v>6000</v>
       </c>
-      <c r="L530" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L530" s="1"/>
       <c r="M530" s="1"/>
       <c r="N530" s="1"/>
       <c r="O530" s="1">
@@ -22885,9 +22764,7 @@
       <c r="K531" s="1">
         <v>2450</v>
       </c>
-      <c r="L531" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L531" s="1"/>
       <c r="M531" s="1"/>
       <c r="N531" s="1"/>
       <c r="O531" s="1">
@@ -22929,9 +22806,7 @@
       <c r="K532" s="1">
         <v>1300</v>
       </c>
-      <c r="L532" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L532" s="1"/>
       <c r="M532" s="1"/>
       <c r="N532" s="1"/>
       <c r="O532" s="1">
@@ -22973,9 +22848,7 @@
       <c r="K533" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L533" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L533" s="1"/>
       <c r="M533" s="1"/>
       <c r="N533" s="1"/>
       <c r="O533" s="1">
@@ -23017,9 +22890,7 @@
       <c r="K534" s="1">
         <v>19500</v>
       </c>
-      <c r="L534" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L534" s="1"/>
       <c r="M534" s="1"/>
       <c r="N534" s="1"/>
       <c r="O534" s="1">
@@ -23061,9 +22932,7 @@
       <c r="K535" s="1">
         <v>3000</v>
       </c>
-      <c r="L535" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L535" s="1"/>
       <c r="M535" s="1"/>
       <c r="N535" s="1"/>
       <c r="O535" s="1">
@@ -23105,9 +22974,7 @@
       <c r="K536" s="1">
         <v>1225</v>
       </c>
-      <c r="L536" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L536" s="1"/>
       <c r="M536" s="1"/>
       <c r="N536" s="1"/>
       <c r="O536" s="1">
@@ -23149,9 +23016,7 @@
       <c r="K537" s="1">
         <v>1300</v>
       </c>
-      <c r="L537" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L537" s="1"/>
       <c r="M537" s="1"/>
       <c r="N537" s="1"/>
       <c r="O537" s="1">
@@ -23193,9 +23058,7 @@
       <c r="K538" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L538" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L538" s="1"/>
       <c r="M538" s="1"/>
       <c r="N538" s="1"/>
       <c r="O538" s="1">
@@ -23237,9 +23100,7 @@
       <c r="K539" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L539" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L539" s="1"/>
       <c r="M539" s="1"/>
       <c r="N539" s="1"/>
       <c r="O539" s="1">
@@ -23281,9 +23142,7 @@
       <c r="K540" s="1">
         <v>52000</v>
       </c>
-      <c r="L540" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L540" s="1"/>
       <c r="M540" s="1"/>
       <c r="N540" s="1"/>
       <c r="O540" s="1">
@@ -23325,9 +23184,7 @@
       <c r="K541" s="1">
         <v>2450</v>
       </c>
-      <c r="L541" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L541" s="1"/>
       <c r="M541" s="1"/>
       <c r="N541" s="1"/>
       <c r="O541" s="1">
@@ -23369,9 +23226,7 @@
       <c r="K542" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L542" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L542" s="1"/>
       <c r="M542" s="1"/>
       <c r="N542" s="1"/>
       <c r="O542" s="1">
@@ -23413,9 +23268,7 @@
       <c r="K543" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L543" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L543" s="1"/>
       <c r="M543" s="1"/>
       <c r="N543" s="1"/>
       <c r="O543" s="1">
@@ -23457,9 +23310,7 @@
       <c r="K544" s="1">
         <v>9750</v>
       </c>
-      <c r="L544" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L544" s="1"/>
       <c r="M544" s="1"/>
       <c r="N544" s="1"/>
       <c r="O544" s="1">
@@ -23501,9 +23352,7 @@
       <c r="K545" s="1">
         <v>6000</v>
       </c>
-      <c r="L545" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L545" s="1"/>
       <c r="M545" s="1"/>
       <c r="N545" s="1"/>
       <c r="O545" s="1">
@@ -23545,9 +23394,7 @@
       <c r="K546" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L546" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L546" s="1"/>
       <c r="M546" s="1"/>
       <c r="N546" s="1"/>
       <c r="O546" s="1">
@@ -23589,9 +23436,7 @@
       <c r="K547" s="1">
         <v>5125</v>
       </c>
-      <c r="L547" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L547" s="1"/>
       <c r="M547" s="1"/>
       <c r="N547" s="1"/>
       <c r="O547" s="1">
@@ -23633,9 +23478,7 @@
       <c r="K548" s="1">
         <v>11000</v>
       </c>
-      <c r="L548" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L548" s="1"/>
       <c r="M548" s="1"/>
       <c r="N548" s="1"/>
       <c r="O548" s="1">
@@ -24147,15 +23990,9 @@
       <c r="K561" s="1">
         <v>6000</v>
       </c>
-      <c r="L561" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M561" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N561" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L561" s="1"/>
+      <c r="M561" s="1"/>
+      <c r="N561" s="1"/>
       <c r="O561" s="1">
         <v>217</v>
       </c>
@@ -24197,15 +24034,9 @@
       <c r="K562" s="1">
         <v>4900</v>
       </c>
-      <c r="L562" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M562" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N562" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L562" s="1"/>
+      <c r="M562" s="1"/>
+      <c r="N562" s="1"/>
       <c r="O562" s="1">
         <v>218</v>
       </c>
@@ -24247,15 +24078,9 @@
       <c r="K563" s="1">
         <v>1300</v>
       </c>
-      <c r="L563" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M563" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N563" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L563" s="1"/>
+      <c r="M563" s="1"/>
+      <c r="N563" s="1"/>
       <c r="O563" s="1">
         <v>219</v>
       </c>
@@ -24297,15 +24122,9 @@
       <c r="K564" s="1">
         <v>750</v>
       </c>
-      <c r="L564" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M564" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N564" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L564" s="1"/>
+      <c r="M564" s="1"/>
+      <c r="N564" s="1"/>
       <c r="O564" s="1">
         <v>220</v>
       </c>
@@ -24347,15 +24166,9 @@
       <c r="K565" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L565" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M565" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N565" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L565" s="1"/>
+      <c r="M565" s="1"/>
+      <c r="N565" s="1"/>
       <c r="O565" s="1">
         <v>221</v>
       </c>
@@ -24397,15 +24210,9 @@
       <c r="K566" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L566" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M566" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N566" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L566" s="1"/>
+      <c r="M566" s="1"/>
+      <c r="N566" s="1"/>
       <c r="O566" s="1">
         <v>222</v>
       </c>
@@ -24447,15 +24254,9 @@
       <c r="K567" s="1">
         <v>6000</v>
       </c>
-      <c r="L567" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M567" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N567" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L567" s="1"/>
+      <c r="M567" s="1"/>
+      <c r="N567" s="1"/>
       <c r="O567" s="1">
         <v>209</v>
       </c>
@@ -24497,15 +24298,9 @@
       <c r="K568" s="1">
         <v>2450</v>
       </c>
-      <c r="L568" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M568" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N568" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L568" s="1"/>
+      <c r="M568" s="1"/>
+      <c r="N568" s="1"/>
       <c r="O568" s="1">
         <v>210</v>
       </c>
@@ -24547,15 +24342,9 @@
       <c r="K569" s="1">
         <v>1300</v>
       </c>
-      <c r="L569" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M569" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N569" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L569" s="1"/>
+      <c r="M569" s="1"/>
+      <c r="N569" s="1"/>
       <c r="O569" s="1">
         <v>211</v>
       </c>
@@ -24597,15 +24386,9 @@
       <c r="K570" s="1">
         <v>750</v>
       </c>
-      <c r="L570" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M570" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N570" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L570" s="1"/>
+      <c r="M570" s="1"/>
+      <c r="N570" s="1"/>
       <c r="O570" s="1">
         <v>212</v>
       </c>
@@ -24647,15 +24430,9 @@
       <c r="K571" s="1">
         <v>2875</v>
       </c>
-      <c r="L571" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M571" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N571" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L571" s="1"/>
+      <c r="M571" s="1"/>
+      <c r="N571" s="1"/>
       <c r="O571" s="1">
         <v>213</v>
       </c>
@@ -24697,15 +24474,9 @@
       <c r="K572" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L572" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M572" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N572" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L572" s="1"/>
+      <c r="M572" s="1"/>
+      <c r="N572" s="1"/>
       <c r="O572" s="1">
         <v>214</v>
       </c>
@@ -24747,15 +24518,9 @@
       <c r="K573" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L573" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M573" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N573" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L573" s="1"/>
+      <c r="M573" s="1"/>
+      <c r="N573" s="1"/>
       <c r="O573" s="1">
         <v>215</v>
       </c>
@@ -24795,15 +24560,9 @@
       <c r="K574" s="1">
         <v>14700</v>
       </c>
-      <c r="L574" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M574" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N574" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L574" s="1"/>
+      <c r="M574" s="1"/>
+      <c r="N574" s="1"/>
       <c r="O574" s="1">
         <v>205</v>
       </c>
@@ -24843,15 +24602,9 @@
       <c r="K575" s="1">
         <v>9000</v>
       </c>
-      <c r="L575" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M575" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N575" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L575" s="1"/>
+      <c r="M575" s="1"/>
+      <c r="N575" s="1"/>
       <c r="O575" s="1">
         <v>206</v>
       </c>
@@ -24891,15 +24644,9 @@
       <c r="K576" s="1">
         <v>750</v>
       </c>
-      <c r="L576" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M576" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N576" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L576" s="1"/>
+      <c r="M576" s="1"/>
+      <c r="N576" s="1"/>
       <c r="O576" s="1">
         <v>207</v>
       </c>
@@ -24939,15 +24686,9 @@
       <c r="K577" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L577" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M577" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N577" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L577" s="1"/>
+      <c r="M577" s="1"/>
+      <c r="N577" s="1"/>
       <c r="O577" s="1">
         <v>208</v>
       </c>
@@ -24987,15 +24728,9 @@
       <c r="K578" s="1">
         <v>51250</v>
       </c>
-      <c r="L578" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M578" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N578" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L578" s="1"/>
+      <c r="M578" s="1"/>
+      <c r="N578" s="1"/>
       <c r="O578" s="1">
         <v>204</v>
       </c>
@@ -25035,15 +24770,9 @@
       <c r="K579" s="1">
         <v>5125</v>
       </c>
-      <c r="L579" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M579" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N579" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L579" s="1"/>
+      <c r="M579" s="1"/>
+      <c r="N579" s="1"/>
       <c r="O579" s="1">
         <v>197</v>
       </c>
@@ -25083,15 +24812,9 @@
       <c r="K580" s="1">
         <v>6000</v>
       </c>
-      <c r="L580" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M580" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N580" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L580" s="1"/>
+      <c r="M580" s="1"/>
+      <c r="N580" s="1"/>
       <c r="O580" s="1">
         <v>198</v>
       </c>
@@ -25131,15 +24854,9 @@
       <c r="K581" s="1">
         <v>2450</v>
       </c>
-      <c r="L581" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M581" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N581" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L581" s="1"/>
+      <c r="M581" s="1"/>
+      <c r="N581" s="1"/>
       <c r="O581" s="1">
         <v>199</v>
       </c>
@@ -25179,15 +24896,9 @@
       <c r="K582" s="1">
         <v>1300</v>
       </c>
-      <c r="L582" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M582" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N582" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L582" s="1"/>
+      <c r="M582" s="1"/>
+      <c r="N582" s="1"/>
       <c r="O582" s="1">
         <v>200</v>
       </c>
@@ -25227,15 +24938,9 @@
       <c r="K583" s="1">
         <v>750</v>
       </c>
-      <c r="L583" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M583" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N583" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L583" s="1"/>
+      <c r="M583" s="1"/>
+      <c r="N583" s="1"/>
       <c r="O583" s="1">
         <v>201</v>
       </c>
@@ -25275,15 +24980,9 @@
       <c r="K584" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L584" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M584" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N584" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L584" s="1"/>
+      <c r="M584" s="1"/>
+      <c r="N584" s="1"/>
       <c r="O584" s="1">
         <v>202</v>
       </c>
@@ -25323,15 +25022,9 @@
       <c r="K585" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L585" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M585" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N585" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L585" s="1"/>
+      <c r="M585" s="1"/>
+      <c r="N585" s="1"/>
       <c r="O585" s="1">
         <v>203</v>
       </c>
@@ -25371,15 +25064,9 @@
       <c r="K586" s="1">
         <v>5125</v>
       </c>
-      <c r="L586" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M586" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N586" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L586" s="1"/>
+      <c r="M586" s="1"/>
+      <c r="N586" s="1"/>
       <c r="O586" s="1">
         <v>193</v>
       </c>
@@ -25419,15 +25106,9 @@
       <c r="K587" s="1">
         <v>1000</v>
       </c>
-      <c r="L587" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M587" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N587" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L587" s="1"/>
+      <c r="M587" s="1"/>
+      <c r="N587" s="1"/>
       <c r="O587" s="1">
         <v>194</v>
       </c>
@@ -25467,15 +25148,9 @@
       <c r="K588" s="1">
         <v>650</v>
       </c>
-      <c r="L588" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M588" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N588" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L588" s="1"/>
+      <c r="M588" s="1"/>
+      <c r="N588" s="1"/>
       <c r="O588" s="1">
         <v>195</v>
       </c>
@@ -25515,15 +25190,9 @@
       <c r="K589" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L589" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M589" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N589" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L589" s="1"/>
+      <c r="M589" s="1"/>
+      <c r="N589" s="1"/>
       <c r="O589" s="1">
         <v>196</v>
       </c>
@@ -25563,15 +25232,9 @@
       <c r="K590" s="1">
         <v>195000</v>
       </c>
-      <c r="L590" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M590" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N590" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L590" s="1"/>
+      <c r="M590" s="1"/>
+      <c r="N590" s="1"/>
       <c r="O590" s="1">
         <v>192</v>
       </c>
@@ -25611,15 +25274,9 @@
       <c r="K591" s="1">
         <v>50000</v>
       </c>
-      <c r="L591" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M591" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N591" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L591" s="1"/>
+      <c r="M591" s="1"/>
+      <c r="N591" s="1"/>
       <c r="O591" s="1">
         <v>190</v>
       </c>
@@ -25659,15 +25316,9 @@
       <c r="K592" s="1">
         <v>10250</v>
       </c>
-      <c r="L592" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M592" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N592" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L592" s="1"/>
+      <c r="M592" s="1"/>
+      <c r="N592" s="1"/>
       <c r="O592" s="1">
         <v>191</v>
       </c>
@@ -25707,15 +25358,9 @@
       <c r="K593" s="1">
         <v>6000</v>
       </c>
-      <c r="L593" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M593" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N593" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L593" s="1"/>
+      <c r="M593" s="1"/>
+      <c r="N593" s="1"/>
       <c r="O593" s="1">
         <v>183</v>
       </c>
@@ -25755,15 +25400,9 @@
       <c r="K594" s="1">
         <v>2450</v>
       </c>
-      <c r="L594" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M594" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N594" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L594" s="1"/>
+      <c r="M594" s="1"/>
+      <c r="N594" s="1"/>
       <c r="O594" s="1">
         <v>184</v>
       </c>
@@ -25803,15 +25442,9 @@
       <c r="K595" s="1">
         <v>650</v>
       </c>
-      <c r="L595" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M595" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N595" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L595" s="1"/>
+      <c r="M595" s="1"/>
+      <c r="N595" s="1"/>
       <c r="O595" s="1">
         <v>185</v>
       </c>
@@ -25851,15 +25484,9 @@
       <c r="K596" s="1">
         <v>750</v>
       </c>
-      <c r="L596" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M596" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N596" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L596" s="1"/>
+      <c r="M596" s="1"/>
+      <c r="N596" s="1"/>
       <c r="O596" s="1">
         <v>186</v>
       </c>
@@ -25899,15 +25526,9 @@
       <c r="K597" s="1">
         <v>2875</v>
       </c>
-      <c r="L597" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M597" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N597" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L597" s="1"/>
+      <c r="M597" s="1"/>
+      <c r="N597" s="1"/>
       <c r="O597" s="1">
         <v>187</v>
       </c>
@@ -25947,15 +25568,9 @@
       <c r="K598" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L598" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M598" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N598" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L598" s="1"/>
+      <c r="M598" s="1"/>
+      <c r="N598" s="1"/>
       <c r="O598" s="1">
         <v>188</v>
       </c>
@@ -25995,15 +25610,9 @@
       <c r="K599" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L599" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M599" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N599" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L599" s="1"/>
+      <c r="M599" s="1"/>
+      <c r="N599" s="1"/>
       <c r="O599" s="1">
         <v>189</v>
       </c>
@@ -26043,15 +25652,9 @@
       <c r="K600" s="1">
         <v>14700</v>
       </c>
-      <c r="L600" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M600" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N600" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L600" s="1"/>
+      <c r="M600" s="1"/>
+      <c r="N600" s="1"/>
       <c r="O600" s="1">
         <v>178</v>
       </c>
@@ -26091,15 +25694,9 @@
       <c r="K601" s="1">
         <v>10250</v>
       </c>
-      <c r="L601" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M601" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N601" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L601" s="1"/>
+      <c r="M601" s="1"/>
+      <c r="N601" s="1"/>
       <c r="O601" s="1">
         <v>179</v>
       </c>
@@ -26139,15 +25736,9 @@
       <c r="K602" s="1">
         <v>10000</v>
       </c>
-      <c r="L602" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M602" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N602" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L602" s="1"/>
+      <c r="M602" s="1"/>
+      <c r="N602" s="1"/>
       <c r="O602" s="1">
         <v>180</v>
       </c>
@@ -26187,15 +25778,9 @@
       <c r="K603" s="1">
         <v>1950</v>
       </c>
-      <c r="L603" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M603" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N603" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L603" s="1"/>
+      <c r="M603" s="1"/>
+      <c r="N603" s="1"/>
       <c r="O603" s="1">
         <v>181</v>
       </c>
@@ -26235,15 +25820,9 @@
       <c r="K604" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L604" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M604" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N604" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L604" s="1"/>
+      <c r="M604" s="1"/>
+      <c r="N604" s="1"/>
       <c r="O604" s="1">
         <v>182</v>
       </c>
@@ -26283,15 +25862,9 @@
       <c r="K605" s="1">
         <v>14000</v>
       </c>
-      <c r="L605" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M605" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N605" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L605" s="1"/>
+      <c r="M605" s="1"/>
+      <c r="N605" s="1"/>
       <c r="O605" s="1">
         <v>174</v>
       </c>
@@ -26331,15 +25904,9 @@
       <c r="K606" s="1">
         <v>19500</v>
       </c>
-      <c r="L606" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M606" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N606" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L606" s="1"/>
+      <c r="M606" s="1"/>
+      <c r="N606" s="1"/>
       <c r="O606" s="1">
         <v>175</v>
       </c>
@@ -26379,15 +25946,9 @@
       <c r="K607" s="1">
         <v>1225</v>
       </c>
-      <c r="L607" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M607" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N607" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L607" s="1"/>
+      <c r="M607" s="1"/>
+      <c r="N607" s="1"/>
       <c r="O607" s="1">
         <v>176</v>
       </c>
@@ -26427,15 +25988,9 @@
       <c r="K608" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L608" s="1">
-        <v>3000</v>
-      </c>
-      <c r="M608" s="1">
-        <v>5000</v>
-      </c>
-      <c r="N608" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="L608" s="1"/>
+      <c r="M608" s="1"/>
+      <c r="N608" s="1"/>
       <c r="O608" s="1">
         <v>177</v>
       </c>
@@ -26937,9 +26492,7 @@
       <c r="K621" s="1">
         <v>9750</v>
       </c>
-      <c r="L621" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L621" s="1"/>
       <c r="M621" s="1"/>
       <c r="N621" s="1"/>
       <c r="O621" s="1">
@@ -26981,9 +26534,7 @@
       <c r="K622" s="1">
         <v>4550</v>
       </c>
-      <c r="L622" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L622" s="1"/>
       <c r="M622" s="1"/>
       <c r="N622" s="1"/>
       <c r="O622" s="1">
@@ -27025,9 +26576,7 @@
       <c r="K623" s="1">
         <v>2450</v>
       </c>
-      <c r="L623" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L623" s="1"/>
       <c r="M623" s="1"/>
       <c r="N623" s="1"/>
       <c r="O623" s="1">
@@ -27069,9 +26618,7 @@
       <c r="K624" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L624" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L624" s="1"/>
       <c r="M624" s="1"/>
       <c r="N624" s="1"/>
       <c r="O624" s="1">
@@ -27113,9 +26660,7 @@
       <c r="K625" s="1">
         <v>27000</v>
       </c>
-      <c r="L625" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L625" s="1"/>
       <c r="M625" s="1"/>
       <c r="N625" s="1"/>
       <c r="O625" s="1">
@@ -27157,9 +26702,7 @@
       <c r="K626" s="1">
         <v>9750</v>
       </c>
-      <c r="L626" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L626" s="1"/>
       <c r="M626" s="1"/>
       <c r="N626" s="1"/>
       <c r="O626" s="1">
@@ -27201,9 +26744,7 @@
       <c r="K627" s="1">
         <v>2450</v>
       </c>
-      <c r="L627" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L627" s="1"/>
       <c r="M627" s="1"/>
       <c r="N627" s="1"/>
       <c r="O627" s="1">
@@ -27245,9 +26786,7 @@
       <c r="K628" s="1">
         <v>1300</v>
       </c>
-      <c r="L628" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L628" s="1"/>
       <c r="M628" s="1"/>
       <c r="N628" s="1"/>
       <c r="O628" s="1">
@@ -27289,9 +26828,7 @@
       <c r="K629" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L629" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L629" s="1"/>
       <c r="M629" s="1"/>
       <c r="N629" s="1"/>
       <c r="O629" s="1">
@@ -27333,9 +26870,7 @@
       <c r="K630" s="1">
         <v>10250</v>
       </c>
-      <c r="L630" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L630" s="1"/>
       <c r="M630" s="1"/>
       <c r="N630" s="1"/>
       <c r="O630" s="1">
@@ -27377,9 +26912,7 @@
       <c r="K631" s="1">
         <v>1000</v>
       </c>
-      <c r="L631" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L631" s="1"/>
       <c r="M631" s="1"/>
       <c r="N631" s="1"/>
       <c r="O631" s="1">
@@ -27421,9 +26954,7 @@
       <c r="K632" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L632" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L632" s="1"/>
       <c r="M632" s="1"/>
       <c r="N632" s="1"/>
       <c r="O632" s="1">
@@ -27465,9 +26996,7 @@
       <c r="K633" s="1">
         <v>650</v>
       </c>
-      <c r="L633" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L633" s="1"/>
       <c r="M633" s="1"/>
       <c r="N633" s="1"/>
       <c r="O633" s="1">
@@ -27509,9 +27038,7 @@
       <c r="K634" s="1">
         <v>19500</v>
       </c>
-      <c r="L634" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L634" s="1"/>
       <c r="M634" s="1"/>
       <c r="N634" s="1"/>
       <c r="O634" s="1">
@@ -27553,9 +27080,7 @@
       <c r="K635" s="1">
         <v>20500</v>
       </c>
-      <c r="L635" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L635" s="1"/>
       <c r="M635" s="1"/>
       <c r="N635" s="1"/>
       <c r="O635" s="1">
@@ -27597,9 +27122,7 @@
       <c r="K636" s="1">
         <v>5000</v>
       </c>
-      <c r="L636" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L636" s="1"/>
       <c r="M636" s="1"/>
       <c r="N636" s="1"/>
       <c r="O636" s="1">
@@ -27641,9 +27164,7 @@
       <c r="K637" s="1">
         <v>1225</v>
       </c>
-      <c r="L637" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L637" s="1"/>
       <c r="M637" s="1"/>
       <c r="N637" s="1"/>
       <c r="O637" s="1">
@@ -27685,9 +27206,7 @@
       <c r="K638" s="1">
         <v>1300</v>
       </c>
-      <c r="L638" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L638" s="1"/>
       <c r="M638" s="1"/>
       <c r="N638" s="1"/>
       <c r="O638" s="1">
@@ -27729,9 +27248,7 @@
       <c r="K639" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L639" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L639" s="1"/>
       <c r="M639" s="1"/>
       <c r="N639" s="1"/>
       <c r="O639" s="1">
@@ -27773,9 +27290,7 @@
       <c r="K640" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L640" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L640" s="1"/>
       <c r="M640" s="1"/>
       <c r="N640" s="1"/>
       <c r="O640" s="1">
@@ -27817,9 +27332,7 @@
       <c r="K641" s="1">
         <v>5125</v>
       </c>
-      <c r="L641" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L641" s="1"/>
       <c r="M641" s="1"/>
       <c r="N641" s="1"/>
       <c r="O641" s="1">
@@ -27861,9 +27374,7 @@
       <c r="K642" s="1">
         <v>12000</v>
       </c>
-      <c r="L642" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L642" s="1"/>
       <c r="M642" s="1"/>
       <c r="N642" s="1"/>
       <c r="O642" s="1">
@@ -27905,9 +27416,7 @@
       <c r="K643" s="1">
         <v>3675</v>
       </c>
-      <c r="L643" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L643" s="1"/>
       <c r="M643" s="1"/>
       <c r="N643" s="1"/>
       <c r="O643" s="1">
@@ -27949,9 +27458,7 @@
       <c r="K644" s="1">
         <v>1300</v>
       </c>
-      <c r="L644" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L644" s="1"/>
       <c r="M644" s="1"/>
       <c r="N644" s="1"/>
       <c r="O644" s="1">
@@ -27993,9 +27500,7 @@
       <c r="K645" s="1">
         <v>19500</v>
       </c>
-      <c r="L645" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L645" s="1"/>
       <c r="M645" s="1"/>
       <c r="N645" s="1"/>
       <c r="O645" s="1">
@@ -28037,9 +27542,7 @@
       <c r="K646" s="1">
         <v>19500</v>
       </c>
-      <c r="L646" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L646" s="1"/>
       <c r="M646" s="1"/>
       <c r="N646" s="1"/>
       <c r="O646" s="1">
@@ -28081,9 +27584,7 @@
       <c r="K647" s="1">
         <v>5125</v>
       </c>
-      <c r="L647" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L647" s="1"/>
       <c r="M647" s="1"/>
       <c r="N647" s="1"/>
       <c r="O647" s="1">
@@ -28125,9 +27626,7 @@
       <c r="K648" s="1">
         <v>12000</v>
       </c>
-      <c r="L648" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L648" s="1"/>
       <c r="M648" s="1"/>
       <c r="N648" s="1"/>
       <c r="O648" s="1">
@@ -28169,9 +27668,7 @@
       <c r="K649" s="1">
         <v>1300</v>
       </c>
-      <c r="L649" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L649" s="1"/>
       <c r="M649" s="1"/>
       <c r="N649" s="1"/>
       <c r="O649" s="1">
@@ -28213,9 +27710,7 @@
       <c r="K650" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L650" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L650" s="1"/>
       <c r="M650" s="1"/>
       <c r="N650" s="1"/>
       <c r="O650" s="1">
@@ -28257,9 +27752,7 @@
       <c r="K651" s="1">
         <v>29000</v>
       </c>
-      <c r="L651" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L651" s="1"/>
       <c r="M651" s="1"/>
       <c r="N651" s="1"/>
       <c r="O651" s="1">
@@ -28301,9 +27794,7 @@
       <c r="K652" s="1">
         <v>25625</v>
       </c>
-      <c r="L652" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L652" s="1"/>
       <c r="M652" s="1"/>
       <c r="N652" s="1"/>
       <c r="O652" s="1">
@@ -28345,9 +27836,7 @@
       <c r="K653" s="1">
         <v>68250</v>
       </c>
-      <c r="L653" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L653" s="1"/>
       <c r="M653" s="1"/>
       <c r="N653" s="1"/>
       <c r="O653" s="1">
@@ -28389,9 +27878,7 @@
       <c r="K654" s="1">
         <v>2450</v>
       </c>
-      <c r="L654" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L654" s="1"/>
       <c r="M654" s="1"/>
       <c r="N654" s="1"/>
       <c r="O654" s="1">
@@ -28433,9 +27920,7 @@
       <c r="K655" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L655" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L655" s="1"/>
       <c r="M655" s="1"/>
       <c r="N655" s="1"/>
       <c r="O655" s="1">
@@ -28477,9 +27962,7 @@
       <c r="K656" s="1">
         <v>2875</v>
       </c>
-      <c r="L656" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L656" s="1"/>
       <c r="M656" s="1"/>
       <c r="N656" s="1"/>
       <c r="O656" s="1">
@@ -28521,9 +28004,7 @@
       <c r="K657" s="1">
         <v>10250</v>
       </c>
-      <c r="L657" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L657" s="1"/>
       <c r="M657" s="1"/>
       <c r="N657" s="1"/>
       <c r="O657" s="1">
@@ -28565,9 +28046,7 @@
       <c r="K658" s="1">
         <v>19500</v>
       </c>
-      <c r="L658" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L658" s="1"/>
       <c r="M658" s="1"/>
       <c r="N658" s="1"/>
       <c r="O658" s="1">
@@ -28609,9 +28088,7 @@
       <c r="K659" s="1">
         <v>1000</v>
       </c>
-      <c r="L659" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L659" s="1"/>
       <c r="M659" s="1"/>
       <c r="N659" s="1"/>
       <c r="O659" s="1">
@@ -28653,9 +28130,7 @@
       <c r="K660" s="1">
         <v>2450</v>
       </c>
-      <c r="L660" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L660" s="1"/>
       <c r="M660" s="1"/>
       <c r="N660" s="1"/>
       <c r="O660" s="1">
@@ -28697,9 +28172,7 @@
       <c r="K661" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L661" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L661" s="1"/>
       <c r="M661" s="1"/>
       <c r="N661" s="1"/>
       <c r="O661" s="1">
@@ -28741,9 +28214,7 @@
       <c r="K662" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L662" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L662" s="1"/>
       <c r="M662" s="1"/>
       <c r="N662" s="1"/>
       <c r="O662" s="1">
@@ -28785,9 +28256,7 @@
       <c r="K663" s="1">
         <v>9750</v>
       </c>
-      <c r="L663" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L663" s="1"/>
       <c r="M663" s="1"/>
       <c r="N663" s="1"/>
       <c r="O663" s="1">
@@ -28829,9 +28298,7 @@
       <c r="K664" s="1">
         <v>9000</v>
       </c>
-      <c r="L664" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L664" s="1"/>
       <c r="M664" s="1"/>
       <c r="N664" s="1"/>
       <c r="O664" s="1">
@@ -28873,9 +28340,7 @@
       <c r="K665" s="1">
         <v>1225</v>
       </c>
-      <c r="L665" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L665" s="1"/>
       <c r="M665" s="1"/>
       <c r="N665" s="1"/>
       <c r="O665" s="1">
@@ -28961,9 +28426,7 @@
       <c r="K667" s="1">
         <v>39000</v>
       </c>
-      <c r="L667" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L667" s="1"/>
       <c r="M667" s="1"/>
       <c r="N667" s="1"/>
       <c r="O667" s="1">
@@ -29005,9 +28468,7 @@
       <c r="K668" s="1">
         <v>4900</v>
       </c>
-      <c r="L668" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L668" s="1"/>
       <c r="M668" s="1"/>
       <c r="N668" s="1"/>
       <c r="O668" s="1">
@@ -29049,9 +28510,7 @@
       <c r="K669" s="1">
         <v>6000</v>
       </c>
-      <c r="L669" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L669" s="1"/>
       <c r="M669" s="1"/>
       <c r="N669" s="1"/>
       <c r="O669" s="1">
@@ -29093,9 +28552,7 @@
       <c r="K670" s="1">
         <v>1300</v>
       </c>
-      <c r="L670" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L670" s="1"/>
       <c r="M670" s="1"/>
       <c r="N670" s="1"/>
       <c r="O670" s="1">
@@ -29137,9 +28594,7 @@
       <c r="K671" s="1">
         <v>1458.3334</v>
       </c>
-      <c r="L671" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L671" s="1"/>
       <c r="M671" s="1"/>
       <c r="N671" s="1"/>
       <c r="O671" s="1">
@@ -29181,9 +28636,7 @@
       <c r="K672" s="1">
         <v>2791.6667000000002</v>
       </c>
-      <c r="L672" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L672" s="1"/>
       <c r="M672" s="1"/>
       <c r="N672" s="1"/>
       <c r="O672" s="1">
@@ -29225,9 +28678,7 @@
       <c r="K673" s="1">
         <v>1225</v>
       </c>
-      <c r="L673" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L673" s="1"/>
       <c r="M673" s="1"/>
       <c r="N673" s="1"/>
       <c r="O673" s="1">
@@ -29269,9 +28720,7 @@
       <c r="K674" s="1">
         <v>11000</v>
       </c>
-      <c r="L674" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L674" s="1"/>
       <c r="M674" s="1"/>
       <c r="N674" s="1"/>
       <c r="O674" s="1">
@@ -29313,9 +28762,7 @@
       <c r="K675" s="1">
         <v>1300</v>
       </c>
-      <c r="L675" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L675" s="1"/>
       <c r="M675" s="1"/>
       <c r="N675" s="1"/>
       <c r="O675" s="1">
@@ -29357,9 +28804,7 @@
       <c r="K676" s="1">
         <v>2450</v>
       </c>
-      <c r="L676" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L676" s="1"/>
       <c r="M676" s="1"/>
       <c r="N676" s="1"/>
       <c r="O676" s="1">
@@ -29401,9 +28846,7 @@
       <c r="K677" s="1">
         <v>8000</v>
       </c>
-      <c r="L677" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L677" s="1"/>
       <c r="M677" s="1"/>
       <c r="N677" s="1"/>
       <c r="O677" s="1">
@@ -29445,9 +28888,7 @@
       <c r="K678" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L678" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L678" s="1"/>
       <c r="M678" s="1"/>
       <c r="N678" s="1"/>
       <c r="O678" s="1">
@@ -29489,9 +28930,7 @@
       <c r="K679" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L679" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L679" s="1"/>
       <c r="M679" s="1"/>
       <c r="N679" s="1"/>
       <c r="O679" s="1">
@@ -29533,9 +28972,7 @@
       <c r="K680" s="1">
         <v>5125</v>
       </c>
-      <c r="L680" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L680" s="1"/>
       <c r="M680" s="1"/>
       <c r="N680" s="1"/>
       <c r="O680" s="1">
@@ -29577,9 +29014,7 @@
       <c r="K681" s="1">
         <v>19500</v>
       </c>
-      <c r="L681" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L681" s="1"/>
       <c r="M681" s="1"/>
       <c r="N681" s="1"/>
       <c r="O681" s="1">
@@ -29621,9 +29056,7 @@
       <c r="K682" s="1">
         <v>1225</v>
       </c>
-      <c r="L682" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L682" s="1"/>
       <c r="M682" s="1"/>
       <c r="N682" s="1"/>
       <c r="O682" s="1">
@@ -29665,9 +29098,7 @@
       <c r="K683" s="1">
         <v>4000</v>
       </c>
-      <c r="L683" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L683" s="1"/>
       <c r="M683" s="1"/>
       <c r="N683" s="1"/>
       <c r="O683" s="1">
@@ -29709,9 +29140,7 @@
       <c r="K684" s="1">
         <v>18145.833999999999</v>
       </c>
-      <c r="L684" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L684" s="1"/>
       <c r="M684" s="1"/>
       <c r="N684" s="1"/>
       <c r="O684" s="1">
@@ -29753,9 +29182,7 @@
       <c r="K685" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L685" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L685" s="1"/>
       <c r="M685" s="1"/>
       <c r="N685" s="1"/>
       <c r="O685" s="1">
@@ -29797,9 +29224,7 @@
       <c r="K686" s="1">
         <v>5125</v>
       </c>
-      <c r="L686" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L686" s="1"/>
       <c r="M686" s="1"/>
       <c r="N686" s="1"/>
       <c r="O686" s="1">
@@ -29841,9 +29266,7 @@
       <c r="K687" s="1">
         <v>1225</v>
       </c>
-      <c r="L687" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L687" s="1"/>
       <c r="M687" s="1"/>
       <c r="N687" s="1"/>
       <c r="O687" s="1">
@@ -29885,9 +29308,7 @@
       <c r="K688" s="1">
         <v>4000</v>
       </c>
-      <c r="L688" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L688" s="1"/>
       <c r="M688" s="1"/>
       <c r="N688" s="1"/>
       <c r="O688" s="1">
@@ -29929,9 +29350,7 @@
       <c r="K689" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L689" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L689" s="1"/>
       <c r="M689" s="1"/>
       <c r="N689" s="1"/>
       <c r="O689" s="1">
@@ -29973,9 +29392,7 @@
       <c r="K690" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L690" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L690" s="1"/>
       <c r="M690" s="1"/>
       <c r="N690" s="1"/>
       <c r="O690" s="1">
@@ -30017,9 +29434,7 @@
       <c r="K691" s="1">
         <v>9750</v>
       </c>
-      <c r="L691" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L691" s="1"/>
       <c r="M691" s="1"/>
       <c r="N691" s="1"/>
       <c r="O691" s="1">
@@ -30061,9 +29476,7 @@
       <c r="K692" s="1">
         <v>1225</v>
       </c>
-      <c r="L692" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L692" s="1"/>
       <c r="M692" s="1"/>
       <c r="N692" s="1"/>
       <c r="O692" s="1">
@@ -30105,9 +29518,7 @@
       <c r="K693" s="1">
         <v>5000</v>
       </c>
-      <c r="L693" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L693" s="1"/>
       <c r="M693" s="1"/>
       <c r="N693" s="1"/>
       <c r="O693" s="1">
@@ -30149,9 +29560,7 @@
       <c r="K694" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L694" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L694" s="1"/>
       <c r="M694" s="1"/>
       <c r="N694" s="1"/>
       <c r="O694" s="1">
@@ -30193,9 +29602,7 @@
       <c r="K695" s="1">
         <v>5125</v>
       </c>
-      <c r="L695" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L695" s="1"/>
       <c r="M695" s="1"/>
       <c r="N695" s="1"/>
       <c r="O695" s="1">
@@ -30237,9 +29644,7 @@
       <c r="K696" s="1">
         <v>2450</v>
       </c>
-      <c r="L696" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L696" s="1"/>
       <c r="M696" s="1"/>
       <c r="N696" s="1"/>
       <c r="O696" s="1">
@@ -30281,9 +29686,7 @@
       <c r="K697" s="1">
         <v>6000</v>
       </c>
-      <c r="L697" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L697" s="1"/>
       <c r="M697" s="1"/>
       <c r="N697" s="1"/>
       <c r="O697" s="1">
@@ -30325,9 +29728,7 @@
       <c r="K698" s="1">
         <v>10250</v>
       </c>
-      <c r="L698" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L698" s="1"/>
       <c r="M698" s="1"/>
       <c r="N698" s="1"/>
       <c r="O698" s="1">
@@ -30369,9 +29770,7 @@
       <c r="K699" s="1">
         <v>1225</v>
       </c>
-      <c r="L699" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L699" s="1"/>
       <c r="M699" s="1"/>
       <c r="N699" s="1"/>
       <c r="O699" s="1">
@@ -30413,9 +29812,7 @@
       <c r="K700" s="1">
         <v>8000</v>
       </c>
-      <c r="L700" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L700" s="1"/>
       <c r="M700" s="1"/>
       <c r="N700" s="1"/>
       <c r="O700" s="1">
@@ -30457,9 +29854,7 @@
       <c r="K701" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L701" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L701" s="1"/>
       <c r="M701" s="1"/>
       <c r="N701" s="1"/>
       <c r="O701" s="1">
@@ -30501,9 +29896,7 @@
       <c r="K702" s="1">
         <v>10250</v>
       </c>
-      <c r="L702" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L702" s="1"/>
       <c r="M702" s="1"/>
       <c r="N702" s="1"/>
       <c r="O702" s="1">
@@ -30545,9 +29938,7 @@
       <c r="K703" s="1">
         <v>19500</v>
       </c>
-      <c r="L703" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L703" s="1"/>
       <c r="M703" s="1"/>
       <c r="N703" s="1"/>
       <c r="O703" s="1">
@@ -30589,9 +29980,7 @@
       <c r="K704" s="1">
         <v>2450</v>
       </c>
-      <c r="L704" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L704" s="1"/>
       <c r="M704" s="1"/>
       <c r="N704" s="1"/>
       <c r="O704" s="1">
@@ -30633,9 +30022,7 @@
       <c r="K705" s="1">
         <v>18000</v>
       </c>
-      <c r="L705" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L705" s="1"/>
       <c r="M705" s="1"/>
       <c r="N705" s="1"/>
       <c r="O705" s="1">
@@ -30677,9 +30064,7 @@
       <c r="K706" s="1">
         <v>1300</v>
       </c>
-      <c r="L706" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L706" s="1"/>
       <c r="M706" s="1"/>
       <c r="N706" s="1"/>
       <c r="O706" s="1">
@@ -30721,9 +30106,7 @@
       <c r="K707" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L707" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L707" s="1"/>
       <c r="M707" s="1"/>
       <c r="N707" s="1"/>
       <c r="O707" s="1">
@@ -30765,9 +30148,7 @@
       <c r="K708" s="1">
         <v>2875</v>
       </c>
-      <c r="L708" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L708" s="1"/>
       <c r="M708" s="1"/>
       <c r="N708" s="1"/>
       <c r="O708" s="1">
@@ -32113,12 +31494,8 @@
       <c r="K743" s="1">
         <v>6000</v>
       </c>
-      <c r="L743" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M743" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L743" s="1"/>
+      <c r="M743" s="1"/>
       <c r="N743" s="1"/>
       <c r="O743" s="1">
         <v>35</v>
@@ -32161,12 +31538,8 @@
       <c r="K744" s="1">
         <v>6125</v>
       </c>
-      <c r="L744" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M744" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L744" s="1"/>
+      <c r="M744" s="1"/>
       <c r="N744" s="1"/>
       <c r="O744" s="1">
         <v>36</v>
@@ -32209,12 +31582,8 @@
       <c r="K745" s="1">
         <v>1300</v>
       </c>
-      <c r="L745" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M745" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L745" s="1"/>
+      <c r="M745" s="1"/>
       <c r="N745" s="1"/>
       <c r="O745" s="1">
         <v>37</v>
@@ -32257,12 +31626,8 @@
       <c r="K746" s="1">
         <v>750</v>
       </c>
-      <c r="L746" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M746" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L746" s="1"/>
+      <c r="M746" s="1"/>
       <c r="N746" s="1"/>
       <c r="O746" s="1">
         <v>38</v>
@@ -32305,12 +31670,8 @@
       <c r="K747" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L747" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M747" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L747" s="1"/>
+      <c r="M747" s="1"/>
       <c r="N747" s="1"/>
       <c r="O747" s="1">
         <v>39</v>
@@ -32351,12 +31712,8 @@
       <c r="K748" s="1">
         <v>25625</v>
       </c>
-      <c r="L748" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M748" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L748" s="1"/>
+      <c r="M748" s="1"/>
       <c r="N748" s="1"/>
       <c r="O748" s="1">
         <v>29</v>
@@ -32397,12 +31754,8 @@
       <c r="K749" s="1">
         <v>19500</v>
       </c>
-      <c r="L749" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M749" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L749" s="1"/>
+      <c r="M749" s="1"/>
       <c r="N749" s="1"/>
       <c r="O749" s="1">
         <v>30</v>
@@ -32443,12 +31796,8 @@
       <c r="K750" s="1">
         <v>2000</v>
       </c>
-      <c r="L750" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M750" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L750" s="1"/>
+      <c r="M750" s="1"/>
       <c r="N750" s="1"/>
       <c r="O750" s="1">
         <v>31</v>
@@ -32489,12 +31838,8 @@
       <c r="K751" s="1">
         <v>1225</v>
       </c>
-      <c r="L751" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M751" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L751" s="1"/>
+      <c r="M751" s="1"/>
       <c r="N751" s="1"/>
       <c r="O751" s="1">
         <v>32</v>
@@ -32535,12 +31880,8 @@
       <c r="K752" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L752" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M752" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L752" s="1"/>
+      <c r="M752" s="1"/>
       <c r="N752" s="1"/>
       <c r="O752" s="1">
         <v>33</v>
@@ -32581,12 +31922,8 @@
       <c r="K753" s="1">
         <v>750</v>
       </c>
-      <c r="L753" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M753" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L753" s="1"/>
+      <c r="M753" s="1"/>
       <c r="N753" s="1"/>
       <c r="O753" s="1">
         <v>34</v>
@@ -32627,12 +31964,8 @@
       <c r="K754" s="1">
         <v>20500</v>
       </c>
-      <c r="L754" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M754" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L754" s="1"/>
+      <c r="M754" s="1"/>
       <c r="N754" s="1"/>
       <c r="O754" s="1">
         <v>22</v>
@@ -32673,12 +32006,8 @@
       <c r="K755" s="1">
         <v>19500</v>
       </c>
-      <c r="L755" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M755" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L755" s="1"/>
+      <c r="M755" s="1"/>
       <c r="N755" s="1"/>
       <c r="O755" s="1">
         <v>23</v>
@@ -32719,12 +32048,8 @@
       <c r="K756" s="1">
         <v>6000</v>
       </c>
-      <c r="L756" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M756" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L756" s="1"/>
+      <c r="M756" s="1"/>
       <c r="N756" s="1"/>
       <c r="O756" s="1">
         <v>24</v>
@@ -32765,12 +32090,8 @@
       <c r="K757" s="1">
         <v>3675</v>
       </c>
-      <c r="L757" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M757" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L757" s="1"/>
+      <c r="M757" s="1"/>
       <c r="N757" s="1"/>
       <c r="O757" s="1">
         <v>25</v>
@@ -32811,12 +32132,8 @@
       <c r="K758" s="1">
         <v>1300</v>
       </c>
-      <c r="L758" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M758" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L758" s="1"/>
+      <c r="M758" s="1"/>
       <c r="N758" s="1"/>
       <c r="O758" s="1">
         <v>26</v>
@@ -32857,12 +32174,8 @@
       <c r="K759" s="1">
         <v>750</v>
       </c>
-      <c r="L759" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M759" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L759" s="1"/>
+      <c r="M759" s="1"/>
       <c r="N759" s="1"/>
       <c r="O759" s="1">
         <v>27</v>
@@ -32903,12 +32216,8 @@
       <c r="K760" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L760" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M760" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L760" s="1"/>
+      <c r="M760" s="1"/>
       <c r="N760" s="1"/>
       <c r="O760" s="1">
         <v>28</v>
@@ -32949,12 +32258,8 @@
       <c r="K761" s="1">
         <v>6000</v>
       </c>
-      <c r="L761" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M761" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L761" s="1"/>
+      <c r="M761" s="1"/>
       <c r="N761" s="1"/>
       <c r="O761" s="1">
         <v>17</v>
@@ -32995,12 +32300,8 @@
       <c r="K762" s="1">
         <v>3675</v>
       </c>
-      <c r="L762" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M762" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L762" s="1"/>
+      <c r="M762" s="1"/>
       <c r="N762" s="1"/>
       <c r="O762" s="1">
         <v>18</v>
@@ -33041,12 +32342,8 @@
       <c r="K763" s="1">
         <v>1300</v>
       </c>
-      <c r="L763" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M763" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L763" s="1"/>
+      <c r="M763" s="1"/>
       <c r="N763" s="1"/>
       <c r="O763" s="1">
         <v>19</v>
@@ -33087,12 +32384,8 @@
       <c r="K764" s="1">
         <v>750</v>
       </c>
-      <c r="L764" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M764" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L764" s="1"/>
+      <c r="M764" s="1"/>
       <c r="N764" s="1"/>
       <c r="O764" s="1">
         <v>20</v>
@@ -33133,12 +32426,8 @@
       <c r="K765" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L765" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M765" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L765" s="1"/>
+      <c r="M765" s="1"/>
       <c r="N765" s="1"/>
       <c r="O765" s="1">
         <v>21</v>
@@ -33179,12 +32468,8 @@
       <c r="K766" s="1">
         <v>25625</v>
       </c>
-      <c r="L766" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M766" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L766" s="1"/>
+      <c r="M766" s="1"/>
       <c r="N766" s="1"/>
       <c r="O766" s="1">
         <v>12</v>
@@ -33225,12 +32510,8 @@
       <c r="K767" s="1">
         <v>19500</v>
       </c>
-      <c r="L767" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M767" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L767" s="1"/>
+      <c r="M767" s="1"/>
       <c r="N767" s="1"/>
       <c r="O767" s="1">
         <v>13</v>
@@ -33271,12 +32552,8 @@
       <c r="K768" s="1">
         <v>4000</v>
       </c>
-      <c r="L768" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M768" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L768" s="1"/>
+      <c r="M768" s="1"/>
       <c r="N768" s="1"/>
       <c r="O768" s="1">
         <v>14</v>
@@ -33317,12 +32594,8 @@
       <c r="K769" s="1">
         <v>1225</v>
       </c>
-      <c r="L769" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M769" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L769" s="1"/>
+      <c r="M769" s="1"/>
       <c r="N769" s="1"/>
       <c r="O769" s="1">
         <v>15</v>
@@ -33363,12 +32636,8 @@
       <c r="K770" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L770" s="1">
-        <v>1500</v>
-      </c>
-      <c r="M770" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L770" s="1"/>
+      <c r="M770" s="1"/>
       <c r="N770" s="1"/>
       <c r="O770" s="1">
         <v>16</v>

</xml_diff>

<commit_message>
Rapport du 15 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -6211,10 +6211,10 @@
         </is>
       </c>
       <c r="J109" s="1" t="n">
-        <v>32.6</v>
+        <v>33.6</v>
       </c>
       <c r="K109" s="1" t="n">
-        <v>399350.0</v>
+        <v>411600.0</v>
       </c>
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>

</xml_diff>

<commit_message>
Rapport du 17 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8918CBA6-C23E-4640-8C18-364995C323D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7439CEF5-14FE-4453-A198-13F9F028313B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -338,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -349,6 +349,12 @@
     <font>
       <sz val="11"/>
       <name val="TIMES"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -711,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E98" workbookViewId="0">
-      <selection activeCell="L112" sqref="L112:N157"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -791,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -837,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
@@ -879,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
@@ -921,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -963,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
@@ -1005,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1047,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
@@ -1089,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -1131,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -1173,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -1215,7 +1221,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1257,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
@@ -1299,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
@@ -1341,7 +1347,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -1383,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -1425,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -1467,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -1509,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1551,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
@@ -1593,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -1635,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1677,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1719,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1761,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1803,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1845,7 +1851,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1887,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1929,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
@@ -1971,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -2013,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -2055,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -2097,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -2139,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>17</v>
@@ -2181,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>17</v>
@@ -2223,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>17</v>
@@ -2265,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>17</v>
@@ -2307,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>17</v>
@@ -2349,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>17</v>
@@ -2391,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>17</v>
@@ -2433,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>17</v>
@@ -2475,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>17</v>
@@ -2517,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>17</v>
@@ -2559,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>17</v>
@@ -2601,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>17</v>
@@ -2643,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>17</v>
@@ -2685,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>17</v>
@@ -2727,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>17</v>
@@ -2769,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>17</v>
@@ -2811,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>17</v>
@@ -2853,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>17</v>
@@ -2895,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>17</v>
@@ -53472,6 +53478,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rpport du 18 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="J9" s="1" t="n">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>162925.0</v>
+        <v>164150.0</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="C124" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D124" s="1" t="inlineStr">
@@ -7235,7 +7235,7 @@
       </c>
       <c r="C125" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D125" s="1" t="inlineStr">
@@ -7293,7 +7293,7 @@
       </c>
       <c r="C126" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D126" s="1" t="inlineStr">
@@ -7351,7 +7351,7 @@
       </c>
       <c r="C127" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D127" s="1" t="inlineStr">
@@ -7409,7 +7409,7 @@
       </c>
       <c r="C128" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D128" s="1" t="inlineStr">
@@ -7467,7 +7467,7 @@
       </c>
       <c r="C129" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D129" s="1" t="inlineStr">
@@ -7525,7 +7525,7 @@
       </c>
       <c r="C130" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D130" s="1" t="inlineStr">
@@ -7583,7 +7583,7 @@
       </c>
       <c r="C131" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D131" s="1" t="inlineStr">
@@ -7641,7 +7641,7 @@
       </c>
       <c r="C132" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D132" s="1" t="inlineStr">
@@ -7699,7 +7699,7 @@
       </c>
       <c r="C133" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D133" s="1" t="inlineStr">
@@ -7757,7 +7757,7 @@
       </c>
       <c r="C134" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D134" s="1" t="inlineStr">
@@ -7815,7 +7815,7 @@
       </c>
       <c r="C135" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D135" s="1" t="inlineStr">
@@ -7873,7 +7873,7 @@
       </c>
       <c r="C136" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D136" s="1" t="inlineStr">
@@ -7931,7 +7931,7 @@
       </c>
       <c r="C137" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D137" s="1" t="inlineStr">
@@ -7989,7 +7989,7 @@
       </c>
       <c r="C138" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D138" s="1" t="inlineStr">
@@ -8047,7 +8047,7 @@
       </c>
       <c r="C139" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D139" s="1" t="inlineStr">
@@ -8105,7 +8105,7 @@
       </c>
       <c r="C140" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D140" s="1" t="inlineStr">
@@ -8163,7 +8163,7 @@
       </c>
       <c r="C141" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D141" s="1" t="inlineStr">
@@ -8221,7 +8221,7 @@
       </c>
       <c r="C142" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D142" s="1" t="inlineStr">
@@ -8279,7 +8279,7 @@
       </c>
       <c r="C143" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D143" s="1" t="inlineStr">
@@ -8337,7 +8337,7 @@
       </c>
       <c r="C144" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D144" s="1" t="inlineStr">
@@ -8395,7 +8395,7 @@
       </c>
       <c r="C145" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D145" s="1" t="inlineStr">
@@ -8453,7 +8453,7 @@
       </c>
       <c r="C146" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D146" s="1" t="inlineStr">
@@ -8511,7 +8511,7 @@
       </c>
       <c r="C147" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D147" s="1" t="inlineStr">
@@ -8569,7 +8569,7 @@
       </c>
       <c r="C148" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D148" s="1" t="inlineStr">
@@ -8627,7 +8627,7 @@
       </c>
       <c r="C149" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D149" s="1" t="inlineStr">
@@ -8685,7 +8685,7 @@
       </c>
       <c r="C150" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D150" s="1" t="inlineStr">
@@ -8743,7 +8743,7 @@
       </c>
       <c r="C151" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D151" s="1" t="inlineStr">
@@ -8801,7 +8801,7 @@
       </c>
       <c r="C152" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D152" s="1" t="inlineStr">
@@ -8859,7 +8859,7 @@
       </c>
       <c r="C153" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D153" s="1" t="inlineStr">
@@ -8917,7 +8917,7 @@
       </c>
       <c r="C154" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D154" s="1" t="inlineStr">
@@ -8975,7 +8975,7 @@
       </c>
       <c r="C155" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D155" s="1" t="inlineStr">
@@ -9033,7 +9033,7 @@
       </c>
       <c r="C156" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D156" s="1" t="inlineStr">
@@ -9091,7 +9091,7 @@
       </c>
       <c r="C157" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D157" s="1" t="inlineStr">
@@ -9149,7 +9149,7 @@
       </c>
       <c r="C158" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D158" s="1" t="inlineStr">
@@ -9207,7 +9207,7 @@
       </c>
       <c r="C159" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D159" s="1" t="inlineStr">
@@ -9265,7 +9265,7 @@
       </c>
       <c r="C160" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D160" s="1" t="inlineStr">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="C161" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D161" s="1" t="inlineStr">
@@ -9381,7 +9381,7 @@
       </c>
       <c r="C162" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D162" s="1" t="inlineStr">
@@ -9439,7 +9439,7 @@
       </c>
       <c r="C163" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D163" s="1" t="inlineStr">
@@ -9497,7 +9497,7 @@
       </c>
       <c r="C164" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D164" s="1" t="inlineStr">
@@ -9555,7 +9555,7 @@
       </c>
       <c r="C165" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D165" s="1" t="inlineStr">
@@ -9613,7 +9613,7 @@
       </c>
       <c r="C166" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D166" s="1" t="inlineStr">
@@ -9671,7 +9671,7 @@
       </c>
       <c r="C167" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D167" s="1" t="inlineStr">
@@ -9729,7 +9729,7 @@
       </c>
       <c r="C168" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D168" s="1" t="inlineStr">
@@ -9787,7 +9787,7 @@
       </c>
       <c r="C169" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D169" s="1" t="inlineStr">
@@ -9845,7 +9845,7 @@
       </c>
       <c r="C170" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D170" s="1" t="inlineStr">
@@ -9903,7 +9903,7 @@
       </c>
       <c r="C171" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D171" s="1" t="inlineStr">
@@ -9961,7 +9961,7 @@
       </c>
       <c r="C172" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D172" s="1" t="inlineStr">
@@ -10019,7 +10019,7 @@
       </c>
       <c r="C173" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D173" s="1" t="inlineStr">
@@ -10077,7 +10077,7 @@
       </c>
       <c r="C174" s="1" t="inlineStr">
         <is>
-          <t>TATA 3</t>
+          <t>TATA 2</t>
         </is>
       </c>
       <c r="D174" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Rapport du 19 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A0D57-F800-4B43-9861-C2C1E7F8623C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFAB990-0133-46A4-ACB0-23CCC1CCA3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -726,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="G162" sqref="G162:G191"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4422,7 +4435,7 @@
         <v>0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>42</v>
@@ -4464,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>42</v>
@@ -4506,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>42</v>
@@ -4548,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>42</v>
@@ -4590,7 +4603,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>42</v>
@@ -4632,7 +4645,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>42</v>
@@ -4674,7 +4687,7 @@
         <v>0</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>42</v>
@@ -4716,7 +4729,7 @@
         <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>42</v>
@@ -4758,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>42</v>
@@ -4800,7 +4813,7 @@
         <v>0</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>42</v>
@@ -4842,7 +4855,7 @@
         <v>0</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>42</v>
@@ -4884,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>42</v>
@@ -4926,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>42</v>
@@ -4968,7 +4981,7 @@
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>42</v>
@@ -5010,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>42</v>
@@ -5052,7 +5065,7 @@
         <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>42</v>
@@ -5094,7 +5107,7 @@
         <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>42</v>
@@ -5136,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>42</v>
@@ -5178,7 +5191,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>42</v>
@@ -5220,7 +5233,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>42</v>
@@ -5262,7 +5275,7 @@
         <v>0</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>42</v>
@@ -5304,7 +5317,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>42</v>
@@ -5346,7 +5359,7 @@
         <v>0</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>42</v>
@@ -5388,7 +5401,7 @@
         <v>0</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>42</v>
@@ -5430,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>42</v>
@@ -5472,7 +5485,7 @@
         <v>0</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>42</v>
@@ -5514,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>42</v>
@@ -5556,7 +5569,7 @@
         <v>0</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Rapport du 22 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -76,7 +76,7 @@
     <col min="5" max="5" width="16.5234375" customWidth="true"/>
     <col min="6" max="6" width="12.36328125" customWidth="true"/>
     <col min="7" max="7" width="20.43359375" customWidth="true"/>
-    <col min="8" max="8" width="15.54296875" customWidth="true"/>
+    <col min="8" max="8" width="19.3359375" customWidth="true"/>
     <col min="9" max="9" width="37.31640625" customWidth="true"/>
     <col min="10" max="10" width="13.96484375" customWidth="true"/>
     <col min="11" max="11" width="11.515625" customWidth="true"/>
@@ -181,7 +181,7 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>DJIBRIL DIOP</t>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -201,7 +201,7 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>Seynabou sow RZ</t>
+          <t>Ndague Ndao</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
@@ -210,18 +210,16 @@
         </is>
       </c>
       <c r="J2" s="1" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>39000.0</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>4000.0</v>
-      </c>
+        <v>97500.0</v>
+      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="n">
-        <v>101.0</v>
+        <v>104.0</v>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
@@ -238,7 +236,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -268,14 +266,14 @@
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J3" s="1" t="n">
         <v>2.0</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>20500.0</v>
+        <v>39000.0</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>4000.0</v>
@@ -283,7 +281,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="n">
-        <v>102.0</v>
+        <v>101.0</v>
       </c>
       <c r="P3" s="1" t="inlineStr">
         <is>
@@ -300,7 +298,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -330,14 +328,14 @@
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J4" s="1" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>12250.0</v>
+        <v>20500.0</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>4000.0</v>
@@ -345,7 +343,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="n">
-        <v>103.0</v>
+        <v>102.0</v>
       </c>
       <c r="P4" s="1" t="inlineStr">
         <is>
@@ -362,7 +360,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -387,7 +385,7 @@
       </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
-          <t>Mariama sadio</t>
+          <t>Seynabou sow RZ</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
@@ -407,7 +405,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="n">
-        <v>100.0</v>
+        <v>103.0</v>
       </c>
       <c r="P5" s="1" t="inlineStr">
         <is>
@@ -424,7 +422,7 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
@@ -444,20 +442,24 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>Fatou THIOMBENE</t>
-        </is>
-      </c>
-      <c r="H6" s="1"/>
+          <t>Autre</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>Mariama sadio</t>
+        </is>
+      </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
           <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J6" s="1" t="n">
-        <v>0.3</v>
+        <v>1.0</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>3675.0</v>
+        <v>12250.0</v>
       </c>
       <c r="L6" s="1" t="n">
         <v>4000.0</v>
@@ -465,7 +467,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="n">
-        <v>96.0</v>
+        <v>100.0</v>
       </c>
       <c r="P6" s="1" t="inlineStr">
         <is>
@@ -482,7 +484,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -508,14 +510,14 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.3</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>729.1667</v>
+        <v>3675.0</v>
       </c>
       <c r="L7" s="1" t="n">
         <v>4000.0</v>
@@ -523,7 +525,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1" t="n">
-        <v>97.0</v>
+        <v>96.0</v>
       </c>
       <c r="P7" s="1" t="inlineStr">
         <is>
@@ -540,7 +542,7 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
@@ -566,14 +568,14 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0.083333336</v>
+        <v>0.041666668</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>2875.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L8" s="1" t="n">
         <v>4000.0</v>
@@ -581,7 +583,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="n">
-        <v>98.0</v>
+        <v>97.0</v>
       </c>
       <c r="P8" s="1" t="inlineStr">
         <is>
@@ -598,7 +600,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -624,14 +626,14 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J9" s="1" t="n">
-        <v>1.0</v>
+        <v>0.083333336</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>10250.0</v>
+        <v>2875.0</v>
       </c>
       <c r="L9" s="1" t="n">
         <v>4000.0</v>
@@ -639,7 +641,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="n">
-        <v>99.0</v>
+        <v>98.0</v>
       </c>
       <c r="P9" s="1" t="inlineStr">
         <is>
@@ -656,7 +658,7 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
@@ -676,7 +678,7 @@
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>Anta CISSE</t>
+          <t>Fatou THIOMBENE</t>
         </is>
       </c>
       <c r="H10" s="1"/>
@@ -686,10 +688,10 @@
         </is>
       </c>
       <c r="J10" s="1" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>5125.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L10" s="1" t="n">
         <v>4000.0</v>
@@ -697,7 +699,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="n">
-        <v>94.0</v>
+        <v>99.0</v>
       </c>
       <c r="P10" s="1" t="inlineStr">
         <is>
@@ -714,7 +716,7 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
@@ -740,14 +742,14 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>4900.0</v>
+        <v>5125.0</v>
       </c>
       <c r="L11" s="1" t="n">
         <v>4000.0</v>
@@ -755,7 +757,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="n">
-        <v>95.0</v>
+        <v>94.0</v>
       </c>
       <c r="P11" s="1" t="inlineStr">
         <is>
@@ -772,7 +774,7 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
@@ -792,20 +794,20 @@
       </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>Aida SENE</t>
+          <t>Anta CISSE</t>
         </is>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J12" s="1" t="n">
-        <v>1.0</v>
+        <v>0.4</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>10250.0</v>
+        <v>4900.0</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>4000.0</v>
@@ -813,7 +815,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1" t="n">
-        <v>92.0</v>
+        <v>95.0</v>
       </c>
       <c r="P12" s="1" t="inlineStr">
         <is>
@@ -830,7 +832,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
@@ -856,14 +858,14 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J13" s="1" t="n">
-        <v>0.2</v>
+        <v>1.0</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>2450.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>4000.0</v>
@@ -871,7 +873,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="n">
-        <v>93.0</v>
+        <v>92.0</v>
       </c>
       <c r="P13" s="1" t="inlineStr">
         <is>
@@ -888,7 +890,7 @@
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
@@ -908,20 +910,20 @@
       </c>
       <c r="G14" s="1" t="inlineStr">
         <is>
-          <t>Alimatou BADIANE</t>
+          <t>Aida SENE</t>
         </is>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J14" s="1" t="n">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>29250.0</v>
+        <v>2450.0</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>4000.0</v>
@@ -929,7 +931,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1" t="n">
-        <v>89.0</v>
+        <v>93.0</v>
       </c>
       <c r="P14" s="1" t="inlineStr">
         <is>
@@ -946,7 +948,7 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
@@ -972,14 +974,14 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J15" s="1" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>5125.0</v>
+        <v>29250.0</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>4000.0</v>
@@ -987,7 +989,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="n">
-        <v>90.0</v>
+        <v>89.0</v>
       </c>
       <c r="P15" s="1" t="inlineStr">
         <is>
@@ -1004,7 +1006,7 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
@@ -1030,14 +1032,14 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J16" s="1" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>2450.0</v>
+        <v>5125.0</v>
       </c>
       <c r="L16" s="1" t="n">
         <v>4000.0</v>
@@ -1045,7 +1047,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1" t="n">
-        <v>91.0</v>
+        <v>90.0</v>
       </c>
       <c r="P16" s="1" t="inlineStr">
         <is>
@@ -1062,7 +1064,7 @@
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
@@ -1082,20 +1084,20 @@
       </c>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>Khady SANE</t>
+          <t>Alimatou BADIANE</t>
         </is>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>KamLac Lait concentré sucré 24x1kg</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J17" s="1" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="K17" s="1" t="n">
-        <v>14250.0</v>
+        <v>2450.0</v>
       </c>
       <c r="L17" s="1" t="n">
         <v>4000.0</v>
@@ -1103,7 +1105,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1" t="n">
-        <v>86.0</v>
+        <v>91.0</v>
       </c>
       <c r="P17" s="1" t="inlineStr">
         <is>
@@ -1120,7 +1122,7 @@
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D18" s="1" t="inlineStr">
@@ -1146,14 +1148,14 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>KamLac Lait concentré sucré 24x1kg</t>
         </is>
       </c>
       <c r="J18" s="1" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>3675.0</v>
+        <v>14250.0</v>
       </c>
       <c r="L18" s="1" t="n">
         <v>4000.0</v>
@@ -1161,7 +1163,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1" t="n">
-        <v>87.0</v>
+        <v>86.0</v>
       </c>
       <c r="P18" s="1" t="inlineStr">
         <is>
@@ -1178,7 +1180,7 @@
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
@@ -1204,14 +1206,14 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J19" s="1" t="n">
-        <v>2.0</v>
+        <v>0.3</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>39000.0</v>
+        <v>3675.0</v>
       </c>
       <c r="L19" s="1" t="n">
         <v>4000.0</v>
@@ -1219,7 +1221,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1" t="n">
-        <v>88.0</v>
+        <v>87.0</v>
       </c>
       <c r="P19" s="1" t="inlineStr">
         <is>
@@ -1236,7 +1238,7 @@
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
@@ -1256,20 +1258,20 @@
       </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
-          <t>Colle CISSE</t>
+          <t>Khady SANE</t>
         </is>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J20" s="1" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>10250.0</v>
+        <v>39000.0</v>
       </c>
       <c r="L20" s="1" t="n">
         <v>4000.0</v>
@@ -1277,7 +1279,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1" t="n">
-        <v>81.0</v>
+        <v>88.0</v>
       </c>
       <c r="P20" s="1" t="inlineStr">
         <is>
@@ -1294,7 +1296,7 @@
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
@@ -1320,14 +1322,14 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J21" s="1" t="n">
         <v>1.0</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>12250.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>4000.0</v>
@@ -1335,7 +1337,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1" t="n">
-        <v>82.0</v>
+        <v>81.0</v>
       </c>
       <c r="P21" s="1" t="inlineStr">
         <is>
@@ -1352,7 +1354,7 @@
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
@@ -1378,14 +1380,14 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J22" s="1" t="n">
-        <v>0.041666668</v>
+        <v>1.0</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>729.1667</v>
+        <v>12250.0</v>
       </c>
       <c r="L22" s="1" t="n">
         <v>4000.0</v>
@@ -1393,7 +1395,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1" t="n">
-        <v>83.0</v>
+        <v>82.0</v>
       </c>
       <c r="P22" s="1" t="inlineStr">
         <is>
@@ -1410,7 +1412,7 @@
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
@@ -1436,14 +1438,14 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J23" s="1" t="n">
         <v>0.041666668</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>1395.8334</v>
+        <v>729.1667</v>
       </c>
       <c r="L23" s="1" t="n">
         <v>4000.0</v>
@@ -1451,7 +1453,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1" t="n">
-        <v>84.0</v>
+        <v>83.0</v>
       </c>
       <c r="P23" s="1" t="inlineStr">
         <is>
@@ -1468,7 +1470,7 @@
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D24" s="1" t="inlineStr">
@@ -1494,14 +1496,14 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>KamLac Lait concentré sucré 24x1kg</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J24" s="1" t="n">
-        <v>0.29166666</v>
+        <v>0.041666668</v>
       </c>
       <c r="K24" s="1" t="n">
-        <v>8312.5</v>
+        <v>1395.8334</v>
       </c>
       <c r="L24" s="1" t="n">
         <v>4000.0</v>
@@ -1509,7 +1511,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1" t="n">
-        <v>85.0</v>
+        <v>84.0</v>
       </c>
       <c r="P24" s="1" t="inlineStr">
         <is>
@@ -1526,7 +1528,7 @@
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D25" s="1" t="inlineStr">
@@ -1546,20 +1548,20 @@
       </c>
       <c r="G25" s="1" t="inlineStr">
         <is>
-          <t>Fama DIOUF</t>
+          <t>Colle CISSE</t>
         </is>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>KamLac Lait concentré sucré 24x1kg</t>
         </is>
       </c>
       <c r="J25" s="1" t="n">
-        <v>5.0</v>
+        <v>0.29166666</v>
       </c>
       <c r="K25" s="1" t="n">
-        <v>97500.0</v>
+        <v>8312.5</v>
       </c>
       <c r="L25" s="1" t="n">
         <v>4000.0</v>
@@ -1567,7 +1569,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1" t="n">
-        <v>80.0</v>
+        <v>85.0</v>
       </c>
       <c r="P25" s="1" t="inlineStr">
         <is>
@@ -1584,7 +1586,7 @@
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
@@ -1604,7 +1606,7 @@
       </c>
       <c r="G26" s="1" t="inlineStr">
         <is>
-          <t>Ibrahima COLY</t>
+          <t>Fama DIOUF</t>
         </is>
       </c>
       <c r="H26" s="1"/>
@@ -1614,10 +1616,10 @@
         </is>
       </c>
       <c r="J26" s="1" t="n">
-        <v>1.5</v>
+        <v>5.0</v>
       </c>
       <c r="K26" s="1" t="n">
-        <v>29250.0</v>
+        <v>97500.0</v>
       </c>
       <c r="L26" s="1" t="n">
         <v>4000.0</v>
@@ -1625,7 +1627,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1" t="n">
-        <v>76.0</v>
+        <v>80.0</v>
       </c>
       <c r="P26" s="1" t="inlineStr">
         <is>
@@ -1642,7 +1644,7 @@
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
@@ -1668,14 +1670,14 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J27" s="1" t="n">
-        <v>1.0</v>
+        <v>1.5</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>10250.0</v>
+        <v>29250.0</v>
       </c>
       <c r="L27" s="1" t="n">
         <v>4000.0</v>
@@ -1683,7 +1685,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1" t="n">
-        <v>77.0</v>
+        <v>76.0</v>
       </c>
       <c r="P27" s="1" t="inlineStr">
         <is>
@@ -1700,7 +1702,7 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
@@ -1726,14 +1728,14 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J28" s="1" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>6125.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L28" s="1" t="n">
         <v>4000.0</v>
@@ -1741,7 +1743,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1" t="n">
-        <v>78.0</v>
+        <v>77.0</v>
       </c>
       <c r="P28" s="1" t="inlineStr">
         <is>
@@ -1758,7 +1760,7 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
@@ -1784,14 +1786,14 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J29" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.5</v>
       </c>
       <c r="K29" s="1" t="n">
-        <v>1395.8334</v>
+        <v>6125.0</v>
       </c>
       <c r="L29" s="1" t="n">
         <v>4000.0</v>
@@ -1799,7 +1801,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1" t="n">
-        <v>79.0</v>
+        <v>78.0</v>
       </c>
       <c r="P29" s="1" t="inlineStr">
         <is>
@@ -1816,7 +1818,7 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
@@ -1836,20 +1838,20 @@
       </c>
       <c r="G30" s="1" t="inlineStr">
         <is>
-          <t>Saly SEYDI</t>
+          <t>Ibrahima COLY</t>
         </is>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J30" s="1" t="n">
-        <v>1.6</v>
+        <v>0.041666668</v>
       </c>
       <c r="K30" s="1" t="n">
-        <v>19600.0</v>
+        <v>1395.8334</v>
       </c>
       <c r="L30" s="1" t="n">
         <v>4000.0</v>
@@ -1857,7 +1859,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1" t="n">
-        <v>71.0</v>
+        <v>79.0</v>
       </c>
       <c r="P30" s="1" t="inlineStr">
         <is>
@@ -1874,7 +1876,7 @@
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
@@ -1900,14 +1902,14 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J31" s="1" t="n">
-        <v>0.041666668</v>
+        <v>1.6</v>
       </c>
       <c r="K31" s="1" t="n">
-        <v>427.08334</v>
+        <v>19600.0</v>
       </c>
       <c r="L31" s="1" t="n">
         <v>4000.0</v>
@@ -1915,7 +1917,7 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1" t="n">
-        <v>72.0</v>
+        <v>71.0</v>
       </c>
       <c r="P31" s="1" t="inlineStr">
         <is>
@@ -1932,7 +1934,7 @@
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D32" s="1" t="inlineStr">
@@ -1958,14 +1960,14 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J32" s="1" t="n">
-        <v>0.5</v>
+        <v>0.041666668</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>9750.0</v>
+        <v>427.08334</v>
       </c>
       <c r="L32" s="1" t="n">
         <v>4000.0</v>
@@ -1973,7 +1975,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1" t="n">
-        <v>73.0</v>
+        <v>72.0</v>
       </c>
       <c r="P32" s="1" t="inlineStr">
         <is>
@@ -1990,7 +1992,7 @@
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D33" s="1" t="inlineStr">
@@ -2016,14 +2018,14 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J33" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.5</v>
       </c>
       <c r="K33" s="1" t="n">
-        <v>1395.8334</v>
+        <v>9750.0</v>
       </c>
       <c r="L33" s="1" t="n">
         <v>4000.0</v>
@@ -2031,7 +2033,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1" t="n">
-        <v>74.0</v>
+        <v>73.0</v>
       </c>
       <c r="P33" s="1" t="inlineStr">
         <is>
@@ -2048,7 +2050,7 @@
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D34" s="1" t="inlineStr">
@@ -2074,14 +2076,14 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J34" s="1" t="n">
         <v>0.041666668</v>
       </c>
       <c r="K34" s="1" t="n">
-        <v>729.1667</v>
+        <v>1395.8334</v>
       </c>
       <c r="L34" s="1" t="n">
         <v>4000.0</v>
@@ -2089,7 +2091,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1" t="n">
-        <v>75.0</v>
+        <v>74.0</v>
       </c>
       <c r="P34" s="1" t="inlineStr">
         <is>
@@ -2106,7 +2108,7 @@
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D35" s="1" t="inlineStr">
@@ -2126,20 +2128,20 @@
       </c>
       <c r="G35" s="1" t="inlineStr">
         <is>
-          <t>Fatou TEUW</t>
+          <t>Saly SEYDI</t>
         </is>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J35" s="1" t="n">
-        <v>0.5</v>
+        <v>0.041666668</v>
       </c>
       <c r="K35" s="1" t="n">
-        <v>5125.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L35" s="1" t="n">
         <v>4000.0</v>
@@ -2147,7 +2149,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1" t="n">
-        <v>66.0</v>
+        <v>75.0</v>
       </c>
       <c r="P35" s="1" t="inlineStr">
         <is>
@@ -2164,7 +2166,7 @@
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D36" s="1" t="inlineStr">
@@ -2190,14 +2192,14 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J36" s="1" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="K36" s="1" t="n">
-        <v>7350.0</v>
+        <v>5125.0</v>
       </c>
       <c r="L36" s="1" t="n">
         <v>4000.0</v>
@@ -2205,7 +2207,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1" t="n">
-        <v>67.0</v>
+        <v>66.0</v>
       </c>
       <c r="P36" s="1" t="inlineStr">
         <is>
@@ -2222,7 +2224,7 @@
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D37" s="1" t="inlineStr">
@@ -2248,14 +2250,14 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J37" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.6</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>729.1667</v>
+        <v>7350.0</v>
       </c>
       <c r="L37" s="1" t="n">
         <v>4000.0</v>
@@ -2263,7 +2265,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1" t="n">
-        <v>68.0</v>
+        <v>67.0</v>
       </c>
       <c r="P37" s="1" t="inlineStr">
         <is>
@@ -2280,7 +2282,7 @@
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D38" s="1" t="inlineStr">
@@ -2306,14 +2308,14 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J38" s="1" t="n">
         <v>0.041666668</v>
       </c>
       <c r="K38" s="1" t="n">
-        <v>1395.8334</v>
+        <v>729.1667</v>
       </c>
       <c r="L38" s="1" t="n">
         <v>4000.0</v>
@@ -2321,7 +2323,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1" t="n">
-        <v>69.0</v>
+        <v>68.0</v>
       </c>
       <c r="P38" s="1" t="inlineStr">
         <is>
@@ -2338,7 +2340,7 @@
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D39" s="1" t="inlineStr">
@@ -2364,14 +2366,14 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J39" s="1" t="n">
-        <v>0.083333336</v>
+        <v>0.041666668</v>
       </c>
       <c r="K39" s="1" t="n">
-        <v>2875.0</v>
+        <v>1395.8334</v>
       </c>
       <c r="L39" s="1" t="n">
         <v>4000.0</v>
@@ -2379,7 +2381,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1" t="n">
-        <v>70.0</v>
+        <v>69.0</v>
       </c>
       <c r="P39" s="1" t="inlineStr">
         <is>
@@ -2396,7 +2398,7 @@
       </c>
       <c r="C40" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D40" s="1" t="inlineStr">
@@ -2416,20 +2418,20 @@
       </c>
       <c r="G40" s="1" t="inlineStr">
         <is>
-          <t>Adama DABO</t>
+          <t>Fatou TEUW</t>
         </is>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J40" s="1" t="n">
-        <v>1.5</v>
+        <v>0.083333336</v>
       </c>
       <c r="K40" s="1" t="n">
-        <v>15375.0</v>
+        <v>2875.0</v>
       </c>
       <c r="L40" s="1" t="n">
         <v>4000.0</v>
@@ -2437,7 +2439,7 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1" t="n">
-        <v>64.0</v>
+        <v>70.0</v>
       </c>
       <c r="P40" s="1" t="inlineStr">
         <is>
@@ -2454,7 +2456,7 @@
       </c>
       <c r="C41" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D41" s="1" t="inlineStr">
@@ -2480,14 +2482,14 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J41" s="1" t="n">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="K41" s="1" t="n">
-        <v>1225.0</v>
+        <v>15375.0</v>
       </c>
       <c r="L41" s="1" t="n">
         <v>4000.0</v>
@@ -2495,7 +2497,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1" t="n">
-        <v>65.0</v>
+        <v>64.0</v>
       </c>
       <c r="P41" s="1" t="inlineStr">
         <is>
@@ -2512,38 +2514,48 @@
       </c>
       <c r="C42" s="1" t="inlineStr">
         <is>
-          <t>TATA 2</t>
+          <t>TATA 1</t>
         </is>
       </c>
       <c r="D42" s="1" t="inlineStr">
         <is>
-          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+          <t>DJIBRIL DIOP</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr">
         <is>
-          <t>Stock Descente</t>
-        </is>
-      </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+          <t>Vente</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>THIAROYE</t>
+        </is>
+      </c>
+      <c r="G42" s="1" t="inlineStr">
+        <is>
+          <t>Adama DABO</t>
+        </is>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J42" s="1" t="n">
-        <v>47.0</v>
+        <v>0.1</v>
       </c>
       <c r="K42" s="1" t="n">
-        <v>481750.0</v>
-      </c>
-      <c r="L42" s="1"/>
+        <v>1225.0</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>4000.0</v>
+      </c>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1" t="n">
-        <v>53.0</v>
+        <v>65.0</v>
       </c>
       <c r="P42" s="1" t="inlineStr">
         <is>
@@ -2578,20 +2590,20 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J43" s="1" t="n">
-        <v>13.0</v>
+        <v>47.0</v>
       </c>
       <c r="K43" s="1" t="n">
-        <v>253500.0</v>
+        <v>481750.0</v>
       </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1" t="n">
-        <v>54.0</v>
+        <v>53.0</v>
       </c>
       <c r="P43" s="1" t="inlineStr">
         <is>
@@ -2626,20 +2638,20 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J44" s="1" t="n">
-        <v>26.25</v>
+        <v>13.0</v>
       </c>
       <c r="K44" s="1" t="n">
-        <v>459375.0</v>
+        <v>253500.0</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1" t="n">
-        <v>55.0</v>
+        <v>54.0</v>
       </c>
       <c r="P44" s="1" t="inlineStr">
         <is>
@@ -2674,20 +2686,20 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J45" s="1" t="n">
-        <v>8.583333</v>
+        <v>26.25</v>
       </c>
       <c r="K45" s="1" t="n">
-        <v>287541.66</v>
+        <v>459375.0</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1" t="n">
-        <v>56.0</v>
+        <v>55.0</v>
       </c>
       <c r="P45" s="1" t="inlineStr">
         <is>
@@ -2722,20 +2734,20 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J46" s="1" t="n">
-        <v>22.666666</v>
+        <v>8.583333</v>
       </c>
       <c r="K46" s="1" t="n">
-        <v>782000.0</v>
+        <v>287541.66</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1" t="n">
-        <v>57.0</v>
+        <v>56.0</v>
       </c>
       <c r="P46" s="1" t="inlineStr">
         <is>
@@ -2770,20 +2782,20 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1" t="inlineStr">
         <is>
-          <t>KamLac Lait concentré sucré 24x1kg</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J47" s="1" t="n">
-        <v>30.5</v>
+        <v>22.666666</v>
       </c>
       <c r="K47" s="1" t="n">
-        <v>869250.0</v>
+        <v>782000.0</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1" t="n">
-        <v>58.0</v>
+        <v>57.0</v>
       </c>
       <c r="P47" s="1" t="inlineStr">
         <is>
@@ -2818,20 +2830,20 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 18gx100</t>
+          <t>KamLac Lait concentré sucré 24x1kg</t>
         </is>
       </c>
       <c r="J48" s="1" t="n">
-        <v>34.4</v>
+        <v>30.5</v>
       </c>
       <c r="K48" s="1" t="n">
-        <v>223600.0</v>
+        <v>869250.0</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1" t="n">
-        <v>59.0</v>
+        <v>58.0</v>
       </c>
       <c r="P48" s="1" t="inlineStr">
         <is>
@@ -2866,20 +2878,20 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="inlineStr">
         <is>
-          <t>Lait Kamlac sachet 18gx100</t>
+          <t>Lait Janus 18gx100</t>
         </is>
       </c>
       <c r="J49" s="1" t="n">
-        <v>20.6</v>
+        <v>34.4</v>
       </c>
       <c r="K49" s="1" t="n">
-        <v>154500.0</v>
+        <v>223600.0</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1" t="n">
-        <v>60.0</v>
+        <v>59.0</v>
       </c>
       <c r="P49" s="1" t="inlineStr">
         <is>
@@ -2914,20 +2926,20 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Lait Kamlac sachet 18gx100</t>
         </is>
       </c>
       <c r="J50" s="1" t="n">
-        <v>29.3</v>
+        <v>20.6</v>
       </c>
       <c r="K50" s="1" t="n">
-        <v>358925.0</v>
+        <v>154500.0</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1" t="n">
-        <v>61.0</v>
+        <v>60.0</v>
       </c>
       <c r="P50" s="1" t="inlineStr">
         <is>
@@ -2962,20 +2974,20 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 20gx100</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J51" s="1" t="n">
-        <v>13.1</v>
+        <v>29.3</v>
       </c>
       <c r="K51" s="1" t="n">
-        <v>85150.0</v>
+        <v>358925.0</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1" t="n">
-        <v>62.0</v>
+        <v>61.0</v>
       </c>
       <c r="P51" s="1" t="inlineStr">
         <is>
@@ -3010,20 +3022,20 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="inlineStr">
         <is>
-          <t>Jus Lido</t>
+          <t>Lait Janus 20gx100</t>
         </is>
       </c>
       <c r="J52" s="1" t="n">
-        <v>44.166668</v>
+        <v>13.1</v>
       </c>
       <c r="K52" s="1" t="n">
-        <v>530000.0</v>
+        <v>85150.0</v>
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1" t="n">
-        <v>63.0</v>
+        <v>62.0</v>
       </c>
       <c r="P52" s="1" t="inlineStr">
         <is>
@@ -3050,38 +3062,28 @@
       </c>
       <c r="E53" s="1" t="inlineStr">
         <is>
-          <t>Vente</t>
-        </is>
-      </c>
-      <c r="F53" s="1" t="inlineStr">
-        <is>
-          <t>THIAROYE</t>
-        </is>
-      </c>
-      <c r="G53" s="1" t="inlineStr">
-        <is>
-          <t>Autre</t>
-        </is>
-      </c>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Jus Lido</t>
         </is>
       </c>
       <c r="J53" s="1" t="n">
-        <v>1.1</v>
+        <v>44.166668</v>
       </c>
       <c r="K53" s="1" t="n">
-        <v>13475.0</v>
-      </c>
-      <c r="L53" s="1" t="n">
-        <v>1000.0</v>
-      </c>
+        <v>530000.0</v>
+      </c>
+      <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1" t="n">
-        <v>52.0</v>
+        <v>63.0</v>
       </c>
       <c r="P53" s="1" t="inlineStr">
         <is>
@@ -3118,20 +3120,24 @@
       </c>
       <c r="G54" s="1" t="inlineStr">
         <is>
-          <t>Arthur NGOM</t>
-        </is>
-      </c>
-      <c r="H54" s="1"/>
+          <t>Autre</t>
+        </is>
+      </c>
+      <c r="H54" s="1" t="inlineStr">
+        <is>
+          <t>Codou SAMOURE</t>
+        </is>
+      </c>
       <c r="I54" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J54" s="1" t="n">
-        <v>1.0</v>
+        <v>1.1</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>10250.0</v>
+        <v>13475.0</v>
       </c>
       <c r="L54" s="1" t="n">
         <v>1000.0</v>
@@ -3139,7 +3145,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1" t="n">
-        <v>48.0</v>
+        <v>52.0</v>
       </c>
       <c r="P54" s="1" t="inlineStr">
         <is>
@@ -3182,14 +3188,14 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J55" s="1" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="K55" s="1" t="n">
-        <v>16750.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L55" s="1" t="n">
         <v>1000.0</v>
@@ -3197,7 +3203,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1" t="n">
-        <v>49.0</v>
+        <v>48.0</v>
       </c>
       <c r="P55" s="1" t="inlineStr">
         <is>
@@ -3240,14 +3246,14 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J56" s="1" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K56" s="1" t="n">
-        <v>1225.0</v>
+        <v>16750.0</v>
       </c>
       <c r="L56" s="1" t="n">
         <v>1000.0</v>
@@ -3255,7 +3261,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1" t="n">
-        <v>50.0</v>
+        <v>49.0</v>
       </c>
       <c r="P56" s="1" t="inlineStr">
         <is>
@@ -3298,14 +3304,14 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J57" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.1</v>
       </c>
       <c r="K57" s="1" t="n">
-        <v>1395.8334</v>
+        <v>1225.0</v>
       </c>
       <c r="L57" s="1" t="n">
         <v>1000.0</v>
@@ -3313,7 +3319,7 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1" t="n">
-        <v>51.0</v>
+        <v>50.0</v>
       </c>
       <c r="P57" s="1" t="inlineStr">
         <is>
@@ -3350,7 +3356,7 @@
       </c>
       <c r="G58" s="1" t="inlineStr">
         <is>
-          <t>Papa SAMOURE</t>
+          <t>Arthur NGOM</t>
         </is>
       </c>
       <c r="H58" s="1"/>
@@ -3360,10 +3366,10 @@
         </is>
       </c>
       <c r="J58" s="1" t="n">
-        <v>0.5</v>
+        <v>0.041666668</v>
       </c>
       <c r="K58" s="1" t="n">
-        <v>16750.0</v>
+        <v>1395.8334</v>
       </c>
       <c r="L58" s="1" t="n">
         <v>1000.0</v>
@@ -3371,7 +3377,7 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1" t="n">
-        <v>46.0</v>
+        <v>51.0</v>
       </c>
       <c r="P58" s="1" t="inlineStr">
         <is>
@@ -3414,14 +3420,14 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J59" s="1" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>10250.0</v>
+        <v>16750.0</v>
       </c>
       <c r="L59" s="1" t="n">
         <v>1000.0</v>
@@ -3429,7 +3435,7 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1" t="n">
-        <v>47.0</v>
+        <v>46.0</v>
       </c>
       <c r="P59" s="1" t="inlineStr">
         <is>
@@ -3466,7 +3472,7 @@
       </c>
       <c r="G60" s="1" t="inlineStr">
         <is>
-          <t>Arabe DIEDHIOU</t>
+          <t>Papa SAMOURE</t>
         </is>
       </c>
       <c r="H60" s="1"/>
@@ -3476,10 +3482,10 @@
         </is>
       </c>
       <c r="J60" s="1" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K60" s="1" t="n">
-        <v>20500.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L60" s="1" t="n">
         <v>1000.0</v>
@@ -3487,7 +3493,7 @@
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1" t="n">
-        <v>42.0</v>
+        <v>47.0</v>
       </c>
       <c r="P60" s="1" t="inlineStr">
         <is>
@@ -3530,14 +3536,14 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J61" s="1" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K61" s="1" t="n">
-        <v>58500.0</v>
+        <v>20500.0</v>
       </c>
       <c r="L61" s="1" t="n">
         <v>1000.0</v>
@@ -3545,7 +3551,7 @@
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1" t="n">
-        <v>43.0</v>
+        <v>42.0</v>
       </c>
       <c r="P61" s="1" t="inlineStr">
         <is>
@@ -3588,14 +3594,14 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J62" s="1" t="n">
-        <v>0.1</v>
+        <v>3.0</v>
       </c>
       <c r="K62" s="1" t="n">
-        <v>1225.0</v>
+        <v>58500.0</v>
       </c>
       <c r="L62" s="1" t="n">
         <v>1000.0</v>
@@ -3603,7 +3609,7 @@
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="P62" s="1" t="inlineStr">
         <is>
@@ -3646,14 +3652,14 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J63" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.1</v>
       </c>
       <c r="K63" s="1" t="n">
-        <v>729.1667</v>
+        <v>1225.0</v>
       </c>
       <c r="L63" s="1" t="n">
         <v>1000.0</v>
@@ -3661,7 +3667,7 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1" t="n">
-        <v>45.0</v>
+        <v>44.0</v>
       </c>
       <c r="P63" s="1" t="inlineStr">
         <is>
@@ -3698,20 +3704,20 @@
       </c>
       <c r="G64" s="1" t="inlineStr">
         <is>
-          <t>Aissatou DIALLO</t>
+          <t>Arabe DIEDHIOU</t>
         </is>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J64" s="1" t="n">
-        <v>1.0</v>
+        <v>0.041666668</v>
       </c>
       <c r="K64" s="1" t="n">
-        <v>10250.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L64" s="1" t="n">
         <v>1000.0</v>
@@ -3719,7 +3725,7 @@
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1" t="n">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="P64" s="1" t="inlineStr">
         <is>
@@ -3762,14 +3768,14 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J65" s="1" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="K65" s="1" t="n">
-        <v>6125.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L65" s="1" t="n">
         <v>1000.0</v>
@@ -3777,7 +3783,7 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1" t="n">
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="P65" s="1" t="inlineStr">
         <is>
@@ -3820,14 +3826,14 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J66" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.5</v>
       </c>
       <c r="K66" s="1" t="n">
-        <v>729.1667</v>
+        <v>6125.0</v>
       </c>
       <c r="L66" s="1" t="n">
         <v>1000.0</v>
@@ -3835,7 +3841,7 @@
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1" t="n">
-        <v>41.0</v>
+        <v>40.0</v>
       </c>
       <c r="P66" s="1" t="inlineStr">
         <is>
@@ -3872,20 +3878,20 @@
       </c>
       <c r="G67" s="1" t="inlineStr">
         <is>
-          <t>Khady Gueye</t>
+          <t>Aissatou DIALLO</t>
         </is>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J67" s="1" t="n">
-        <v>0.5</v>
+        <v>0.041666668</v>
       </c>
       <c r="K67" s="1" t="n">
-        <v>5125.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L67" s="1" t="n">
         <v>1000.0</v>
@@ -3893,7 +3899,7 @@
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1" t="n">
-        <v>35.0</v>
+        <v>41.0</v>
       </c>
       <c r="P67" s="1" t="inlineStr">
         <is>
@@ -3936,14 +3942,14 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J68" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="K68" s="1" t="n">
-        <v>6125.0</v>
+        <v>5125.0</v>
       </c>
       <c r="L68" s="1" t="n">
         <v>1000.0</v>
@@ -3951,7 +3957,7 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1" t="n">
-        <v>36.0</v>
+        <v>35.0</v>
       </c>
       <c r="P68" s="1" t="inlineStr">
         <is>
@@ -3994,14 +4000,14 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J69" s="1" t="n">
-        <v>0.083333336</v>
+        <v>0.5</v>
       </c>
       <c r="K69" s="1" t="n">
-        <v>2875.0</v>
+        <v>6125.0</v>
       </c>
       <c r="L69" s="1" t="n">
         <v>1000.0</v>
@@ -4009,7 +4015,7 @@
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1" t="n">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="P69" s="1" t="inlineStr">
         <is>
@@ -4052,14 +4058,14 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J70" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.083333336</v>
       </c>
       <c r="K70" s="1" t="n">
-        <v>729.1667</v>
+        <v>2875.0</v>
       </c>
       <c r="L70" s="1" t="n">
         <v>1000.0</v>
@@ -4067,7 +4073,7 @@
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1" t="n">
-        <v>38.0</v>
+        <v>37.0</v>
       </c>
       <c r="P70" s="1" t="inlineStr">
         <is>
@@ -4104,20 +4110,20 @@
       </c>
       <c r="G71" s="1" t="inlineStr">
         <is>
-          <t>Gnagna Diop</t>
+          <t>Khady Gueye</t>
         </is>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J71" s="1" t="n">
-        <v>1.0</v>
+        <v>0.041666668</v>
       </c>
       <c r="K71" s="1" t="n">
-        <v>19500.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L71" s="1" t="n">
         <v>1000.0</v>
@@ -4125,7 +4131,7 @@
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1" t="n">
-        <v>33.0</v>
+        <v>38.0</v>
       </c>
       <c r="P71" s="1" t="inlineStr">
         <is>
@@ -4168,14 +4174,14 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J72" s="1" t="n">
         <v>1.0</v>
       </c>
       <c r="K72" s="1" t="n">
-        <v>33500.0</v>
+        <v>19500.0</v>
       </c>
       <c r="L72" s="1" t="n">
         <v>1000.0</v>
@@ -4183,7 +4189,7 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1" t="n">
-        <v>34.0</v>
+        <v>33.0</v>
       </c>
       <c r="P72" s="1" t="inlineStr">
         <is>
@@ -4220,20 +4226,20 @@
       </c>
       <c r="G73" s="1" t="inlineStr">
         <is>
-          <t>Ndeye Maréme SY</t>
+          <t>Gnagna Diop</t>
         </is>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J73" s="1" t="n">
-        <v>0.3</v>
+        <v>1.0</v>
       </c>
       <c r="K73" s="1" t="n">
-        <v>3675.0</v>
+        <v>33500.0</v>
       </c>
       <c r="L73" s="1" t="n">
         <v>1000.0</v>
@@ -4241,7 +4247,7 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1" t="n">
-        <v>31.0</v>
+        <v>34.0</v>
       </c>
       <c r="P73" s="1" t="inlineStr">
         <is>
@@ -4284,14 +4290,14 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J74" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.3</v>
       </c>
       <c r="K74" s="1" t="n">
-        <v>729.1667</v>
+        <v>3675.0</v>
       </c>
       <c r="L74" s="1" t="n">
         <v>1000.0</v>
@@ -4299,7 +4305,7 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1" t="n">
-        <v>32.0</v>
+        <v>31.0</v>
       </c>
       <c r="P74" s="1" t="inlineStr">
         <is>
@@ -4336,20 +4342,20 @@
       </c>
       <c r="G75" s="1" t="inlineStr">
         <is>
-          <t>Collé Diouf</t>
+          <t>Ndeye Maréme SY</t>
         </is>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J75" s="1" t="n">
-        <v>0.5</v>
+        <v>0.041666668</v>
       </c>
       <c r="K75" s="1" t="n">
-        <v>5125.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L75" s="1" t="n">
         <v>1000.0</v>
@@ -4357,7 +4363,7 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
       <c r="P75" s="1" t="inlineStr">
         <is>
@@ -4400,14 +4406,14 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J76" s="1" t="n">
-        <v>0.16666667</v>
+        <v>0.5</v>
       </c>
       <c r="K76" s="1" t="n">
-        <v>5750.0</v>
+        <v>5125.0</v>
       </c>
       <c r="L76" s="1" t="n">
         <v>1000.0</v>
@@ -4415,7 +4421,7 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1" t="n">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="P76" s="1" t="inlineStr">
         <is>
@@ -4458,14 +4464,14 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J77" s="1" t="n">
-        <v>1.0</v>
+        <v>0.16666667</v>
       </c>
       <c r="K77" s="1" t="n">
-        <v>12250.0</v>
+        <v>5750.0</v>
       </c>
       <c r="L77" s="1" t="n">
         <v>1000.0</v>
@@ -4473,7 +4479,7 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1" t="n">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
       <c r="P77" s="1" t="inlineStr">
         <is>
@@ -4510,20 +4516,20 @@
       </c>
       <c r="G78" s="1" t="inlineStr">
         <is>
-          <t>Aida DIOP</t>
+          <t>Collé Diouf</t>
         </is>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J78" s="1" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="K78" s="1" t="n">
-        <v>5125.0</v>
+        <v>12250.0</v>
       </c>
       <c r="L78" s="1" t="n">
         <v>1000.0</v>
@@ -4531,7 +4537,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1" t="n">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
       <c r="P78" s="1" t="inlineStr">
         <is>
@@ -4574,14 +4580,14 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J79" s="1" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K79" s="1" t="n">
-        <v>1225.0</v>
+        <v>5125.0</v>
       </c>
       <c r="L79" s="1" t="n">
         <v>1000.0</v>
@@ -4589,7 +4595,7 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1" t="n">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="P79" s="1" t="inlineStr">
         <is>
@@ -4632,14 +4638,14 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J80" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.1</v>
       </c>
       <c r="K80" s="1" t="n">
-        <v>1395.8334</v>
+        <v>1225.0</v>
       </c>
       <c r="L80" s="1" t="n">
         <v>1000.0</v>
@@ -4647,7 +4653,7 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1" t="n">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
       <c r="P80" s="1" t="inlineStr">
         <is>
@@ -4690,14 +4696,14 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J81" s="1" t="n">
         <v>0.041666668</v>
       </c>
       <c r="K81" s="1" t="n">
-        <v>729.1667</v>
+        <v>1395.8334</v>
       </c>
       <c r="L81" s="1" t="n">
         <v>1000.0</v>
@@ -4705,7 +4711,7 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1" t="n">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="P81" s="1" t="inlineStr">
         <is>
@@ -4742,20 +4748,20 @@
       </c>
       <c r="G82" s="1" t="inlineStr">
         <is>
-          <t>Baye Cheikh</t>
+          <t>Aida DIOP</t>
         </is>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J82" s="1" t="n">
-        <v>1.0</v>
+        <v>0.041666668</v>
       </c>
       <c r="K82" s="1" t="n">
-        <v>10250.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L82" s="1" t="n">
         <v>1000.0</v>
@@ -4763,7 +4769,7 @@
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1" t="n">
-        <v>20.0</v>
+        <v>27.0</v>
       </c>
       <c r="P82" s="1" t="inlineStr">
         <is>
@@ -4806,14 +4812,14 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J83" s="1" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="K83" s="1" t="n">
-        <v>9750.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L83" s="1" t="n">
         <v>1000.0</v>
@@ -4821,7 +4827,7 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1" t="n">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="P83" s="1" t="inlineStr">
         <is>
@@ -4864,14 +4870,14 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J84" s="1" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="K84" s="1" t="n">
-        <v>1225.0</v>
+        <v>9750.0</v>
       </c>
       <c r="L84" s="1" t="n">
         <v>1000.0</v>
@@ -4879,7 +4885,7 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1" t="n">
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="P84" s="1" t="inlineStr">
         <is>
@@ -4922,14 +4928,14 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J85" s="1" t="n">
-        <v>0.041666668</v>
+        <v>0.1</v>
       </c>
       <c r="K85" s="1" t="n">
-        <v>729.1667</v>
+        <v>1225.0</v>
       </c>
       <c r="L85" s="1" t="n">
         <v>1000.0</v>
@@ -4937,7 +4943,7 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1" t="n">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
       <c r="P85" s="1" t="inlineStr">
         <is>
@@ -4974,20 +4980,20 @@
       </c>
       <c r="G86" s="1" t="inlineStr">
         <is>
-          <t>Momadou BA</t>
+          <t>Baye Cheikh</t>
         </is>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J86" s="1" t="n">
-        <v>1.0</v>
+        <v>0.041666668</v>
       </c>
       <c r="K86" s="1" t="n">
-        <v>10250.0</v>
+        <v>729.1667</v>
       </c>
       <c r="L86" s="1" t="n">
         <v>1000.0</v>
@@ -4995,7 +5001,7 @@
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
       </c>
       <c r="P86" s="1" t="inlineStr">
         <is>
@@ -5038,14 +5044,14 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J87" s="1" t="n">
-        <v>1.5</v>
+        <v>1.0</v>
       </c>
       <c r="K87" s="1" t="n">
-        <v>29250.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L87" s="1" t="n">
         <v>1000.0</v>
@@ -5053,7 +5059,7 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1" t="n">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="P87" s="1" t="inlineStr">
         <is>
@@ -5096,14 +5102,14 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J88" s="1" t="n">
-        <v>1.0</v>
+        <v>1.5</v>
       </c>
       <c r="K88" s="1" t="n">
-        <v>12250.0</v>
+        <v>29250.0</v>
       </c>
       <c r="L88" s="1" t="n">
         <v>1000.0</v>
@@ -5111,7 +5117,7 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1" t="n">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="P88" s="1" t="inlineStr">
         <is>
@@ -5148,20 +5154,20 @@
       </c>
       <c r="G89" s="1" t="inlineStr">
         <is>
-          <t>Astou DIENG</t>
+          <t>Momadou BA</t>
         </is>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J89" s="1" t="n">
         <v>1.0</v>
       </c>
       <c r="K89" s="1" t="n">
-        <v>17500.0</v>
+        <v>12250.0</v>
       </c>
       <c r="L89" s="1" t="n">
         <v>1000.0</v>
@@ -5169,7 +5175,7 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="P89" s="1" t="inlineStr">
         <is>
@@ -5212,14 +5218,14 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J90" s="1" t="n">
-        <v>1.1</v>
+        <v>1.0</v>
       </c>
       <c r="K90" s="1" t="n">
-        <v>13475.0</v>
+        <v>17500.0</v>
       </c>
       <c r="L90" s="1" t="n">
         <v>1000.0</v>
@@ -5227,7 +5233,7 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1" t="n">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="P90" s="1" t="inlineStr">
         <is>
@@ -5264,20 +5270,20 @@
       </c>
       <c r="G91" s="1" t="inlineStr">
         <is>
-          <t>Fallou SOLY</t>
+          <t>Astou DIENG</t>
         </is>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J91" s="1" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="K91" s="1" t="n">
-        <v>15375.0</v>
+        <v>13475.0</v>
       </c>
       <c r="L91" s="1" t="n">
         <v>1000.0</v>
@@ -5285,7 +5291,7 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="P91" s="1" t="inlineStr">
         <is>
@@ -5328,14 +5334,14 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J92" s="1" t="n">
         <v>1.5</v>
       </c>
       <c r="K92" s="1" t="n">
-        <v>29250.0</v>
+        <v>15375.0</v>
       </c>
       <c r="L92" s="1" t="n">
         <v>1000.0</v>
@@ -5343,7 +5349,7 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="P92" s="1" t="inlineStr">
         <is>
@@ -5386,14 +5392,14 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J93" s="1" t="n">
-        <v>0.083333336</v>
+        <v>1.5</v>
       </c>
       <c r="K93" s="1" t="n">
-        <v>2875.0</v>
+        <v>29250.0</v>
       </c>
       <c r="L93" s="1" t="n">
         <v>1000.0</v>
@@ -5401,7 +5407,7 @@
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="P93" s="1" t="inlineStr">
         <is>
@@ -5428,28 +5434,38 @@
       </c>
       <c r="E94" s="1" t="inlineStr">
         <is>
-          <t>Stock Lundi</t>
-        </is>
-      </c>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
+          <t>Vente</t>
+        </is>
+      </c>
+      <c r="F94" s="1" t="inlineStr">
+        <is>
+          <t>THIAROYE</t>
+        </is>
+      </c>
+      <c r="G94" s="1" t="inlineStr">
+        <is>
+          <t>Fallou SOLY</t>
+        </is>
+      </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 50g</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J94" s="1" t="n">
-        <v>67.0</v>
+        <v>0.083333336</v>
       </c>
       <c r="K94" s="1" t="n">
-        <v>686750.0</v>
-      </c>
-      <c r="L94" s="1"/>
+        <v>2875.0</v>
+      </c>
+      <c r="L94" s="1" t="n">
+        <v>1000.0</v>
+      </c>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="P94" s="1" t="inlineStr">
         <is>
@@ -5484,20 +5500,20 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1" t="inlineStr">
         <is>
-          <t>Café pot Refraish 200g</t>
+          <t>Café pot Refraish 50g</t>
         </is>
       </c>
       <c r="J95" s="1" t="n">
-        <v>38.0</v>
+        <v>67.0</v>
       </c>
       <c r="K95" s="1" t="n">
-        <v>741000.0</v>
+        <v>686750.0</v>
       </c>
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="P95" s="1" t="inlineStr">
         <is>
@@ -5532,20 +5548,20 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Café pot Refraish 200g</t>
         </is>
       </c>
       <c r="J96" s="1" t="n">
-        <v>27.708334</v>
+        <v>38.0</v>
       </c>
       <c r="K96" s="1" t="n">
-        <v>484895.84</v>
+        <v>741000.0</v>
       </c>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="P96" s="1" t="inlineStr">
         <is>
@@ -5580,20 +5596,20 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J97" s="1" t="n">
-        <v>10.833333</v>
+        <v>27.708334</v>
       </c>
       <c r="K97" s="1" t="n">
-        <v>362916.66</v>
+        <v>484895.84</v>
       </c>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="P97" s="1" t="inlineStr">
         <is>
@@ -5628,20 +5644,20 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J98" s="1" t="n">
-        <v>38.0</v>
+        <v>10.833333</v>
       </c>
       <c r="K98" s="1" t="n">
-        <v>1311000.0</v>
+        <v>362916.66</v>
       </c>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="P98" s="1" t="inlineStr">
         <is>
@@ -5676,20 +5692,20 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1" t="inlineStr">
         <is>
-          <t>KamLac Lait concentré sucré 24x1kg</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J99" s="1" t="n">
-        <v>31.291666</v>
+        <v>38.0</v>
       </c>
       <c r="K99" s="1" t="n">
-        <v>891812.5</v>
+        <v>1311000.0</v>
       </c>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="P99" s="1" t="inlineStr">
         <is>
@@ -5724,20 +5740,20 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 18gx100</t>
+          <t>KamLac Lait concentré sucré 24x1kg</t>
         </is>
       </c>
       <c r="J100" s="1" t="n">
-        <v>34.4</v>
+        <v>31.291666</v>
       </c>
       <c r="K100" s="1" t="n">
-        <v>223600.0</v>
+        <v>891812.5</v>
       </c>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="P100" s="1" t="inlineStr">
         <is>
@@ -5772,20 +5788,20 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1" t="inlineStr">
         <is>
-          <t>Lait Kamlac sachet 18gx100</t>
+          <t>Lait Janus 18gx100</t>
         </is>
       </c>
       <c r="J101" s="1" t="n">
-        <v>20.6</v>
+        <v>34.4</v>
       </c>
       <c r="K101" s="1" t="n">
-        <v>154500.0</v>
+        <v>223600.0</v>
       </c>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="P101" s="1" t="inlineStr">
         <is>
@@ -5820,20 +5836,20 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Lait Kamlac sachet 18gx100</t>
         </is>
       </c>
       <c r="J102" s="1" t="n">
-        <v>43.1</v>
+        <v>20.6</v>
       </c>
       <c r="K102" s="1" t="n">
-        <v>527975.0</v>
+        <v>154500.0</v>
       </c>
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="P102" s="1" t="inlineStr">
         <is>
@@ -5868,20 +5884,20 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 20gx100</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J103" s="1" t="n">
-        <v>13.1</v>
+        <v>43.1</v>
       </c>
       <c r="K103" s="1" t="n">
-        <v>85150.0</v>
+        <v>527975.0</v>
       </c>
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="P103" s="1" t="inlineStr">
         <is>
@@ -5916,22 +5932,70 @@
       <c r="H104" s="1"/>
       <c r="I104" s="1" t="inlineStr">
         <is>
-          <t>Jus Lido</t>
+          <t>Lait Janus 20gx100</t>
         </is>
       </c>
       <c r="J104" s="1" t="n">
-        <v>44.166668</v>
+        <v>13.1</v>
       </c>
       <c r="K104" s="1" t="n">
-        <v>530000.0</v>
+        <v>85150.0</v>
       </c>
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="P104" s="1" t="inlineStr">
+        <is>
+          <t>S39</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>45922.0</v>
+      </c>
+      <c r="B105" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C105" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D105" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E105" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1" t="inlineStr">
+        <is>
+          <t>Jus Lido</t>
+        </is>
+      </c>
+      <c r="J105" s="1" t="n">
+        <v>44.166668</v>
+      </c>
+      <c r="K105" s="1" t="n">
+        <v>530000.0</v>
+      </c>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1" t="n">
         <v>11.0</v>
       </c>
-      <c r="P104" s="1" t="inlineStr">
+      <c r="P105" s="1" t="inlineStr">
         <is>
           <t>S39</t>
         </is>

</xml_diff>

<commit_message>
Rapport du 23 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D69765-C199-4D9C-A63B-118AF1D9CF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850EF810-8DDD-43CF-9E90-E6F1F5F8F600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Jus Lido</t>
-  </si>
-  <si>
-    <t>TATA 1</t>
   </si>
   <si>
     <t>DJIBRIL DIOP</t>
@@ -648,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67:C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1110,16 +1107,16 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
@@ -1154,20 +1151,20 @@
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J13" s="1">
         <v>0.1</v>
@@ -1198,16 +1195,16 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
@@ -1242,16 +1239,16 @@
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
@@ -1286,16 +1283,16 @@
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
@@ -1330,16 +1327,16 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1" t="s">
@@ -1374,22 +1371,22 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J18" s="1">
         <v>0.8</v>
@@ -1420,19 +1417,19 @@
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>19</v>
@@ -1466,19 +1463,19 @@
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>21</v>
@@ -1512,19 +1509,19 @@
         <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>23</v>
@@ -1558,19 +1555,19 @@
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>25</v>
@@ -1604,16 +1601,16 @@
         <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
@@ -1648,16 +1645,16 @@
         <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
@@ -1692,16 +1689,16 @@
         <v>16</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
@@ -1736,16 +1733,16 @@
         <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
@@ -1780,20 +1777,20 @@
         <v>16</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" s="1">
         <v>0.1</v>
@@ -1824,16 +1821,16 @@
         <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
@@ -1868,16 +1865,16 @@
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G29" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
@@ -1912,20 +1909,20 @@
         <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J30" s="1">
         <v>0.3</v>
@@ -1956,16 +1953,16 @@
         <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
@@ -2000,16 +1997,16 @@
         <v>16</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
@@ -2044,16 +2041,16 @@
         <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
@@ -2088,16 +2085,16 @@
         <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
@@ -2132,16 +2129,16 @@
         <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
@@ -2176,16 +2173,16 @@
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
@@ -2220,20 +2217,20 @@
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J37" s="1">
         <v>0.5</v>
@@ -2264,16 +2261,16 @@
         <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
@@ -2308,16 +2305,16 @@
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
@@ -2352,16 +2349,16 @@
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
@@ -2396,16 +2393,16 @@
         <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
@@ -2440,16 +2437,16 @@
         <v>16</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1" t="s">
@@ -2487,13 +2484,13 @@
         <v>17</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
@@ -2531,13 +2528,13 @@
         <v>17</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
@@ -2575,13 +2572,13 @@
         <v>17</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1" t="s">
@@ -2619,13 +2616,13 @@
         <v>17</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1" t="s">
@@ -2663,17 +2660,17 @@
         <v>17</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J47" s="1">
         <v>0.2</v>
@@ -2707,13 +2704,13 @@
         <v>17</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1" t="s">
@@ -2751,13 +2748,13 @@
         <v>17</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G49" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
@@ -2795,13 +2792,13 @@
         <v>17</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
@@ -2839,13 +2836,13 @@
         <v>17</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
@@ -2883,13 +2880,13 @@
         <v>17</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
@@ -2927,17 +2924,17 @@
         <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J53" s="1">
         <v>0.4</v>
@@ -2971,13 +2968,13 @@
         <v>17</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G54" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1" t="s">
@@ -3015,13 +3012,13 @@
         <v>17</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="s">
@@ -3059,13 +3056,13 @@
         <v>17</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
@@ -3103,13 +3100,13 @@
         <v>17</v>
       </c>
       <c r="E57" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G57" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1" t="s">
@@ -3147,13 +3144,13 @@
         <v>17</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
@@ -3191,17 +3188,17 @@
         <v>17</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G59" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J59" s="1">
         <v>0.2</v>
@@ -3235,17 +3232,17 @@
         <v>17</v>
       </c>
       <c r="E60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G60" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J60" s="1">
         <v>0.3</v>
@@ -3279,13 +3276,13 @@
         <v>17</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G61" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1" t="s">
@@ -3323,13 +3320,13 @@
         <v>17</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G62" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
@@ -3367,13 +3364,13 @@
         <v>17</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G63" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -3403,13 +3400,13 @@
         <v>17</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G64" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1" t="s">
@@ -3447,17 +3444,17 @@
         <v>17</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G65" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J65" s="1">
         <v>0.1</v>
@@ -3491,13 +3488,13 @@
         <v>17</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G66" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
@@ -3535,13 +3532,13 @@
         <v>17</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G67" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
@@ -3579,16 +3576,16 @@
         <v>17</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F68" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>21</v>
@@ -3617,22 +3614,22 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E69" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>21</v>
@@ -3663,22 +3660,22 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E70" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>19</v>
@@ -3709,25 +3706,25 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E71" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J71" s="1">
         <v>1</v>
@@ -3755,23 +3752,23 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E72" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J72" s="1">
         <v>1</v>
@@ -3799,23 +3796,23 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J73" s="1">
         <v>0.3</v>
@@ -3843,19 +3840,19 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E74" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1" t="s">
@@ -3887,19 +3884,19 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E75" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1" t="s">
@@ -3931,19 +3928,19 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E76" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1" t="s">
@@ -3975,19 +3972,19 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E77" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="s">
@@ -4019,23 +4016,23 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E78" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J78" s="1">
         <v>0.4</v>
@@ -4063,19 +4060,19 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E79" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="s">
@@ -4107,23 +4104,23 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E80" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J80" s="1">
         <v>0.2</v>
@@ -4151,19 +4148,19 @@
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E81" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
@@ -4195,19 +4192,19 @@
         <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E82" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
@@ -4239,23 +4236,23 @@
         <v>0</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E83" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J83" s="1">
         <v>0.2</v>
@@ -4283,19 +4280,19 @@
         <v>0</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E84" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1" t="s">
@@ -4327,23 +4324,23 @@
         <v>0</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E85" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J85" s="1">
         <v>0.3</v>
@@ -4371,19 +4368,19 @@
         <v>0</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E86" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1" t="s">
@@ -4415,19 +4412,19 @@
         <v>0</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E87" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1" t="s">
@@ -4459,23 +4456,23 @@
         <v>0</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E88" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J88" s="1">
         <v>1</v>
@@ -4503,19 +4500,19 @@
         <v>0</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E89" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1" t="s">
@@ -4547,19 +4544,19 @@
         <v>0</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E90" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1" t="s">
@@ -4591,19 +4588,19 @@
         <v>0</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E91" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1" t="s">
@@ -4635,19 +4632,19 @@
         <v>0</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E92" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1" t="s">
@@ -4679,19 +4676,19 @@
         <v>0</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E93" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1" t="s">
@@ -4723,19 +4720,19 @@
         <v>0</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E94" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1" t="s">
@@ -4767,23 +4764,23 @@
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E95" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J95" s="1">
         <v>0.5</v>
@@ -4811,19 +4808,19 @@
         <v>0</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E96" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1" t="s">
@@ -4855,23 +4852,23 @@
         <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E97" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J97" s="1">
         <v>1.6</v>
@@ -4899,19 +4896,19 @@
         <v>0</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D98" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="s">
@@ -4943,19 +4940,19 @@
         <v>0</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E99" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1" t="s">
@@ -4987,19 +4984,19 @@
         <v>0</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E100" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1" t="s">
@@ -5031,19 +5028,19 @@
         <v>0</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E101" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1" t="s">
@@ -5075,19 +5072,19 @@
         <v>0</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E102" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1" t="s">
@@ -5119,23 +5116,23 @@
         <v>0</v>
       </c>
       <c r="C103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E103" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H103" s="1"/>
       <c r="I103" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J103" s="1">
         <v>0.6</v>
@@ -5163,19 +5160,19 @@
         <v>0</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E104" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H104" s="1"/>
       <c r="I104" s="1" t="s">
@@ -5207,19 +5204,19 @@
         <v>0</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E105" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H105" s="1"/>
       <c r="I105" s="1" t="s">
@@ -5251,19 +5248,19 @@
         <v>0</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E106" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H106" s="1"/>
       <c r="I106" s="1" t="s">
@@ -5295,19 +5292,19 @@
         <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E107" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1" t="s">
@@ -5339,23 +5336,23 @@
         <v>0</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E108" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J108" s="1">
         <v>0.1</v>
@@ -5699,7 +5696,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
       <c r="I117" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J117" s="1">
         <v>29.3</v>
@@ -5807,17 +5804,17 @@
         <v>17</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J120" s="1">
         <v>1.1000000000000001</v>
@@ -5853,13 +5850,13 @@
         <v>17</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H121" s="1"/>
       <c r="I121" s="1" t="s">
@@ -5899,13 +5896,13 @@
         <v>17</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H122" s="1"/>
       <c r="I122" s="1" t="s">
@@ -5945,17 +5942,17 @@
         <v>17</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H123" s="1"/>
       <c r="I123" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J123" s="1">
         <v>0.1</v>
@@ -5991,13 +5988,13 @@
         <v>17</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H124" s="1"/>
       <c r="I124" s="1" t="s">
@@ -6037,13 +6034,13 @@
         <v>17</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H125" s="1"/>
       <c r="I125" s="1" t="s">
@@ -6083,13 +6080,13 @@
         <v>17</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H126" s="1"/>
       <c r="I126" s="1" t="s">
@@ -6129,13 +6126,13 @@
         <v>17</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H127" s="1"/>
       <c r="I127" s="1" t="s">
@@ -6175,13 +6172,13 @@
         <v>17</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H128" s="1"/>
       <c r="I128" s="1" t="s">
@@ -6221,17 +6218,17 @@
         <v>17</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J129" s="1">
         <v>0.1</v>
@@ -6267,13 +6264,13 @@
         <v>17</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H130" s="1"/>
       <c r="I130" s="1" t="s">
@@ -6313,13 +6310,13 @@
         <v>17</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H131" s="1"/>
       <c r="I131" s="1" t="s">
@@ -6359,17 +6356,17 @@
         <v>17</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H132" s="1"/>
       <c r="I132" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J132" s="1">
         <v>0.5</v>
@@ -6405,13 +6402,13 @@
         <v>17</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H133" s="1"/>
       <c r="I133" s="1" t="s">
@@ -6451,13 +6448,13 @@
         <v>17</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H134" s="1"/>
       <c r="I134" s="1" t="s">
@@ -6497,17 +6494,17 @@
         <v>17</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H135" s="1"/>
       <c r="I135" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J135" s="1">
         <v>0.5</v>
@@ -6543,13 +6540,13 @@
         <v>17</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H136" s="1"/>
       <c r="I136" s="1" t="s">
@@ -6589,13 +6586,13 @@
         <v>17</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H137" s="1"/>
       <c r="I137" s="1" t="s">
@@ -6635,13 +6632,13 @@
         <v>17</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H138" s="1"/>
       <c r="I138" s="1" t="s">
@@ -6681,13 +6678,13 @@
         <v>17</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="1" t="s">
@@ -6727,17 +6724,17 @@
         <v>17</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H140" s="1"/>
       <c r="I140" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J140" s="1">
         <v>0.3</v>
@@ -6773,13 +6770,13 @@
         <v>17</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H141" s="1"/>
       <c r="I141" s="1" t="s">
@@ -6819,13 +6816,13 @@
         <v>17</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H142" s="1"/>
       <c r="I142" s="1" t="s">
@@ -6865,13 +6862,13 @@
         <v>17</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H143" s="1"/>
       <c r="I143" s="1" t="s">
@@ -6911,17 +6908,17 @@
         <v>17</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H144" s="1"/>
       <c r="I144" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J144" s="1">
         <v>1</v>
@@ -6957,13 +6954,13 @@
         <v>17</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H145" s="1"/>
       <c r="I145" s="1" t="s">
@@ -7003,17 +7000,17 @@
         <v>17</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H146" s="1"/>
       <c r="I146" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J146" s="1">
         <v>0.1</v>
@@ -7049,13 +7046,13 @@
         <v>17</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H147" s="1"/>
       <c r="I147" s="1" t="s">
@@ -7095,13 +7092,13 @@
         <v>17</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H148" s="1"/>
       <c r="I148" s="1" t="s">
@@ -7141,13 +7138,13 @@
         <v>17</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H149" s="1"/>
       <c r="I149" s="1" t="s">
@@ -7187,13 +7184,13 @@
         <v>17</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H150" s="1"/>
       <c r="I150" s="1" t="s">
@@ -7233,17 +7230,17 @@
         <v>17</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H151" s="1"/>
       <c r="I151" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J151" s="1">
         <v>0.8</v>
@@ -7279,13 +7276,13 @@
         <v>17</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H152" s="1"/>
       <c r="I152" s="1" t="s">
@@ -7325,13 +7322,13 @@
         <v>17</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H153" s="1"/>
       <c r="I153" s="1" t="s">
@@ -7371,13 +7368,13 @@
         <v>17</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H154" s="1"/>
       <c r="I154" s="1" t="s">
@@ -7417,17 +7414,17 @@
         <v>17</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H155" s="1"/>
       <c r="I155" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J155" s="1">
         <v>1</v>
@@ -7463,13 +7460,13 @@
         <v>17</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H156" s="1"/>
       <c r="I156" s="1" t="s">
@@ -7509,17 +7506,17 @@
         <v>17</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H157" s="1"/>
       <c r="I157" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J157" s="1">
         <v>1.1000000000000001</v>
@@ -7555,13 +7552,13 @@
         <v>17</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H158" s="1"/>
       <c r="I158" s="1" t="s">
@@ -7601,13 +7598,13 @@
         <v>17</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H159" s="1"/>
       <c r="I159" s="1" t="s">
@@ -7647,13 +7644,13 @@
         <v>17</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H160" s="1"/>
       <c r="I160" s="1" t="s">
@@ -7693,7 +7690,7 @@
         <v>17</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
@@ -7731,7 +7728,7 @@
         <v>17</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
@@ -7769,7 +7766,7 @@
         <v>17</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
@@ -7807,7 +7804,7 @@
         <v>17</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
@@ -7845,7 +7842,7 @@
         <v>17</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
@@ -7883,7 +7880,7 @@
         <v>17</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
@@ -7921,7 +7918,7 @@
         <v>17</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
@@ -7959,7 +7956,7 @@
         <v>17</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
@@ -7997,13 +7994,13 @@
         <v>17</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
       <c r="I169" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J169" s="1">
         <v>43.1</v>
@@ -8035,7 +8032,7 @@
         <v>17</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
@@ -8073,7 +8070,7 @@
         <v>17</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
@@ -8111,17 +8108,17 @@
         <v>17</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F172" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G172" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G172" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H172" s="1"/>
       <c r="I172" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J172" s="1">
         <v>1.3</v>
@@ -8138,7 +8135,7 @@
         <v>154</v>
       </c>
       <c r="P172" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.45">
@@ -8155,13 +8152,13 @@
         <v>17</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F173" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G173" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G173" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H173" s="1"/>
       <c r="I173" s="1" t="s">
@@ -8182,7 +8179,7 @@
         <v>155</v>
       </c>
       <c r="P173" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.45">
@@ -8199,13 +8196,13 @@
         <v>17</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F174" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G174" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H174" s="1"/>
       <c r="I174" s="1" t="s">
@@ -8226,7 +8223,7 @@
         <v>156</v>
       </c>
       <c r="P174" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.45">
@@ -8243,13 +8240,13 @@
         <v>17</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H175" s="1"/>
       <c r="I175" s="1" t="s">
@@ -8270,7 +8267,7 @@
         <v>151</v>
       </c>
       <c r="P175" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.45">
@@ -8287,17 +8284,17 @@
         <v>17</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H176" s="1"/>
       <c r="I176" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J176" s="1">
         <v>0.2</v>
@@ -8314,7 +8311,7 @@
         <v>152</v>
       </c>
       <c r="P176" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.45">
@@ -8331,13 +8328,13 @@
         <v>17</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H177" s="1"/>
       <c r="I177" s="1" t="s">
@@ -8358,7 +8355,7 @@
         <v>153</v>
       </c>
       <c r="P177" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.45">
@@ -8375,13 +8372,13 @@
         <v>17</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H178" s="1"/>
       <c r="I178" s="1" t="s">
@@ -8402,7 +8399,7 @@
         <v>149</v>
       </c>
       <c r="P178" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.45">
@@ -8419,13 +8416,13 @@
         <v>17</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H179" s="1"/>
       <c r="I179" s="1" t="s">
@@ -8446,7 +8443,7 @@
         <v>150</v>
       </c>
       <c r="P179" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.45">
@@ -8463,13 +8460,13 @@
         <v>17</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H180" s="1"/>
       <c r="I180" s="1" t="s">
@@ -8490,7 +8487,7 @@
         <v>145</v>
       </c>
       <c r="P180" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.45">
@@ -8507,13 +8504,13 @@
         <v>17</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H181" s="1"/>
       <c r="I181" s="1" t="s">
@@ -8534,7 +8531,7 @@
         <v>146</v>
       </c>
       <c r="P181" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.45">
@@ -8551,17 +8548,17 @@
         <v>17</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H182" s="1"/>
       <c r="I182" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J182" s="1">
         <v>0.5</v>
@@ -8578,7 +8575,7 @@
         <v>147</v>
       </c>
       <c r="P182" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.45">
@@ -8595,13 +8592,13 @@
         <v>17</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H183" s="1"/>
       <c r="I183" s="1" t="s">
@@ -8622,7 +8619,7 @@
         <v>148</v>
       </c>
       <c r="P183" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.45">
@@ -8639,13 +8636,13 @@
         <v>17</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H184" s="1"/>
       <c r="I184" s="1" t="s">
@@ -8666,7 +8663,7 @@
         <v>143</v>
       </c>
       <c r="P184" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.45">
@@ -8683,17 +8680,17 @@
         <v>17</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H185" s="1"/>
       <c r="I185" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J185" s="1">
         <v>0.3</v>
@@ -8710,7 +8707,7 @@
         <v>144</v>
       </c>
       <c r="P185" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.45">
@@ -8727,13 +8724,13 @@
         <v>17</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H186" s="1"/>
       <c r="I186" s="1" t="s">
@@ -8754,7 +8751,7 @@
         <v>140</v>
       </c>
       <c r="P186" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.45">
@@ -8771,13 +8768,13 @@
         <v>17</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H187" s="1"/>
       <c r="I187" s="1" t="s">
@@ -8798,7 +8795,7 @@
         <v>141</v>
       </c>
       <c r="P187" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.45">
@@ -8815,13 +8812,13 @@
         <v>17</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H188" s="1"/>
       <c r="I188" s="1" t="s">
@@ -8842,7 +8839,7 @@
         <v>142</v>
       </c>
       <c r="P188" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.45">
@@ -8859,13 +8856,13 @@
         <v>17</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H189" s="1"/>
       <c r="I189" s="1" t="s">
@@ -8886,7 +8883,7 @@
         <v>136</v>
       </c>
       <c r="P189" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.45">
@@ -8903,17 +8900,17 @@
         <v>17</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H190" s="1"/>
       <c r="I190" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J190" s="1">
         <v>0.1</v>
@@ -8930,7 +8927,7 @@
         <v>137</v>
       </c>
       <c r="P190" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.45">
@@ -8947,13 +8944,13 @@
         <v>17</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H191" s="1"/>
       <c r="I191" s="1" t="s">
@@ -8974,7 +8971,7 @@
         <v>138</v>
       </c>
       <c r="P191" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.45">
@@ -8991,13 +8988,13 @@
         <v>17</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H192" s="1"/>
       <c r="I192" s="1" t="s">
@@ -9018,7 +9015,7 @@
         <v>139</v>
       </c>
       <c r="P192" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.45">
@@ -9035,13 +9032,13 @@
         <v>17</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H193" s="1"/>
       <c r="I193" s="1" t="s">
@@ -9062,7 +9059,7 @@
         <v>133</v>
       </c>
       <c r="P193" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.45">
@@ -9079,17 +9076,17 @@
         <v>17</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H194" s="1"/>
       <c r="I194" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J194" s="1">
         <v>0.3</v>
@@ -9106,7 +9103,7 @@
         <v>134</v>
       </c>
       <c r="P194" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.45">
@@ -9123,13 +9120,13 @@
         <v>17</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H195" s="1"/>
       <c r="I195" s="1" t="s">
@@ -9150,7 +9147,7 @@
         <v>135</v>
       </c>
       <c r="P195" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.45">
@@ -9167,13 +9164,13 @@
         <v>17</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H196" s="1"/>
       <c r="I196" s="1" t="s">
@@ -9194,7 +9191,7 @@
         <v>132</v>
       </c>
       <c r="P196" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.45">
@@ -9211,13 +9208,13 @@
         <v>17</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H197" s="1"/>
       <c r="I197" s="1" t="s">
@@ -9238,7 +9235,7 @@
         <v>129</v>
       </c>
       <c r="P197" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.45">
@@ -9255,13 +9252,13 @@
         <v>17</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H198" s="1"/>
       <c r="I198" s="1" t="s">
@@ -9282,7 +9279,7 @@
         <v>130</v>
       </c>
       <c r="P198" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.45">
@@ -9299,13 +9296,13 @@
         <v>17</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H199" s="1"/>
       <c r="I199" s="1" t="s">
@@ -9326,7 +9323,7 @@
         <v>131</v>
       </c>
       <c r="P199" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rpport du 24 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -5426,10 +5426,10 @@
         </is>
       </c>
       <c r="J93" s="1" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="K93" s="1" t="n">
-        <v>214500.0</v>
+        <v>195000.0</v>
       </c>
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
@@ -5618,10 +5618,10 @@
         </is>
       </c>
       <c r="J97" s="1" t="n">
-        <v>20.0</v>
+        <v>19.9</v>
       </c>
       <c r="K97" s="1" t="n">
-        <v>130000.0</v>
+        <v>129350.0</v>
       </c>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>

</xml_diff>

<commit_message>
Rapport du 25 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -12674,10 +12674,10 @@
         </is>
       </c>
       <c r="J221" s="1" t="n">
-        <v>15.0</v>
+        <v>40.0</v>
       </c>
       <c r="K221" s="1" t="n">
-        <v>292500.0</v>
+        <v>780000.0</v>
       </c>
       <c r="L221" s="1"/>
       <c r="M221" s="1"/>
@@ -22368,10 +22368,10 @@
         </is>
       </c>
       <c r="J392" s="1" t="n">
-        <v>48.0</v>
+        <v>73.0</v>
       </c>
       <c r="K392" s="1" t="n">
-        <v>936000.0</v>
+        <v>1423500.0</v>
       </c>
       <c r="L392" s="1"/>
       <c r="M392" s="1"/>

</xml_diff>

<commit_message>
Rapport du 27 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34747576-B2F5-4766-BA56-287D90D39492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3B62C9-9648-418D-A4F0-B8DE653BAC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P563"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Rapport du 29 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -3622,10 +3622,10 @@
         </is>
       </c>
       <c r="J67" s="1" t="n">
-        <v>9.375</v>
+        <v>7.375</v>
       </c>
       <c r="K67" s="1" t="n">
-        <v>314062.5</v>
+        <v>247062.5</v>
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
@@ -3766,10 +3766,10 @@
         </is>
       </c>
       <c r="J70" s="1" t="n">
-        <v>37.3</v>
+        <v>31.3</v>
       </c>
       <c r="K70" s="1" t="n">
-        <v>242450.0</v>
+        <v>203450.0</v>
       </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>

</xml_diff>

<commit_message>
Rapport du 01 Aout 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -15153,10 +15153,10 @@
         </is>
       </c>
       <c r="J266" s="1" t="n">
-        <v>26.7</v>
+        <v>24.7</v>
       </c>
       <c r="K266" s="1" t="n">
-        <v>173550.0</v>
+        <v>160550.0</v>
       </c>
       <c r="L266" s="1"/>
       <c r="M266" s="1"/>
@@ -15249,10 +15249,10 @@
         </is>
       </c>
       <c r="J268" s="1" t="n">
-        <v>40.8</v>
+        <v>33.8</v>
       </c>
       <c r="K268" s="1" t="n">
-        <v>499800.0</v>
+        <v>414050.0</v>
       </c>
       <c r="L268" s="1"/>
       <c r="M268" s="1"/>
@@ -15729,10 +15729,10 @@
         </is>
       </c>
       <c r="J278" s="1" t="n">
-        <v>29.0</v>
+        <v>36.0</v>
       </c>
       <c r="K278" s="1" t="n">
-        <v>355250.0</v>
+        <v>441000.0</v>
       </c>
       <c r="L278" s="1"/>
       <c r="M278" s="1"/>
@@ -15777,10 +15777,10 @@
         </is>
       </c>
       <c r="J279" s="1" t="n">
-        <v>34.1</v>
+        <v>36.1</v>
       </c>
       <c r="K279" s="1" t="n">
-        <v>221650.0</v>
+        <v>234650.0</v>
       </c>
       <c r="L279" s="1"/>
       <c r="M279" s="1"/>

</xml_diff>

<commit_message>
Rapport du 02 Aout 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -3693,10 +3693,10 @@
         </is>
       </c>
       <c r="J62" s="1" t="n">
-        <v>20.833334</v>
+        <v>20.791666</v>
       </c>
       <c r="K62" s="1" t="n">
-        <v>593750.0</v>
+        <v>592562.5</v>
       </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -3885,10 +3885,10 @@
         </is>
       </c>
       <c r="J66" s="1" t="n">
-        <v>10.0</v>
+        <v>9.8</v>
       </c>
       <c r="K66" s="1" t="n">
-        <v>65000.0</v>
+        <v>63700.0</v>
       </c>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -3933,10 +3933,10 @@
         </is>
       </c>
       <c r="J67" s="1" t="n">
-        <v>17.375</v>
+        <v>17.333334</v>
       </c>
       <c r="K67" s="1" t="n">
-        <v>304062.5</v>
+        <v>303333.34</v>
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
@@ -3981,10 +3981,10 @@
         </is>
       </c>
       <c r="J68" s="1" t="n">
-        <v>3.0</v>
+        <v>2.9583333</v>
       </c>
       <c r="K68" s="1" t="n">
-        <v>100500.0</v>
+        <v>99104.164</v>
       </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>

</xml_diff>

<commit_message>
Rapport du 04 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -1207,10 +1207,10 @@
         </is>
       </c>
       <c r="J23" s="1" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>37500.0</v>
+        <v>25000.0</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="J25" s="1" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="K25" s="1" t="n">
-        <v>31000.0</v>
+        <v>46500.0</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>

</xml_diff>

<commit_message>
Rapport du 08 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E830B26-F65B-449D-A417-B20B59506CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D231A05-3F5F-4354-9BA9-EB48F4CA6150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7550" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7547" uniqueCount="101">
   <si>
     <t>Date</t>
   </si>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F385" workbookViewId="0">
-      <selection activeCell="L396" sqref="L396:L425"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -1814,10 +1814,7 @@
         <v>19</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>32</v>
@@ -1846,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
@@ -1858,10 +1855,7 @@
         <v>19</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>33</v>
@@ -1890,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
@@ -1902,10 +1896,7 @@
         <v>19</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Rapport du 09 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -4615,10 +4615,10 @@
         </is>
       </c>
       <c r="J78" s="1" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K78" s="1" t="n">
-        <v>1300.0</v>
+        <v>3250.0</v>
       </c>
       <c r="L78" s="1" t="n">
         <v>2000.0</v>
@@ -8349,10 +8349,10 @@
         </is>
       </c>
       <c r="J146" s="1" t="n">
-        <v>14.6</v>
+        <v>22.6</v>
       </c>
       <c r="K146" s="1" t="n">
-        <v>94900.0</v>
+        <v>146900.0</v>
       </c>
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
@@ -8393,14 +8393,14 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 18gx100</t>
+          <t>Café Altimo pot 50g x 24 pcs</t>
         </is>
       </c>
       <c r="J147" s="1" t="n">
-        <v>22.6</v>
+        <v>14.875</v>
       </c>
       <c r="K147" s="1" t="n">
-        <v>146900.0</v>
+        <v>260312.5</v>
       </c>
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
@@ -8441,14 +8441,14 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 50g x 24 pcs</t>
+          <t>Café Altimo pot 100g x 24 pcs</t>
         </is>
       </c>
       <c r="J148" s="1" t="n">
-        <v>14.875</v>
+        <v>8.0</v>
       </c>
       <c r="K148" s="1" t="n">
-        <v>260312.5</v>
+        <v>268000.0</v>
       </c>
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
@@ -8489,14 +8489,14 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 100g x 24 pcs</t>
+          <t>Café Altimo pot 200g x 12 pcs</t>
         </is>
       </c>
       <c r="J149" s="1" t="n">
-        <v>8.0</v>
+        <v>8.083333</v>
       </c>
       <c r="K149" s="1" t="n">
-        <v>268000.0</v>
+        <v>278875.0</v>
       </c>
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
@@ -8537,14 +8537,14 @@
       <c r="H150" s="1"/>
       <c r="I150" s="1" t="inlineStr">
         <is>
-          <t>Café Altimo pot 200g x 12 pcs</t>
+          <t>Kamlac évaporé 48x160g</t>
         </is>
       </c>
       <c r="J150" s="1" t="n">
-        <v>8.083333</v>
+        <v>6.0</v>
       </c>
       <c r="K150" s="1" t="n">
-        <v>278875.0</v>
+        <v>69000.0</v>
       </c>
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
@@ -8585,14 +8585,14 @@
       <c r="H151" s="1"/>
       <c r="I151" s="1" t="inlineStr">
         <is>
-          <t>Kamlac évaporé 48x160g</t>
+          <t>Lait Janus 400gx10</t>
         </is>
       </c>
       <c r="J151" s="1" t="n">
-        <v>6.0</v>
+        <v>13.7</v>
       </c>
       <c r="K151" s="1" t="n">
-        <v>69000.0</v>
+        <v>167825.0</v>
       </c>
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
@@ -8633,14 +8633,14 @@
       <c r="H152" s="1"/>
       <c r="I152" s="1" t="inlineStr">
         <is>
-          <t>Lait Janus 400gx10</t>
+          <t>Jus Lido</t>
         </is>
       </c>
       <c r="J152" s="1" t="n">
-        <v>13.7</v>
+        <v>2.3333333</v>
       </c>
       <c r="K152" s="1" t="n">
-        <v>167825.0</v>
+        <v>28000.0</v>
       </c>
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
@@ -8681,14 +8681,14 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1" t="inlineStr">
         <is>
-          <t>Jus Lido</t>
+          <t>Chocolat 3-en-1 30x120 pcs</t>
         </is>
       </c>
       <c r="J153" s="1" t="n">
-        <v>2.3333333</v>
+        <v>5.0</v>
       </c>
       <c r="K153" s="1" t="n">
-        <v>28000.0</v>
+        <v>65000.0</v>
       </c>
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
@@ -8729,14 +8729,14 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1" t="inlineStr">
         <is>
-          <t>Chocolat 3-en-1 30x120 pcs</t>
+          <t>Chocolat transparent 200gx24pcs</t>
         </is>
       </c>
       <c r="J154" s="1" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="K154" s="1" t="n">
-        <v>65000.0</v>
+        <v>50000.0</v>
       </c>
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
@@ -8777,14 +8777,14 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1" t="inlineStr">
         <is>
-          <t>Chocolat transparent 200gx24pcs</t>
+          <t>Chocolat transparent 400gx24pcs</t>
         </is>
       </c>
       <c r="J155" s="1" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="K155" s="1" t="n">
-        <v>50000.0</v>
+        <v>62500.0</v>
       </c>
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
@@ -8825,14 +8825,14 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1" t="inlineStr">
         <is>
-          <t>Chocolat transparent 400gx24pcs</t>
+          <t>Chocolat jaune 200g x 24 pcs</t>
         </is>
       </c>
       <c r="J156" s="1" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="K156" s="1" t="n">
-        <v>62500.0</v>
+        <v>62000.0</v>
       </c>
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
@@ -8873,14 +8873,14 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1" t="inlineStr">
         <is>
-          <t>Chocolat jaune 200g x 24 pcs</t>
+          <t>Chocolat jaune 400g x 24 pcs</t>
         </is>
       </c>
       <c r="J157" s="1" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="K157" s="1" t="n">
-        <v>62000.0</v>
+        <v>77500.0</v>
       </c>
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
@@ -8921,14 +8921,14 @@
       <c r="H158" s="1"/>
       <c r="I158" s="1" t="inlineStr">
         <is>
-          <t>Chocolat jaune 400g x 24 pcs</t>
+          <t>Chocolat Jaune 10gx60pcsx6 boites</t>
         </is>
       </c>
       <c r="J158" s="1" t="n">
         <v>5.0</v>
       </c>
       <c r="K158" s="1" t="n">
-        <v>77500.0</v>
+        <v>50000.0</v>
       </c>
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
@@ -8969,14 +8969,14 @@
       <c r="H159" s="1"/>
       <c r="I159" s="1" t="inlineStr">
         <is>
-          <t>Chocolat Jaune 10gx60pcsx6 boites</t>
+          <t>Chocolat Orange 200g x24 pcs</t>
         </is>
       </c>
       <c r="J159" s="1" t="n">
         <v>5.0</v>
       </c>
       <c r="K159" s="1" t="n">
-        <v>50000.0</v>
+        <v>105000.0</v>
       </c>
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
@@ -9017,7 +9017,7 @@
       <c r="H160" s="1"/>
       <c r="I160" s="1" t="inlineStr">
         <is>
-          <t>Chocolat Orange 200g x24 pcs</t>
+          <t>Chocolat Orange 400g x24 pcs</t>
         </is>
       </c>
       <c r="J160" s="1" t="n">
@@ -9065,14 +9065,14 @@
       <c r="H161" s="1"/>
       <c r="I161" s="1" t="inlineStr">
         <is>
-          <t>Chocolat Orange 400g x24 pcs</t>
+          <t>Chocolat Orange 10 g x 60 pcs x 6 boites</t>
         </is>
       </c>
       <c r="J161" s="1" t="n">
         <v>5.0</v>
       </c>
       <c r="K161" s="1" t="n">
-        <v>105000.0</v>
+        <v>75000.0</v>
       </c>
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
@@ -9113,14 +9113,14 @@
       <c r="H162" s="1"/>
       <c r="I162" s="1" t="inlineStr">
         <is>
-          <t>Chocolat Orange 10 g x 60 pcs x 6 boites</t>
+          <t>Lait Kamlac sachet 18gx100</t>
         </is>
       </c>
       <c r="J162" s="1" t="n">
-        <v>5.0</v>
+        <v>14.6</v>
       </c>
       <c r="K162" s="1" t="n">
-        <v>75000.0</v>
+        <v>109500.0</v>
       </c>
       <c r="L162" s="1"/>
       <c r="M162" s="1"/>

</xml_diff>

<commit_message>
Rapport du 10 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -3605,10 +3605,10 @@
         </is>
       </c>
       <c r="J64" s="1" t="n">
-        <v>7.8333335</v>
+        <v>7.4166665</v>
       </c>
       <c r="K64" s="1" t="n">
-        <v>262416.66</v>
+        <v>248458.33</v>
       </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>

</xml_diff>

<commit_message>
Rapport du 11 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8BC9AF-B10A-423B-BF70-0268095953FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB3FB3E-91D0-4C4D-90F1-777E4EDDE729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10181" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10168" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -347,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -358,6 +358,12 @@
     <font>
       <sz val="11"/>
       <name val="TIMES"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -720,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D86" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89:H90"/>
+    <sheetView tabSelected="1" topLeftCell="A661" workbookViewId="0">
+      <selection activeCell="G535" sqref="G535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4389,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>53</v>
@@ -4401,10 +4407,7 @@
         <v>19</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>26</v>
@@ -4433,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>53</v>
@@ -4445,10 +4448,7 @@
         <v>19</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>33</v>
@@ -4477,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>53</v>
@@ -4489,10 +4489,7 @@
         <v>19</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>34</v>
@@ -10393,7 +10390,7 @@
         <v>0</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>53</v>
@@ -10405,10 +10402,7 @@
         <v>71</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H237" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I237" s="1" t="s">
         <v>33</v>
@@ -10437,7 +10431,7 @@
         <v>0</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>53</v>
@@ -10449,10 +10443,7 @@
         <v>71</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H238" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I238" s="1" t="s">
         <v>44</v>
@@ -10481,7 +10472,7 @@
         <v>0</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>53</v>
@@ -10493,10 +10484,7 @@
         <v>71</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H239" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="I239" s="1" t="s">
         <v>33</v>
@@ -15403,7 +15391,7 @@
         <v>0</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D356" s="1" t="s">
         <v>53</v>
@@ -15415,10 +15403,7 @@
         <v>75</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H356" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I356" s="1" t="s">
         <v>33</v>
@@ -15447,7 +15432,7 @@
         <v>0</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D357" s="1" t="s">
         <v>53</v>
@@ -15459,10 +15444,7 @@
         <v>75</v>
       </c>
       <c r="G357" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H357" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I357" s="1" t="s">
         <v>44</v>
@@ -15491,7 +15473,7 @@
         <v>0</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D358" s="1" t="s">
         <v>53</v>
@@ -15503,10 +15485,7 @@
         <v>75</v>
       </c>
       <c r="G358" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H358" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="I358" s="1" t="s">
         <v>26</v>
@@ -15535,7 +15514,7 @@
         <v>0</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D359" s="1" t="s">
         <v>53</v>
@@ -15547,10 +15526,7 @@
         <v>75</v>
       </c>
       <c r="G359" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H359" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="I359" s="1" t="s">
         <v>34</v>
@@ -22733,7 +22709,7 @@
         <v>0</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D536" s="1" t="s">
         <v>53</v>
@@ -22745,10 +22721,7 @@
         <v>79</v>
       </c>
       <c r="G536" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H536" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I536" s="1" t="s">
         <v>33</v>
@@ -22777,7 +22750,7 @@
         <v>0</v>
       </c>
       <c r="C537" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D537" s="1" t="s">
         <v>53</v>
@@ -22789,10 +22762,7 @@
         <v>79</v>
       </c>
       <c r="G537" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H537" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="I537" s="1" t="s">
         <v>26</v>
@@ -22821,7 +22791,7 @@
         <v>0</v>
       </c>
       <c r="C538" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D538" s="1" t="s">
         <v>53</v>
@@ -22833,10 +22803,7 @@
         <v>79</v>
       </c>
       <c r="G538" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H538" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="I538" s="1" t="s">
         <v>34</v>
@@ -65772,6 +65739,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rapport du 14 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B29C15-C154-46BF-96DC-3B850890E7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C1D49A-E21A-4DCC-B795-FD1E6AC7CE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:P1873"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L193" activeCellId="2" sqref="L232:M261 M231 L193:M230"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -835,7 +835,7 @@
         <v>9750</v>
       </c>
       <c r="L2" s="1">
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>

</xml_diff>

<commit_message>
Rapport du 16 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0338323C-94F0-40BF-80DB-EDF7A201395D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B1F63A-CBE8-44C1-985D-18FBFB99B052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G109" workbookViewId="0">
-      <selection activeCell="L127" activeCellId="1" sqref="L174:M213 L127:M172"/>
+    <sheetView tabSelected="1" topLeftCell="C47" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="L22" activeCellId="1" sqref="L63:L106 L22:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2572,9 +2572,7 @@
       <c r="K45" s="1">
         <v>7150</v>
       </c>
-      <c r="L45" s="1">
-        <v>3500</v>
-      </c>
+      <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1">
@@ -3288,7 +3286,9 @@
       <c r="K62" s="1">
         <v>1225</v>
       </c>
-      <c r="L62" s="1"/>
+      <c r="L62" s="1">
+        <v>3500</v>
+      </c>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1">
@@ -5944,7 +5944,9 @@
       <c r="K127" s="1">
         <v>5750</v>
       </c>
-      <c r="L127" s="1"/>
+      <c r="L127" s="1">
+        <v>3000</v>
+      </c>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1">
@@ -5986,7 +5988,9 @@
       <c r="K128" s="1">
         <v>10250</v>
       </c>
-      <c r="L128" s="1"/>
+      <c r="L128" s="1">
+        <v>3000</v>
+      </c>
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1">
@@ -6028,7 +6032,9 @@
       <c r="K129" s="1">
         <v>12000</v>
       </c>
-      <c r="L129" s="1"/>
+      <c r="L129" s="1">
+        <v>3000</v>
+      </c>
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1">
@@ -6070,7 +6076,9 @@
       <c r="K130" s="1">
         <v>10000</v>
       </c>
-      <c r="L130" s="1"/>
+      <c r="L130" s="1">
+        <v>3000</v>
+      </c>
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1">
@@ -6112,7 +6120,9 @@
       <c r="K131" s="1">
         <v>6250</v>
       </c>
-      <c r="L131" s="1"/>
+      <c r="L131" s="1">
+        <v>3000</v>
+      </c>
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1">
@@ -6154,7 +6164,9 @@
       <c r="K132" s="1">
         <v>7350</v>
       </c>
-      <c r="L132" s="1"/>
+      <c r="L132" s="1">
+        <v>3000</v>
+      </c>
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
       <c r="O132" s="1">
@@ -6196,7 +6208,9 @@
       <c r="K133" s="1">
         <v>5125</v>
       </c>
-      <c r="L133" s="1"/>
+      <c r="L133" s="1">
+        <v>3000</v>
+      </c>
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
       <c r="O133" s="1">
@@ -6238,7 +6252,9 @@
       <c r="K134" s="1">
         <v>2000</v>
       </c>
-      <c r="L134" s="1"/>
+      <c r="L134" s="1">
+        <v>3000</v>
+      </c>
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1">
@@ -6280,7 +6296,9 @@
       <c r="K135" s="1">
         <v>9750</v>
       </c>
-      <c r="L135" s="1"/>
+      <c r="L135" s="1">
+        <v>3000</v>
+      </c>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1">
@@ -6322,7 +6340,9 @@
       <c r="K136" s="1">
         <v>1225</v>
       </c>
-      <c r="L136" s="1"/>
+      <c r="L136" s="1">
+        <v>3000</v>
+      </c>
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
       <c r="O136" s="1">
@@ -6364,7 +6384,9 @@
       <c r="K137" s="1">
         <v>5750</v>
       </c>
-      <c r="L137" s="1"/>
+      <c r="L137" s="1">
+        <v>3000</v>
+      </c>
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
       <c r="O137" s="1">
@@ -6406,7 +6428,9 @@
       <c r="K138" s="1">
         <v>5125</v>
       </c>
-      <c r="L138" s="1"/>
+      <c r="L138" s="1">
+        <v>3000</v>
+      </c>
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
       <c r="O138" s="1">
@@ -6448,7 +6472,9 @@
       <c r="K139" s="1">
         <v>9750</v>
       </c>
-      <c r="L139" s="1"/>
+      <c r="L139" s="1">
+        <v>3000</v>
+      </c>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1">
@@ -6490,7 +6516,9 @@
       <c r="K140" s="1">
         <v>21000</v>
       </c>
-      <c r="L140" s="1"/>
+      <c r="L140" s="1">
+        <v>3000</v>
+      </c>
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
       <c r="O140" s="1">
@@ -6532,7 +6560,9 @@
       <c r="K141" s="1">
         <v>7750</v>
       </c>
-      <c r="L141" s="1"/>
+      <c r="L141" s="1">
+        <v>3000</v>
+      </c>
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
       <c r="O141" s="1">
@@ -6574,7 +6604,9 @@
       <c r="K142" s="1">
         <v>7000</v>
       </c>
-      <c r="L142" s="1"/>
+      <c r="L142" s="1">
+        <v>3000</v>
+      </c>
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1">
@@ -6616,7 +6648,9 @@
       <c r="K143" s="1">
         <v>20500</v>
       </c>
-      <c r="L143" s="1"/>
+      <c r="L143" s="1">
+        <v>3000</v>
+      </c>
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1">
@@ -6658,7 +6692,9 @@
       <c r="K144" s="1">
         <v>5000</v>
       </c>
-      <c r="L144" s="1"/>
+      <c r="L144" s="1">
+        <v>3000</v>
+      </c>
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
       <c r="O144" s="1">
@@ -6700,7 +6736,9 @@
       <c r="K145" s="1">
         <v>19500</v>
       </c>
-      <c r="L145" s="1"/>
+      <c r="L145" s="1">
+        <v>3000</v>
+      </c>
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1">
@@ -6742,7 +6780,9 @@
       <c r="K146" s="1">
         <v>15375</v>
       </c>
-      <c r="L146" s="1"/>
+      <c r="L146" s="1">
+        <v>3000</v>
+      </c>
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
       <c r="O146" s="1">
@@ -6784,7 +6824,9 @@
       <c r="K147" s="1">
         <v>23000</v>
       </c>
-      <c r="L147" s="1"/>
+      <c r="L147" s="1">
+        <v>3000</v>
+      </c>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1">
@@ -6826,7 +6868,9 @@
       <c r="K148" s="1">
         <v>1225</v>
       </c>
-      <c r="L148" s="1"/>
+      <c r="L148" s="1">
+        <v>3000</v>
+      </c>
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1">
@@ -6868,7 +6912,9 @@
       <c r="K149" s="1">
         <v>20500</v>
       </c>
-      <c r="L149" s="1"/>
+      <c r="L149" s="1">
+        <v>3000</v>
+      </c>
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1">
@@ -6910,7 +6956,9 @@
       <c r="K150" s="1">
         <v>23000</v>
       </c>
-      <c r="L150" s="1"/>
+      <c r="L150" s="1">
+        <v>3000</v>
+      </c>
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1">
@@ -6952,7 +7000,9 @@
       <c r="K151" s="1">
         <v>1225</v>
       </c>
-      <c r="L151" s="1"/>
+      <c r="L151" s="1">
+        <v>3000</v>
+      </c>
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1">
@@ -6994,7 +7044,9 @@
       <c r="K152" s="1">
         <v>11500</v>
       </c>
-      <c r="L152" s="1"/>
+      <c r="L152" s="1">
+        <v>3000</v>
+      </c>
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1">
@@ -7036,7 +7088,9 @@
       <c r="K153" s="1">
         <v>19500</v>
       </c>
-      <c r="L153" s="1"/>
+      <c r="L153" s="1">
+        <v>3000</v>
+      </c>
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1">
@@ -7078,7 +7132,9 @@
       <c r="K154" s="1">
         <v>5125</v>
       </c>
-      <c r="L154" s="1"/>
+      <c r="L154" s="1">
+        <v>3000</v>
+      </c>
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1">
@@ -7120,7 +7176,9 @@
       <c r="K155" s="1">
         <v>11500</v>
       </c>
-      <c r="L155" s="1"/>
+      <c r="L155" s="1">
+        <v>3000</v>
+      </c>
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1">
@@ -7162,7 +7220,9 @@
       <c r="K156" s="1">
         <v>20500</v>
       </c>
-      <c r="L156" s="1"/>
+      <c r="L156" s="1">
+        <v>3000</v>
+      </c>
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1">
@@ -7204,7 +7264,9 @@
       <c r="K157" s="1">
         <v>1225</v>
       </c>
-      <c r="L157" s="1"/>
+      <c r="L157" s="1">
+        <v>3000</v>
+      </c>
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1">
@@ -7246,7 +7308,9 @@
       <c r="K158" s="1">
         <v>19500</v>
       </c>
-      <c r="L158" s="1"/>
+      <c r="L158" s="1">
+        <v>3000</v>
+      </c>
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1">
@@ -7288,7 +7352,9 @@
       <c r="K159" s="1">
         <v>18750</v>
       </c>
-      <c r="L159" s="1"/>
+      <c r="L159" s="1">
+        <v>3000</v>
+      </c>
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1">
@@ -7330,7 +7396,9 @@
       <c r="K160" s="1">
         <v>15500</v>
       </c>
-      <c r="L160" s="1"/>
+      <c r="L160" s="1">
+        <v>3000</v>
+      </c>
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1">
@@ -7372,7 +7440,9 @@
       <c r="K161" s="1">
         <v>6250</v>
       </c>
-      <c r="L161" s="1"/>
+      <c r="L161" s="1">
+        <v>3000</v>
+      </c>
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1">
@@ -7414,7 +7484,9 @@
       <c r="K162" s="1">
         <v>5000</v>
       </c>
-      <c r="L162" s="1"/>
+      <c r="L162" s="1">
+        <v>3000</v>
+      </c>
       <c r="M162" s="1"/>
       <c r="N162" s="1"/>
       <c r="O162" s="1">
@@ -7456,7 +7528,9 @@
       <c r="K163" s="1">
         <v>7750</v>
       </c>
-      <c r="L163" s="1"/>
+      <c r="L163" s="1">
+        <v>3000</v>
+      </c>
       <c r="M163" s="1"/>
       <c r="N163" s="1"/>
       <c r="O163" s="1">
@@ -7498,7 +7572,9 @@
       <c r="K164" s="1">
         <v>16750</v>
       </c>
-      <c r="L164" s="1"/>
+      <c r="L164" s="1">
+        <v>3000</v>
+      </c>
       <c r="M164" s="1"/>
       <c r="N164" s="1"/>
       <c r="O164" s="1">
@@ -7540,7 +7616,9 @@
       <c r="K165" s="1">
         <v>5125</v>
       </c>
-      <c r="L165" s="1"/>
+      <c r="L165" s="1">
+        <v>3000</v>
+      </c>
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
       <c r="O165" s="1">
@@ -7582,7 +7660,9 @@
       <c r="K166" s="1">
         <v>2000</v>
       </c>
-      <c r="L166" s="1"/>
+      <c r="L166" s="1">
+        <v>3000</v>
+      </c>
       <c r="M166" s="1"/>
       <c r="N166" s="1"/>
       <c r="O166" s="1">
@@ -7624,7 +7704,9 @@
       <c r="K167" s="1">
         <v>10250</v>
       </c>
-      <c r="L167" s="1"/>
+      <c r="L167" s="1">
+        <v>3000</v>
+      </c>
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
       <c r="O167" s="1">
@@ -7666,7 +7748,9 @@
       <c r="K168" s="1">
         <v>1225</v>
       </c>
-      <c r="L168" s="1"/>
+      <c r="L168" s="1">
+        <v>3000</v>
+      </c>
       <c r="M168" s="1"/>
       <c r="N168" s="1"/>
       <c r="O168" s="1">
@@ -7708,7 +7792,9 @@
       <c r="K169" s="1">
         <v>6250</v>
       </c>
-      <c r="L169" s="1"/>
+      <c r="L169" s="1">
+        <v>3000</v>
+      </c>
       <c r="M169" s="1"/>
       <c r="N169" s="1"/>
       <c r="O169" s="1">
@@ -7750,7 +7836,9 @@
       <c r="K170" s="1">
         <v>19500</v>
       </c>
-      <c r="L170" s="1"/>
+      <c r="L170" s="1">
+        <v>3000</v>
+      </c>
       <c r="M170" s="1"/>
       <c r="N170" s="1"/>
       <c r="O170" s="1">
@@ -7792,7 +7880,9 @@
       <c r="K171" s="1">
         <v>5125</v>
       </c>
-      <c r="L171" s="1"/>
+      <c r="L171" s="1">
+        <v>3000</v>
+      </c>
       <c r="M171" s="1"/>
       <c r="N171" s="1"/>
       <c r="O171" s="1">
@@ -7834,7 +7924,9 @@
       <c r="K172" s="1">
         <v>1000</v>
       </c>
-      <c r="L172" s="1"/>
+      <c r="L172" s="1">
+        <v>3000</v>
+      </c>
       <c r="M172" s="1"/>
       <c r="N172" s="1"/>
       <c r="O172" s="1">
@@ -7922,8 +8014,12 @@
       <c r="K174" s="1">
         <v>8575</v>
       </c>
-      <c r="L174" s="1"/>
-      <c r="M174" s="1"/>
+      <c r="L174" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M174" s="1">
+        <v>5000</v>
+      </c>
       <c r="N174" s="1"/>
       <c r="O174" s="1">
         <v>1922</v>
@@ -7964,8 +8060,12 @@
       <c r="K175" s="1">
         <v>5125</v>
       </c>
-      <c r="L175" s="1"/>
-      <c r="M175" s="1"/>
+      <c r="L175" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M175" s="1">
+        <v>5000</v>
+      </c>
       <c r="N175" s="1"/>
       <c r="O175" s="1">
         <v>1923</v>
@@ -8006,8 +8106,12 @@
       <c r="K176" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L176" s="1"/>
-      <c r="M176" s="1"/>
+      <c r="L176" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M176" s="1">
+        <v>5000</v>
+      </c>
       <c r="N176" s="1"/>
       <c r="O176" s="1">
         <v>1924</v>
@@ -8048,8 +8152,12 @@
       <c r="K177" s="1">
         <v>520.83330000000001</v>
       </c>
-      <c r="L177" s="1"/>
-      <c r="M177" s="1"/>
+      <c r="L177" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M177" s="1">
+        <v>5000</v>
+      </c>
       <c r="N177" s="1"/>
       <c r="O177" s="1">
         <v>1925</v>
@@ -8090,8 +8198,12 @@
       <c r="K178" s="1">
         <v>11500</v>
       </c>
-      <c r="L178" s="1"/>
-      <c r="M178" s="1"/>
+      <c r="L178" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M178" s="1">
+        <v>5000</v>
+      </c>
       <c r="N178" s="1"/>
       <c r="O178" s="1">
         <v>1926</v>
@@ -8132,8 +8244,12 @@
       <c r="K179" s="1">
         <v>6250</v>
       </c>
-      <c r="L179" s="1"/>
-      <c r="M179" s="1"/>
+      <c r="L179" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M179" s="1">
+        <v>5000</v>
+      </c>
       <c r="N179" s="1"/>
       <c r="O179" s="1">
         <v>1927</v>
@@ -8174,8 +8290,12 @@
       <c r="K180" s="1">
         <v>9750</v>
       </c>
-      <c r="L180" s="1"/>
-      <c r="M180" s="1"/>
+      <c r="L180" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M180" s="1">
+        <v>5000</v>
+      </c>
       <c r="N180" s="1"/>
       <c r="O180" s="1">
         <v>1928</v>
@@ -8216,8 +8336,12 @@
       <c r="K181" s="1">
         <v>1000</v>
       </c>
-      <c r="L181" s="1"/>
-      <c r="M181" s="1"/>
+      <c r="L181" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M181" s="1">
+        <v>5000</v>
+      </c>
       <c r="N181" s="1"/>
       <c r="O181" s="1">
         <v>1929</v>
@@ -8258,8 +8382,12 @@
       <c r="K182" s="1">
         <v>15500</v>
       </c>
-      <c r="L182" s="1"/>
-      <c r="M182" s="1"/>
+      <c r="L182" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M182" s="1">
+        <v>5000</v>
+      </c>
       <c r="N182" s="1"/>
       <c r="O182" s="1">
         <v>1930</v>
@@ -8300,8 +8428,12 @@
       <c r="K183" s="1">
         <v>20500</v>
       </c>
-      <c r="L183" s="1"/>
-      <c r="M183" s="1"/>
+      <c r="L183" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M183" s="1">
+        <v>5000</v>
+      </c>
       <c r="N183" s="1"/>
       <c r="O183" s="1">
         <v>1931</v>
@@ -8342,8 +8474,12 @@
       <c r="K184" s="1">
         <v>8750</v>
       </c>
-      <c r="L184" s="1"/>
-      <c r="M184" s="1"/>
+      <c r="L184" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M184" s="1">
+        <v>5000</v>
+      </c>
       <c r="N184" s="1"/>
       <c r="O184" s="1">
         <v>1932</v>
@@ -8384,8 +8520,12 @@
       <c r="K185" s="1">
         <v>5750</v>
       </c>
-      <c r="L185" s="1"/>
-      <c r="M185" s="1"/>
+      <c r="L185" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M185" s="1">
+        <v>5000</v>
+      </c>
       <c r="N185" s="1"/>
       <c r="O185" s="1">
         <v>1933</v>
@@ -8426,8 +8566,12 @@
       <c r="K186" s="1">
         <v>10000</v>
       </c>
-      <c r="L186" s="1"/>
-      <c r="M186" s="1"/>
+      <c r="L186" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M186" s="1">
+        <v>5000</v>
+      </c>
       <c r="N186" s="1"/>
       <c r="O186" s="1">
         <v>1934</v>
@@ -8468,8 +8612,12 @@
       <c r="K187" s="1">
         <v>6250</v>
       </c>
-      <c r="L187" s="1"/>
-      <c r="M187" s="1"/>
+      <c r="L187" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M187" s="1">
+        <v>5000</v>
+      </c>
       <c r="N187" s="1"/>
       <c r="O187" s="1">
         <v>1935</v>
@@ -8510,8 +8658,12 @@
       <c r="K188" s="1">
         <v>20500</v>
       </c>
-      <c r="L188" s="1"/>
-      <c r="M188" s="1"/>
+      <c r="L188" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M188" s="1">
+        <v>5000</v>
+      </c>
       <c r="N188" s="1"/>
       <c r="O188" s="1">
         <v>1936</v>
@@ -8552,8 +8704,12 @@
       <c r="K189" s="1">
         <v>11500</v>
       </c>
-      <c r="L189" s="1"/>
-      <c r="M189" s="1"/>
+      <c r="L189" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M189" s="1">
+        <v>5000</v>
+      </c>
       <c r="N189" s="1"/>
       <c r="O189" s="1">
         <v>1937</v>
@@ -8594,8 +8750,12 @@
       <c r="K190" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L190" s="1"/>
-      <c r="M190" s="1"/>
+      <c r="L190" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M190" s="1">
+        <v>5000</v>
+      </c>
       <c r="N190" s="1"/>
       <c r="O190" s="1">
         <v>1938</v>
@@ -8636,8 +8796,12 @@
       <c r="K191" s="1">
         <v>1225</v>
       </c>
-      <c r="L191" s="1"/>
-      <c r="M191" s="1"/>
+      <c r="L191" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M191" s="1">
+        <v>5000</v>
+      </c>
       <c r="N191" s="1"/>
       <c r="O191" s="1">
         <v>1939</v>
@@ -8678,8 +8842,12 @@
       <c r="K192" s="1">
         <v>31250</v>
       </c>
-      <c r="L192" s="1"/>
-      <c r="M192" s="1"/>
+      <c r="L192" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M192" s="1">
+        <v>5000</v>
+      </c>
       <c r="N192" s="1"/>
       <c r="O192" s="1">
         <v>1940</v>
@@ -8720,8 +8888,12 @@
       <c r="K193" s="1">
         <v>23000</v>
       </c>
-      <c r="L193" s="1"/>
-      <c r="M193" s="1"/>
+      <c r="L193" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M193" s="1">
+        <v>5000</v>
+      </c>
       <c r="N193" s="1"/>
       <c r="O193" s="1">
         <v>1941</v>
@@ -8762,8 +8934,12 @@
       <c r="K194" s="1">
         <v>5125</v>
       </c>
-      <c r="L194" s="1"/>
-      <c r="M194" s="1"/>
+      <c r="L194" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M194" s="1">
+        <v>5000</v>
+      </c>
       <c r="N194" s="1"/>
       <c r="O194" s="1">
         <v>1942</v>
@@ -8804,8 +8980,12 @@
       <c r="K195" s="1">
         <v>5000</v>
       </c>
-      <c r="L195" s="1"/>
-      <c r="M195" s="1"/>
+      <c r="L195" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M195" s="1">
+        <v>5000</v>
+      </c>
       <c r="N195" s="1"/>
       <c r="O195" s="1">
         <v>1943</v>
@@ -8846,8 +9026,12 @@
       <c r="K196" s="1">
         <v>10250</v>
       </c>
-      <c r="L196" s="1"/>
-      <c r="M196" s="1"/>
+      <c r="L196" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M196" s="1">
+        <v>5000</v>
+      </c>
       <c r="N196" s="1"/>
       <c r="O196" s="1">
         <v>1944</v>
@@ -8888,8 +9072,12 @@
       <c r="K197" s="1">
         <v>7750</v>
       </c>
-      <c r="L197" s="1"/>
-      <c r="M197" s="1"/>
+      <c r="L197" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M197" s="1">
+        <v>5000</v>
+      </c>
       <c r="N197" s="1"/>
       <c r="O197" s="1">
         <v>1945</v>
@@ -8930,8 +9118,12 @@
       <c r="K198" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L198" s="1"/>
-      <c r="M198" s="1"/>
+      <c r="L198" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M198" s="1">
+        <v>5000</v>
+      </c>
       <c r="N198" s="1"/>
       <c r="O198" s="1">
         <v>1946</v>
@@ -8972,8 +9164,12 @@
       <c r="K199" s="1">
         <v>1225</v>
       </c>
-      <c r="L199" s="1"/>
-      <c r="M199" s="1"/>
+      <c r="L199" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M199" s="1">
+        <v>5000</v>
+      </c>
       <c r="N199" s="1"/>
       <c r="O199" s="1">
         <v>1947</v>
@@ -9014,8 +9210,12 @@
       <c r="K200" s="1">
         <v>23250</v>
       </c>
-      <c r="L200" s="1"/>
-      <c r="M200" s="1"/>
+      <c r="L200" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M200" s="1">
+        <v>5000</v>
+      </c>
       <c r="N200" s="1"/>
       <c r="O200" s="1">
         <v>1948</v>
@@ -9056,8 +9256,12 @@
       <c r="K201" s="1">
         <v>1225</v>
       </c>
-      <c r="L201" s="1"/>
-      <c r="M201" s="1"/>
+      <c r="L201" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M201" s="1">
+        <v>5000</v>
+      </c>
       <c r="N201" s="1"/>
       <c r="O201" s="1">
         <v>1949</v>
@@ -9098,8 +9302,12 @@
       <c r="K202" s="1">
         <v>520.83330000000001</v>
       </c>
-      <c r="L202" s="1"/>
-      <c r="M202" s="1"/>
+      <c r="L202" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M202" s="1">
+        <v>5000</v>
+      </c>
       <c r="N202" s="1"/>
       <c r="O202" s="1">
         <v>1950</v>
@@ -9140,8 +9348,12 @@
       <c r="K203" s="1">
         <v>10250</v>
       </c>
-      <c r="L203" s="1"/>
-      <c r="M203" s="1"/>
+      <c r="L203" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M203" s="1">
+        <v>5000</v>
+      </c>
       <c r="N203" s="1"/>
       <c r="O203" s="1">
         <v>1951</v>
@@ -9182,8 +9394,12 @@
       <c r="K204" s="1">
         <v>1225</v>
       </c>
-      <c r="L204" s="1"/>
-      <c r="M204" s="1"/>
+      <c r="L204" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M204" s="1">
+        <v>5000</v>
+      </c>
       <c r="N204" s="1"/>
       <c r="O204" s="1">
         <v>1952</v>
@@ -9224,8 +9440,12 @@
       <c r="K205" s="1">
         <v>6500</v>
       </c>
-      <c r="L205" s="1"/>
-      <c r="M205" s="1"/>
+      <c r="L205" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M205" s="1">
+        <v>5000</v>
+      </c>
       <c r="N205" s="1"/>
       <c r="O205" s="1">
         <v>1953</v>
@@ -9266,8 +9486,12 @@
       <c r="K206" s="1">
         <v>19500</v>
       </c>
-      <c r="L206" s="1"/>
-      <c r="M206" s="1"/>
+      <c r="L206" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M206" s="1">
+        <v>5000</v>
+      </c>
       <c r="N206" s="1"/>
       <c r="O206" s="1">
         <v>1954</v>
@@ -9308,8 +9532,12 @@
       <c r="K207" s="1">
         <v>10250</v>
       </c>
-      <c r="L207" s="1"/>
-      <c r="M207" s="1"/>
+      <c r="L207" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M207" s="1">
+        <v>5000</v>
+      </c>
       <c r="N207" s="1"/>
       <c r="O207" s="1">
         <v>1955</v>
@@ -9350,8 +9578,12 @@
       <c r="K208" s="1">
         <v>5750</v>
       </c>
-      <c r="L208" s="1"/>
-      <c r="M208" s="1"/>
+      <c r="L208" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M208" s="1">
+        <v>5000</v>
+      </c>
       <c r="N208" s="1"/>
       <c r="O208" s="1">
         <v>1956</v>
@@ -9392,8 +9624,12 @@
       <c r="K209" s="1">
         <v>5000</v>
       </c>
-      <c r="L209" s="1"/>
-      <c r="M209" s="1"/>
+      <c r="L209" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M209" s="1">
+        <v>5000</v>
+      </c>
       <c r="N209" s="1"/>
       <c r="O209" s="1">
         <v>1957</v>
@@ -9434,8 +9670,12 @@
       <c r="K210" s="1">
         <v>15375</v>
       </c>
-      <c r="L210" s="1"/>
-      <c r="M210" s="1"/>
+      <c r="L210" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M210" s="1">
+        <v>5000</v>
+      </c>
       <c r="N210" s="1"/>
       <c r="O210" s="1">
         <v>1958</v>
@@ -9476,8 +9716,12 @@
       <c r="K211" s="1">
         <v>11500</v>
       </c>
-      <c r="L211" s="1"/>
-      <c r="M211" s="1"/>
+      <c r="L211" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M211" s="1">
+        <v>5000</v>
+      </c>
       <c r="N211" s="1"/>
       <c r="O211" s="1">
         <v>1959</v>
@@ -9518,8 +9762,12 @@
       <c r="K212" s="1">
         <v>520.83330000000001</v>
       </c>
-      <c r="L212" s="1"/>
-      <c r="M212" s="1"/>
+      <c r="L212" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M212" s="1">
+        <v>5000</v>
+      </c>
       <c r="N212" s="1"/>
       <c r="O212" s="1">
         <v>1960</v>
@@ -9560,8 +9808,12 @@
       <c r="K213" s="1">
         <v>1225</v>
       </c>
-      <c r="L213" s="1"/>
-      <c r="M213" s="1"/>
+      <c r="L213" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M213" s="1">
+        <v>5000</v>
+      </c>
       <c r="N213" s="1"/>
       <c r="O213" s="1">
         <v>1961</v>

</xml_diff>

<commit_message>
Rapport du 05 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -70,21 +70,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.37109375" customWidth="true"/>
-    <col min="2" max="2" width="26.43359375" customWidth="true"/>
+    <col min="2" max="2" width="2.33984375" customWidth="true"/>
     <col min="3" max="3" width="8.57421875" customWidth="true"/>
     <col min="4" max="4" width="40.35546875" customWidth="true"/>
     <col min="5" max="5" width="16.5234375" customWidth="true"/>
     <col min="6" max="6" width="11.38671875" customWidth="true"/>
-    <col min="7" max="7" width="26.18359375" customWidth="true"/>
-    <col min="8" max="8" width="9.55078125" customWidth="true"/>
+    <col min="7" max="7" width="20.43359375" customWidth="true"/>
     <col min="9" max="9" width="41.47265625" customWidth="true"/>
-    <col min="10" max="10" width="19.4609375" customWidth="true"/>
+    <col min="10" max="10" width="13.96484375" customWidth="true"/>
     <col min="11" max="11" width="11.515625" customWidth="true"/>
-    <col min="12" max="12" width="10.53125" customWidth="true"/>
-    <col min="13" max="13" width="15.3046875" customWidth="true"/>
-    <col min="14" max="14" width="14.3203125" customWidth="true"/>
-    <col min="15" max="15" width="11.51171875" customWidth="true"/>
-    <col min="16" max="16" width="18.48046875" customWidth="true"/>
+    <col min="12" max="12" width="6.01171875" customWidth="true"/>
+    <col min="15" max="15" width="4.7890625" customWidth="true"/>
+    <col min="16" max="16" width="5.03125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5241,6 +5238,1926 @@
         </is>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B96" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D96" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E96" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1" t="inlineStr">
+        <is>
+          <t>Café pot Refraish 50g</t>
+        </is>
+      </c>
+      <c r="J96" s="1" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="K96" s="1" t="n">
+        <v>430500.0</v>
+      </c>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="P96" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B97" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D97" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E97" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1" t="inlineStr">
+        <is>
+          <t>Café stick Altimo 1,5gx09boites</t>
+        </is>
+      </c>
+      <c r="J97" s="1" t="n">
+        <v>14.777778</v>
+      </c>
+      <c r="K97" s="1" t="n">
+        <v>443333.34</v>
+      </c>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="P97" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B98" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C98" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D98" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E98" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1" t="inlineStr">
+        <is>
+          <t>Café Altimo pot 50g x 24 pcs</t>
+        </is>
+      </c>
+      <c r="J98" s="1" t="n">
+        <v>19.166666</v>
+      </c>
+      <c r="K98" s="1" t="n">
+        <v>335416.66</v>
+      </c>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="P98" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B99" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C99" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D99" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E99" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1" t="inlineStr">
+        <is>
+          <t>Café Altimo pot 100g x 24 pcs</t>
+        </is>
+      </c>
+      <c r="J99" s="1" t="n">
+        <v>14.208333</v>
+      </c>
+      <c r="K99" s="1" t="n">
+        <v>475979.16</v>
+      </c>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="P99" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B100" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C100" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D100" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E100" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1" t="inlineStr">
+        <is>
+          <t>Café Altimo pot 200g x 12 pcs</t>
+        </is>
+      </c>
+      <c r="J100" s="1" t="n">
+        <v>12.833333</v>
+      </c>
+      <c r="K100" s="1" t="n">
+        <v>442750.0</v>
+      </c>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="P100" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B101" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C101" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D101" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E101" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1" t="inlineStr">
+        <is>
+          <t>Kamlac évaporé 48x160g</t>
+        </is>
+      </c>
+      <c r="J101" s="1" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K101" s="1" t="n">
+        <v>456750.0</v>
+      </c>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="P101" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B102" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C102" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D102" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E102" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1" t="inlineStr">
+        <is>
+          <t>KamLac Lait concentré sucré 24x1kg</t>
+        </is>
+      </c>
+      <c r="J102" s="1" t="n">
+        <v>10.833333</v>
+      </c>
+      <c r="K102" s="1" t="n">
+        <v>260000.0</v>
+      </c>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="P102" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B103" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C103" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D103" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E103" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1" t="inlineStr">
+        <is>
+          <t>Lait Janus 18gx100</t>
+        </is>
+      </c>
+      <c r="J103" s="1" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="K103" s="1" t="n">
+        <v>57200.0</v>
+      </c>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="P103" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B104" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C104" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D104" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E104" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1" t="inlineStr">
+        <is>
+          <t>Lait Kamlac sachet 18gx100</t>
+        </is>
+      </c>
+      <c r="J104" s="1" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="K104" s="1" t="n">
+        <v>82500.0</v>
+      </c>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="P104" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B105" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C105" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D105" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E105" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1" t="inlineStr">
+        <is>
+          <t>Lait Janus 400gx10</t>
+        </is>
+      </c>
+      <c r="J105" s="1" t="n">
+        <v>50.8</v>
+      </c>
+      <c r="K105" s="1" t="n">
+        <v>622300.0</v>
+      </c>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="P105" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B106" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C106" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D106" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E106" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1" t="inlineStr">
+        <is>
+          <t>Jus Lido</t>
+        </is>
+      </c>
+      <c r="J106" s="1" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="K106" s="1" t="n">
+        <v>468000.0</v>
+      </c>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="P106" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B107" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C107" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D107" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E107" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat 3-en-1 30x120 pcs</t>
+        </is>
+      </c>
+      <c r="J107" s="1" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="K107" s="1" t="n">
+        <v>53300.0</v>
+      </c>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="P107" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B108" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C108" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D108" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E108" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat transparent 200gx24pcs</t>
+        </is>
+      </c>
+      <c r="J108" s="1" t="n">
+        <v>0.41666666</v>
+      </c>
+      <c r="K108" s="1" t="n">
+        <v>5208.3335</v>
+      </c>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="P108" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B109" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C109" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D109" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E109" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat transparent 400gx12pcs</t>
+        </is>
+      </c>
+      <c r="J109" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K109" s="1" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="P109" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B110" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C110" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D110" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E110" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat jaune 200g x 24 pcs</t>
+        </is>
+      </c>
+      <c r="J110" s="1" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="K110" s="1" t="n">
+        <v>201500.0</v>
+      </c>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="P110" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B111" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C111" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D111" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E111" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat jaune 400g x 12 pcs</t>
+        </is>
+      </c>
+      <c r="J111" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="K111" s="1" t="n">
+        <v>178250.0</v>
+      </c>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1" t="n">
+        <v>110.0</v>
+      </c>
+      <c r="P111" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B112" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C112" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D112" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E112" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Jaune 10gx60pcsx6 boites</t>
+        </is>
+      </c>
+      <c r="J112" s="1" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="K112" s="1" t="n">
+        <v>105000.0</v>
+      </c>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="P112" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B113" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C113" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D113" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E113" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Orange 200g x24 pcs</t>
+        </is>
+      </c>
+      <c r="J113" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="K113" s="1" t="n">
+        <v>147000.0</v>
+      </c>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="P113" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B114" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C114" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D114" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E114" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Orange 400g x12 pcs</t>
+        </is>
+      </c>
+      <c r="J114" s="1" t="n">
+        <v>4.8333335</v>
+      </c>
+      <c r="K114" s="1" t="n">
+        <v>101500.0</v>
+      </c>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="P114" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B115" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C115" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D115" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E115" s="1" t="inlineStr">
+        <is>
+          <t>Stock Descente</t>
+        </is>
+      </c>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Orange 10 g x 60 pcs x 6 boites</t>
+        </is>
+      </c>
+      <c r="J115" s="1" t="n">
+        <v>6.1666665</v>
+      </c>
+      <c r="K115" s="1" t="n">
+        <v>92500.0</v>
+      </c>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="P115" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B116" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C116" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D116" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E116" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1" t="inlineStr">
+        <is>
+          <t>Café pot Refraish 50g</t>
+        </is>
+      </c>
+      <c r="J116" s="1" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="K116" s="1" t="n">
+        <v>563750.0</v>
+      </c>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+      <c r="N116" s="1"/>
+      <c r="O116" s="1" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="P116" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B117" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C117" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D117" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E117" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1" t="inlineStr">
+        <is>
+          <t>Café stick Altimo 1,5gx09boites</t>
+        </is>
+      </c>
+      <c r="J117" s="1" t="n">
+        <v>16.222221</v>
+      </c>
+      <c r="K117" s="1" t="n">
+        <v>486666.66</v>
+      </c>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+      <c r="O117" s="1" t="n">
+        <v>116.0</v>
+      </c>
+      <c r="P117" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B118" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C118" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D118" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E118" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1" t="inlineStr">
+        <is>
+          <t>Café Altimo pot 50g x 24 pcs</t>
+        </is>
+      </c>
+      <c r="J118" s="1" t="n">
+        <v>19.166666</v>
+      </c>
+      <c r="K118" s="1" t="n">
+        <v>335416.66</v>
+      </c>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1" t="n">
+        <v>117.0</v>
+      </c>
+      <c r="P118" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B119" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C119" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D119" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E119" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1" t="inlineStr">
+        <is>
+          <t>Café Altimo pot 100g x 24 pcs</t>
+        </is>
+      </c>
+      <c r="J119" s="1" t="n">
+        <v>14.208333</v>
+      </c>
+      <c r="K119" s="1" t="n">
+        <v>475979.16</v>
+      </c>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+      <c r="N119" s="1"/>
+      <c r="O119" s="1" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="P119" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B120" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C120" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D120" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E120" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1" t="inlineStr">
+        <is>
+          <t>Café Altimo pot 200g x 12 pcs</t>
+        </is>
+      </c>
+      <c r="J120" s="1" t="n">
+        <v>12.833333</v>
+      </c>
+      <c r="K120" s="1" t="n">
+        <v>442750.0</v>
+      </c>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+      <c r="N120" s="1"/>
+      <c r="O120" s="1" t="n">
+        <v>119.0</v>
+      </c>
+      <c r="P120" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B121" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C121" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D121" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E121" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1" t="inlineStr">
+        <is>
+          <t>Kamlac évaporé 48x160g</t>
+        </is>
+      </c>
+      <c r="J121" s="1" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="K121" s="1" t="n">
+        <v>572250.0</v>
+      </c>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="O121" s="1" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="P121" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B122" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C122" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D122" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E122" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1" t="inlineStr">
+        <is>
+          <t>KamLac Lait concentré sucré 24x1kg</t>
+        </is>
+      </c>
+      <c r="J122" s="1" t="n">
+        <v>10.833333</v>
+      </c>
+      <c r="K122" s="1" t="n">
+        <v>260000.0</v>
+      </c>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+      <c r="O122" s="1" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="P122" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B123" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C123" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D123" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E123" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1" t="inlineStr">
+        <is>
+          <t>Lait Janus 18gx100</t>
+        </is>
+      </c>
+      <c r="J123" s="1" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="K123" s="1" t="n">
+        <v>57200.0</v>
+      </c>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+      <c r="O123" s="1" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="P123" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B124" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C124" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D124" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E124" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1" t="inlineStr">
+        <is>
+          <t>Lait Kamlac sachet 18gx100</t>
+        </is>
+      </c>
+      <c r="J124" s="1" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="K124" s="1" t="n">
+        <v>82500.0</v>
+      </c>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+      <c r="N124" s="1"/>
+      <c r="O124" s="1" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="P124" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B125" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C125" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D125" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E125" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1" t="inlineStr">
+        <is>
+          <t>Lait Janus 400gx10</t>
+        </is>
+      </c>
+      <c r="J125" s="1" t="n">
+        <v>52.2</v>
+      </c>
+      <c r="K125" s="1" t="n">
+        <v>639450.0</v>
+      </c>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1" t="n">
+        <v>124.0</v>
+      </c>
+      <c r="P125" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B126" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C126" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D126" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E126" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1" t="inlineStr">
+        <is>
+          <t>Jus Lido</t>
+        </is>
+      </c>
+      <c r="J126" s="1" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="K126" s="1" t="n">
+        <v>468000.0</v>
+      </c>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="P126" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B127" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C127" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D127" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E127" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat 3-en-1 30x120 pcs</t>
+        </is>
+      </c>
+      <c r="J127" s="1" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="K127" s="1" t="n">
+        <v>53300.0</v>
+      </c>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+      <c r="N127" s="1"/>
+      <c r="O127" s="1" t="n">
+        <v>126.0</v>
+      </c>
+      <c r="P127" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B128" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C128" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D128" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E128" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat transparent 200gx24pcs</t>
+        </is>
+      </c>
+      <c r="J128" s="1" t="n">
+        <v>0.41666666</v>
+      </c>
+      <c r="K128" s="1" t="n">
+        <v>5208.3335</v>
+      </c>
+      <c r="L128" s="1"/>
+      <c r="M128" s="1"/>
+      <c r="N128" s="1"/>
+      <c r="O128" s="1" t="n">
+        <v>127.0</v>
+      </c>
+      <c r="P128" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B129" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C129" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D129" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E129" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat transparent 400gx12pcs</t>
+        </is>
+      </c>
+      <c r="J129" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K129" s="1" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="L129" s="1"/>
+      <c r="M129" s="1"/>
+      <c r="N129" s="1"/>
+      <c r="O129" s="1" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="P129" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B130" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C130" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D130" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E130" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat jaune 200g x 24 pcs</t>
+        </is>
+      </c>
+      <c r="J130" s="1" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="K130" s="1" t="n">
+        <v>217000.0</v>
+      </c>
+      <c r="L130" s="1"/>
+      <c r="M130" s="1"/>
+      <c r="N130" s="1"/>
+      <c r="O130" s="1" t="n">
+        <v>129.0</v>
+      </c>
+      <c r="P130" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B131" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C131" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D131" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E131" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat jaune 400g x 12 pcs</t>
+        </is>
+      </c>
+      <c r="J131" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="K131" s="1" t="n">
+        <v>178250.0</v>
+      </c>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
+      <c r="O131" s="1" t="n">
+        <v>130.0</v>
+      </c>
+      <c r="P131" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B132" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C132" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D132" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E132" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Jaune 10gx60pcsx6 boites</t>
+        </is>
+      </c>
+      <c r="J132" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="K132" s="1" t="n">
+        <v>115000.0</v>
+      </c>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+      <c r="O132" s="1" t="n">
+        <v>131.0</v>
+      </c>
+      <c r="P132" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B133" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C133" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D133" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E133" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Orange 200g x24 pcs</t>
+        </is>
+      </c>
+      <c r="J133" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="K133" s="1" t="n">
+        <v>147000.0</v>
+      </c>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1" t="n">
+        <v>132.0</v>
+      </c>
+      <c r="P133" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B134" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C134" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D134" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E134" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Orange 400g x12 pcs</t>
+        </is>
+      </c>
+      <c r="J134" s="1" t="n">
+        <v>4.8333335</v>
+      </c>
+      <c r="K134" s="1" t="n">
+        <v>101500.0</v>
+      </c>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1" t="n">
+        <v>133.0</v>
+      </c>
+      <c r="P134" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>46027.0</v>
+      </c>
+      <c r="B135" s="1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C135" s="1" t="inlineStr">
+        <is>
+          <t>TATA 2</t>
+        </is>
+      </c>
+      <c r="D135" s="1" t="inlineStr">
+        <is>
+          <t>ALIOUNE BADARA (MANSOUR) SANE</t>
+        </is>
+      </c>
+      <c r="E135" s="1" t="inlineStr">
+        <is>
+          <t>Stock Lundi</t>
+        </is>
+      </c>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1" t="inlineStr">
+        <is>
+          <t>Chocolat Orange 10 g x 60 pcs x 6 boites</t>
+        </is>
+      </c>
+      <c r="J135" s="1" t="n">
+        <v>6.1666665</v>
+      </c>
+      <c r="K135" s="1" t="n">
+        <v>92500.0</v>
+      </c>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1" t="n">
+        <v>134.0</v>
+      </c>
+      <c r="P135" s="1" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Rapport du 07 Décembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -4462,10 +4462,10 @@
         </is>
       </c>
       <c r="J78" s="1" t="n">
-        <v>10.666667</v>
+        <v>11.111111</v>
       </c>
       <c r="K78" s="1" t="n">
-        <v>320000.0</v>
+        <v>333333.34</v>
       </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>

</xml_diff>

<commit_message>
Rapport du 08 Décembre 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -3296,10 +3296,10 @@
         </is>
       </c>
       <c r="J59" s="1" t="n">
-        <v>44.0</v>
+        <v>35.0</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>451000.0</v>
+        <v>358750.0</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -3344,10 +3344,10 @@
         </is>
       </c>
       <c r="J60" s="1" t="n">
-        <v>60.5</v>
+        <v>50.0</v>
       </c>
       <c r="K60" s="1" t="n">
-        <v>635250.0</v>
+        <v>525000.0</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -3944,10 +3944,10 @@
         </is>
       </c>
       <c r="J70" s="1" t="n">
-        <v>1.5</v>
+        <v>1.0</v>
       </c>
       <c r="K70" s="1" t="n">
-        <v>15375.0</v>
+        <v>10250.0</v>
       </c>
       <c r="L70" s="1" t="n">
         <v>3500.0</v>
@@ -4764,10 +4764,10 @@
         </is>
       </c>
       <c r="J84" s="1" t="n">
-        <v>4.0</v>
+        <v>4.111111</v>
       </c>
       <c r="K84" s="1" t="n">
-        <v>120000.0</v>
+        <v>123333.336</v>
       </c>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
@@ -5148,10 +5148,10 @@
         </is>
       </c>
       <c r="J92" s="1" t="n">
-        <v>44.2</v>
+        <v>41.2</v>
       </c>
       <c r="K92" s="1" t="n">
-        <v>541450.0</v>
+        <v>504700.0</v>
       </c>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
@@ -23506,10 +23506,10 @@
         </is>
       </c>
       <c r="J431" s="1" t="n">
-        <v>16.222221</v>
+        <v>11.222222</v>
       </c>
       <c r="K431" s="1" t="n">
-        <v>486666.66</v>
+        <v>336666.66</v>
       </c>
       <c r="L431" s="1"/>
       <c r="M431" s="1"/>
@@ -23890,10 +23890,10 @@
         </is>
       </c>
       <c r="J439" s="1" t="n">
-        <v>52.0</v>
+        <v>46.0</v>
       </c>
       <c r="K439" s="1" t="n">
-        <v>637000.0</v>
+        <v>563500.0</v>
       </c>
       <c r="L439" s="1"/>
       <c r="M439" s="1"/>

</xml_diff>

<commit_message>
Rapport du 09 Décembre 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -3980,10 +3980,10 @@
         </is>
       </c>
       <c r="J71" s="1" t="n">
-        <v>2.4444444</v>
+        <v>2.5555556</v>
       </c>
       <c r="K71" s="1" t="n">
-        <v>73333.336</v>
+        <v>76666.664</v>
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -4076,10 +4076,10 @@
         </is>
       </c>
       <c r="J73" s="1" t="n">
-        <v>7.7916665</v>
+        <v>7.8333335</v>
       </c>
       <c r="K73" s="1" t="n">
-        <v>261020.83</v>
+        <v>262416.66</v>
       </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -28278,10 +28278,10 @@
         </is>
       </c>
       <c r="J518" s="1" t="n">
-        <v>55.0</v>
+        <v>45.0</v>
       </c>
       <c r="K518" s="1" t="n">
-        <v>563750.0</v>
+        <v>461250.0</v>
       </c>
       <c r="L518" s="1"/>
       <c r="M518" s="1"/>
@@ -28950,10 +28950,10 @@
         </is>
       </c>
       <c r="J532" s="1" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
       <c r="K532" s="1" t="n">
-        <v>217000.0</v>
+        <v>170500.0</v>
       </c>
       <c r="L532" s="1"/>
       <c r="M532" s="1"/>

</xml_diff>

<commit_message>
Rapport du 10 Décembre 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -13018,14 +13018,14 @@
       <c r="H241" s="1"/>
       <c r="I241" s="1" t="inlineStr">
         <is>
-          <t>Café stick Refraish 1,5gx09boites</t>
+          <t>Café stick Altimo 1,5gx09boites</t>
         </is>
       </c>
       <c r="J241" s="1" t="n">
         <v>0.11111111</v>
       </c>
       <c r="K241" s="1" t="n">
-        <v>2888.889</v>
+        <v>3333.3333</v>
       </c>
       <c r="L241" s="1"/>
       <c r="M241" s="1"/>

</xml_diff>

<commit_message>
Rapport du 10 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5ACFD2-AD34-4067-9121-BA23387FC0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968F9C39-FBEC-4CB6-8F5A-252E61583513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A519" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L535" activeCellId="2" sqref="L568:M589 M567 L535:M566"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -836,7 +836,9 @@
       <c r="L4" s="1">
         <v>3000</v>
       </c>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1">
+        <v>10000</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1">
         <v>546</v>
@@ -3160,7 +3162,9 @@
       <c r="L63" s="1">
         <v>2000</v>
       </c>
-      <c r="M63" s="1"/>
+      <c r="M63" s="1">
+        <v>10000</v>
+      </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1">
         <v>605</v>
@@ -5010,7 +5014,9 @@
       <c r="L109" s="1">
         <v>2500</v>
       </c>
-      <c r="M109" s="1"/>
+      <c r="M109" s="1">
+        <v>10000</v>
+      </c>
       <c r="N109" s="1"/>
       <c r="O109" s="1">
         <v>477</v>
@@ -5894,7 +5900,9 @@
       <c r="L130" s="1">
         <v>2000</v>
       </c>
-      <c r="M130" s="1"/>
+      <c r="M130" s="1">
+        <v>10000</v>
+      </c>
       <c r="N130" s="1"/>
       <c r="O130" s="1">
         <v>498</v>

</xml_diff>

<commit_message>
Rapport du 14 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10209E7-E6AD-4DA3-8962-D4D8D5F064A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF410E5-6AC8-4D5C-81CB-A22F20701977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="277" yWindow="368" windowWidth="18923" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="277" yWindow="720" windowWidth="18923" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -674,25 +674,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8ABEBB62-27C1-4305-A526-9E1C0525FB85}" name="Tableau1" displayName="Tableau1" ref="A1:P965" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:P965" xr:uid="{8ABEBB62-27C1-4305-A526-9E1C0525FB85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21EF067F-8877-4EB0-945B-860D4D9C5474}" name="Tableau1" displayName="Tableau1" ref="A1:P965" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:P965" xr:uid="{21EF067F-8877-4EB0-945B-860D4D9C5474}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{B4D5C7B0-7FBF-4BC6-94AB-693AD2D9BC2D}" name="Date" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{9D8DBBE4-8424-4263-BD44-F0B58D7069CD}" name="Telephone_Team_Leader" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{25F5236B-81CA-476A-B734-7A43480D3FF2}" name="tata" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{B27EB97F-BABB-4EB3-9724-15A07EDCA0B2}" name="team_leader" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{297E0B5F-6269-4C8C-BEB4-762C7970CCB0}" name="Operation" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{7EA989DF-AE31-4995-8E9E-6BDCE339AE6B}" name="zone" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{F5004303-2D7B-41B2-AA27-4E705B7F1608}" name="Prenom_Nom_Promoteur" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{D5A0C893-2E53-4277-B1AA-E48870BF2B46}" name="Precisez" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{BE3AB52C-10CD-423E-8B09-2D8686AED546}" name="Produit" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{03121908-3509-46C4-ACA4-9C99C1EA8AA8}" name="Quantites_Cartons" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{D6F7869D-614E-4822-9EE2-0348B7FF51B7}" name="Montant" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{C0616017-C435-44EF-8ACB-666D2FC1A729}" name="Transport" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{46D93369-B306-45C4-B908-9861B96B580D}" name="Stationnement" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{E56C0691-D42F-4B98-B730-620FFB9397E3}" name="Commentaire" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{A9325F34-0904-4248-9C95-F97947F4E429}" name="ID_Produit" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{438B1DD5-034A-4631-8589-F42D87C27723}" name="Numero_semaine" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3E057202-6446-4E9A-9291-E26D07745BA6}" name="Date" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{A2478134-6B28-4470-BCC3-748C2CEFC99B}" name="Telephone_Team_Leader" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{2831EF2A-09A7-488B-9A87-0C90D059ED3E}" name="tata" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{4A94D8B0-E196-4154-8C81-B522700FC777}" name="team_leader" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{5CAF943E-AE51-42D4-A330-0DEDEC13A4DC}" name="Operation" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{DEAE7776-FDB8-4AFB-8A06-5087ECA85666}" name="zone" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{EEEBD602-A7D2-416A-B87C-6F91B2DFB760}" name="Prenom_Nom_Promoteur" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{8A7C8027-0E80-45D6-926D-5800434CF864}" name="Precisez" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{01D7A248-413C-4388-B31E-5457A65BE898}" name="Produit" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{3FBBC331-BC8F-4998-85C6-38937FB76EE8}" name="Quantites_Cartons" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{BAA19FA9-01E1-43CD-9A36-AD2323AD5C90}" name="Montant" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{A3CCD9C9-D973-425D-8FB8-9C7A3F905A42}" name="Transport" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{7FAB47AE-1ECE-4491-8A22-452883BCCCCF}" name="Stationnement" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{00541EAF-D5C3-437D-9AF7-8427EF607641}" name="Commentaire" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{30654B34-9494-4E51-9398-C6FB7798F68C}" name="ID_Produit" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{9F3C791C-48E9-4A0A-B3CB-7A2E6C81D1A8}" name="Numero_semaine" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P965"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I966" sqref="I966"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50:I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Rapport 16 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -4376,10 +4376,10 @@
         </is>
       </c>
       <c r="J78" s="1" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="K78" s="1" t="n">
-        <v>82500.0</v>
+        <v>75000.0</v>
       </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>

</xml_diff>

<commit_message>
Rapport du 16 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DE673F-565F-42E5-BFFC-5558462500CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC3DCA6-250D-44A4-A6C6-5B8CC2B82039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,6 +627,7 @@
         <name val="TIMES"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -661,7 +662,6 @@
         <name val="TIMES"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -677,25 +677,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA037F3A-B313-4C6F-B705-6F38394A38EA}" name="Tableau1" displayName="Tableau1" ref="A1:P1157" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA037F3A-B313-4C6F-B705-6F38394A38EA}" name="Tableau1" displayName="Tableau1" ref="A1:P1157" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:P1157" xr:uid="{BA037F3A-B313-4C6F-B705-6F38394A38EA}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{517179BB-8B63-48AF-9C1E-08E80399B747}" name="Date" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{5999FB53-13D4-40BE-8222-BEC6AA282352}" name="Telephone_Team_Leader" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{2E1F6EC3-859A-429E-88CD-6858908FCAF4}" name="tata" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{771D2E80-F44F-4834-AD3B-BA69AEFC8022}" name="team_leader" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{ADCC0D1C-3A49-44F1-9D60-FF9DB6D7AA30}" name="Operation" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{BB87D7F9-E0EE-41A9-9326-C286CC8C4EA7}" name="zone" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{3D69306F-8236-4947-A063-605ADA322A4E}" name="Prenom_Nom_Promoteur" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{8242FC02-BBFF-4ADA-BE50-C6F74A292879}" name="Precisez" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{5FD03EE2-0FFF-4CBA-A432-D9CB0A9CBF50}" name="Produit" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{385F18F4-A897-4A0C-9B3A-2F72996453DE}" name="Quantites_Cartons" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{DCB4C9C7-474F-4AC3-B63B-FA5E95AA99A2}" name="Montant" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{6B5B7070-CA62-463E-8C6E-190E952A1B6B}" name="Transport" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{3789E7D2-1A03-45E1-B242-68EC54651E48}" name="Stationnement" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{7FDF5791-E063-40DD-809E-628CD9B1A327}" name="Commentaire" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{CF8E6463-6731-4538-8A61-53F50C18C539}" name="ID_Produit" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{F537EB73-2445-43F8-952F-5CCF0AA0843A}" name="Numero_semaine" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{517179BB-8B63-48AF-9C1E-08E80399B747}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{5999FB53-13D4-40BE-8222-BEC6AA282352}" name="Telephone_Team_Leader" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{2E1F6EC3-859A-429E-88CD-6858908FCAF4}" name="tata" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{771D2E80-F44F-4834-AD3B-BA69AEFC8022}" name="team_leader" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{ADCC0D1C-3A49-44F1-9D60-FF9DB6D7AA30}" name="Operation" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{BB87D7F9-E0EE-41A9-9326-C286CC8C4EA7}" name="zone" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{3D69306F-8236-4947-A063-605ADA322A4E}" name="Prenom_Nom_Promoteur" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{8242FC02-BBFF-4ADA-BE50-C6F74A292879}" name="Precisez" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{5FD03EE2-0FFF-4CBA-A432-D9CB0A9CBF50}" name="Produit" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{385F18F4-A897-4A0C-9B3A-2F72996453DE}" name="Quantites_Cartons" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{DCB4C9C7-474F-4AC3-B63B-FA5E95AA99A2}" name="Montant" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{6B5B7070-CA62-463E-8C6E-190E952A1B6B}" name="Transport" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{3789E7D2-1A03-45E1-B242-68EC54651E48}" name="Stationnement" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{7FDF5791-E063-40DD-809E-628CD9B1A327}" name="Commentaire" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{CF8E6463-6731-4538-8A61-53F50C18C539}" name="ID_Produit" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{F537EB73-2445-43F8-952F-5CCF0AA0843A}" name="Numero_semaine" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
-      <selection activeCell="L19" activeCellId="1" sqref="L42:L70 L19:L40"/>
+    <sheetView tabSelected="1" topLeftCell="E65" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2705,7 +2705,9 @@
       <c r="L41" s="1">
         <v>3500</v>
       </c>
-      <c r="M41" s="1"/>
+      <c r="M41" s="1">
+        <v>10000</v>
+      </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1">
         <v>1108</v>
@@ -4183,10 +4185,10 @@
         <v>75</v>
       </c>
       <c r="J77" s="1">
-        <v>0.29166666000000002</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="K77" s="1">
-        <v>2916.6667000000002</v>
+        <v>3333.3333333333298</v>
       </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>

</xml_diff>

<commit_message>
Rapport du 22 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -206,10 +206,10 @@
         </is>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.9791667</v>
+        <v>1.0</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>10281.25</v>
+        <v>10500.0</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>2500.0</v>
@@ -1908,10 +1908,10 @@
         </is>
       </c>
       <c r="J32" s="1" t="n">
-        <v>6.0833335</v>
+        <v>6.1666665</v>
       </c>
       <c r="K32" s="1" t="n">
-        <v>203791.67</v>
+        <v>206583.33</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -3212,10 +3212,10 @@
         </is>
       </c>
       <c r="J59" s="1" t="n">
-        <v>6.7083335</v>
+        <v>6.6666665</v>
       </c>
       <c r="K59" s="1" t="n">
-        <v>224729.17</v>
+        <v>223333.33</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -4768,10 +4768,10 @@
         </is>
       </c>
       <c r="J88" s="1" t="n">
-        <v>0.16666667</v>
+        <v>0.5</v>
       </c>
       <c r="K88" s="1" t="n">
-        <v>1666.6666</v>
+        <v>5000.0</v>
       </c>
       <c r="L88" s="1" t="n">
         <v>3000.0</v>

</xml_diff>

<commit_message>
Rapport du 23 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -342,10 +342,10 @@
         </is>
       </c>
       <c r="J5" s="1" t="n">
-        <v>17.9</v>
+        <v>17.8</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>134250.0</v>
+        <v>133500.0</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2882,10 +2882,10 @@
         </is>
       </c>
       <c r="J51" s="1" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K51" s="1" t="n">
-        <v>10500.0</v>
+        <v>21000.0</v>
       </c>
       <c r="L51" s="1" t="n">
         <v>2500.0</v>
@@ -4962,10 +4962,10 @@
         </is>
       </c>
       <c r="J87" s="1" t="n">
-        <v>6.0416665</v>
+        <v>6.125</v>
       </c>
       <c r="K87" s="1" t="n">
-        <v>202395.83</v>
+        <v>205187.5</v>
       </c>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>

</xml_diff>

<commit_message>
Rapport du 24 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.9791667</v>
+        <v>1.0</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>10281.25</v>
+        <v>10500.0</v>
       </c>
       <c r="L11" s="1" t="n">
         <v>1500.0</v>

</xml_diff>

<commit_message>
Rapport du 27 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADCD97F-0D05-46CF-A5EC-D2F83E695A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE5B8C7-E5FA-409C-8C31-A40DF7E5F6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="277" yWindow="720" windowWidth="18923" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -385,6 +385,12 @@
     <font>
       <sz val="11"/>
       <name val="TIMES"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -747,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1838"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H46" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53:L93"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -826,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
@@ -870,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
@@ -912,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>17</v>
@@ -954,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -996,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
@@ -1038,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1080,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
@@ -1122,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -1164,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -1206,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -1248,7 +1254,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1290,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
@@ -1332,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
@@ -1374,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -1416,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -1458,7 +1464,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -1500,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -1542,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1584,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
@@ -1626,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -1668,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1710,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1752,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1794,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1836,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1878,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1920,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1962,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
@@ -2004,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -2046,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -77411,6 +77417,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rapport du 28 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179EF268-0CD1-4FCD-A65C-3B36DCB50E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC869127-5246-40AB-99A9-C06DE48227B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1930"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56:C83"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3032,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>55</v>
@@ -3076,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>55</v>
@@ -3118,7 +3118,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>55</v>
@@ -3160,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>55</v>
@@ -3202,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>55</v>
@@ -3244,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>55</v>
@@ -3286,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>55</v>
@@ -3328,7 +3328,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>55</v>
@@ -3370,7 +3370,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>55</v>
@@ -3412,7 +3412,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>55</v>
@@ -3454,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>55</v>
@@ -3496,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>55</v>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>55</v>
@@ -3580,7 +3580,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>55</v>
@@ -3622,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>55</v>
@@ -3664,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>55</v>
@@ -3706,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>55</v>
@@ -3748,7 +3748,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>55</v>
@@ -3790,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>55</v>
@@ -3832,7 +3832,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>55</v>
@@ -3874,7 +3874,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>55</v>
@@ -3916,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>55</v>
@@ -3958,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>55</v>
@@ -4000,7 +4000,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>55</v>
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>55</v>
@@ -4084,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>55</v>
@@ -4126,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>55</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Rapport du 29 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E844E2-9E7C-40EE-9A73-A53AC0D5C8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F08BA9-65BA-4E65-8B66-33BCAEAF6EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65:C80"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3404,7 +3404,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>64</v>
@@ -3448,7 +3448,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>64</v>
@@ -3490,7 +3490,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>64</v>
@@ -3532,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>64</v>
@@ -3574,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>64</v>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>64</v>
@@ -3658,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>64</v>
@@ -3700,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>64</v>
@@ -3742,7 +3742,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>64</v>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>64</v>
@@ -3826,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>64</v>
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>64</v>
@@ -3910,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>64</v>
@@ -3952,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>64</v>
@@ -3994,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>64</v>
@@ -4036,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Rapport du 30 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A17DD1-09F2-4AE0-9B0F-1D0B8CAACC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2449A4-47ED-4232-8A64-E26556054150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="277" yWindow="720" windowWidth="18923" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2092"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:C85"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>64</v>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>64</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>64</v>
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>64</v>
@@ -3247,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>64</v>
@@ -3289,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>64</v>
@@ -3331,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>64</v>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>64</v>
@@ -3415,7 +3415,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>64</v>
@@ -3457,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>64</v>
@@ -3499,7 +3499,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>64</v>
@@ -3541,7 +3541,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>64</v>
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>64</v>
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>64</v>
@@ -3667,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>64</v>
@@ -3709,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>64</v>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>64</v>
@@ -3793,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>64</v>
@@ -3835,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>64</v>
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>64</v>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>64</v>
@@ -3961,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>64</v>
@@ -4003,7 +4003,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>64</v>
@@ -4045,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>64</v>
@@ -4087,7 +4087,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>64</v>
@@ -4129,7 +4129,7 @@
         <v>0</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>64</v>
@@ -4171,7 +4171,7 @@
         <v>0</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>64</v>
@@ -4213,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>64</v>
@@ -4255,7 +4255,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Rapport du 31 Janvier 2026
</commit_message>
<xml_diff>
--- a/Donnees_Promoteurs.xlsx
+++ b/Donnees_Promoteurs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF86CE2-033C-4BBD-887D-8FC6C6D207AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDDCA3E-F055-4267-AF06-CA9D242AFD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="C51" sqref="C51:C77"/>
     </sheetView>
   </sheetViews>
@@ -776,7 +776,7 @@
     <col min="3" max="3" width="8.59765625" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" customWidth="1"/>
     <col min="5" max="5" width="16.53125" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.3984375" customWidth="1"/>
     <col min="9" max="9" width="41.46484375" customWidth="1"/>
     <col min="10" max="10" width="13.9296875" customWidth="1"/>
@@ -2832,7 +2832,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>57</v>
@@ -2876,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>57</v>
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>57</v>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>57</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>57</v>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>57</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>57</v>
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>57</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>57</v>
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>57</v>
@@ -3254,7 +3254,7 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>57</v>
@@ -3296,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>57</v>
@@ -3338,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>57</v>
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>57</v>
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>57</v>
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>57</v>
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>57</v>
@@ -3548,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>57</v>
@@ -3590,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>57</v>
@@ -3632,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>57</v>
@@ -3674,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>57</v>
@@ -3716,7 +3716,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>57</v>
@@ -3758,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>57</v>
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>57</v>
@@ -3842,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>57</v>
@@ -3884,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>57</v>
@@ -3926,7 +3926,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>57</v>
@@ -4682,9 +4682,7 @@
       <c r="K96" s="1">
         <v>40000</v>
       </c>
-      <c r="L96" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L96" s="1"/>
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1">
@@ -4726,9 +4724,7 @@
       <c r="K97" s="1">
         <v>10500</v>
       </c>
-      <c r="L97" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L97" s="1"/>
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1">
@@ -4770,9 +4766,7 @@
       <c r="K98" s="1">
         <v>8750</v>
       </c>
-      <c r="L98" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L98" s="1"/>
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1">
@@ -4814,9 +4808,7 @@
       <c r="K99" s="1">
         <v>10500</v>
       </c>
-      <c r="L99" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1">
@@ -4858,9 +4850,7 @@
       <c r="K100" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L100" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1">
@@ -4902,9 +4892,7 @@
       <c r="K101" s="1">
         <v>10500</v>
       </c>
-      <c r="L101" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1">
@@ -4946,9 +4934,7 @@
       <c r="K102" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L102" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1">
@@ -4990,9 +4976,7 @@
       <c r="K103" s="1">
         <v>10500</v>
       </c>
-      <c r="L103" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L103" s="1"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1">
@@ -5034,9 +5018,7 @@
       <c r="K104" s="1">
         <v>10000</v>
       </c>
-      <c r="L104" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L104" s="1"/>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1">
@@ -5078,9 +5060,7 @@
       <c r="K105" s="1">
         <v>5250</v>
       </c>
-      <c r="L105" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1">
@@ -5122,9 +5102,7 @@
       <c r="K106" s="1">
         <v>8750</v>
       </c>
-      <c r="L106" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1">
@@ -5166,9 +5144,7 @@
       <c r="K107" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L107" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1">
@@ -5210,9 +5186,7 @@
       <c r="K108" s="1">
         <v>10500</v>
       </c>
-      <c r="L108" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1">
@@ -5254,9 +5228,7 @@
       <c r="K109" s="1">
         <v>3600</v>
       </c>
-      <c r="L109" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L109" s="1"/>
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1">
@@ -5298,9 +5270,7 @@
       <c r="K110" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L110" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L110" s="1"/>
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1">
@@ -5342,9 +5312,7 @@
       <c r="K111" s="1">
         <v>15750</v>
       </c>
-      <c r="L111" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L111" s="1"/>
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1">
@@ -5386,9 +5354,7 @@
       <c r="K112" s="1">
         <v>1875</v>
       </c>
-      <c r="L112" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L112" s="1"/>
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1">
@@ -5430,9 +5396,7 @@
       <c r="K113" s="1">
         <v>10000</v>
       </c>
-      <c r="L113" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L113" s="1"/>
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1">
@@ -5474,9 +5438,7 @@
       <c r="K114" s="1">
         <v>33600</v>
       </c>
-      <c r="L114" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L114" s="1"/>
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
       <c r="O114" s="1">
@@ -5520,9 +5482,7 @@
       <c r="K115" s="1">
         <v>24000</v>
       </c>
-      <c r="L115" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L115" s="1"/>
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1">
@@ -5566,9 +5526,7 @@
       <c r="K116" s="1">
         <v>11400</v>
       </c>
-      <c r="L116" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L116" s="1"/>
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1">
@@ -5612,9 +5570,7 @@
       <c r="K117" s="1">
         <v>7500</v>
       </c>
-      <c r="L117" s="1">
-        <v>5000</v>
-      </c>
+      <c r="L117" s="1"/>
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1">
@@ -6322,9 +6278,7 @@
       <c r="K134" s="1">
         <v>10500</v>
       </c>
-      <c r="L134" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L134" s="1"/>
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1">
@@ -6366,9 +6320,7 @@
       <c r="K135" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L135" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L135" s="1"/>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1">
@@ -6410,9 +6362,7 @@
       <c r="K136" s="1">
         <v>10500</v>
       </c>
-      <c r="L136" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L136" s="1"/>
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
       <c r="O136" s="1">
@@ -6454,9 +6404,7 @@
       <c r="K137" s="1">
         <v>10500</v>
       </c>
-      <c r="L137" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L137" s="1"/>
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
       <c r="O137" s="1">
@@ -6498,9 +6446,7 @@
       <c r="K138" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L138" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L138" s="1"/>
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
       <c r="O138" s="1">
@@ -6542,9 +6488,7 @@
       <c r="K139" s="1">
         <v>21000</v>
       </c>
-      <c r="L139" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L139" s="1"/>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1">
@@ -6586,9 +6530,7 @@
       <c r="K140" s="1">
         <v>10000</v>
       </c>
-      <c r="L140" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L140" s="1"/>
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
       <c r="O140" s="1">
@@ -6630,9 +6572,7 @@
       <c r="K141" s="1">
         <v>3750</v>
       </c>
-      <c r="L141" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L141" s="1"/>
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
       <c r="O141" s="1">
@@ -6674,9 +6614,7 @@
       <c r="K142" s="1">
         <v>3750</v>
       </c>
-      <c r="L142" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L142" s="1"/>
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1">
@@ -6718,9 +6656,7 @@
       <c r="K143" s="1">
         <v>26250</v>
       </c>
-      <c r="L143" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L143" s="1"/>
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1">
@@ -6762,9 +6698,7 @@
       <c r="K144" s="1">
         <v>23333.333999999999</v>
       </c>
-      <c r="L144" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L144" s="1"/>
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
       <c r="O144" s="1">
@@ -6806,9 +6740,7 @@
       <c r="K145" s="1">
         <v>1100</v>
       </c>
-      <c r="L145" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L145" s="1"/>
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1">
@@ -6850,9 +6782,7 @@
       <c r="K146" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L146" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L146" s="1"/>
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
       <c r="O146" s="1">
@@ -6894,9 +6824,7 @@
       <c r="K147" s="1">
         <v>15750</v>
       </c>
-      <c r="L147" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L147" s="1"/>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1">
@@ -6938,9 +6866,7 @@
       <c r="K148" s="1">
         <v>26250</v>
       </c>
-      <c r="L148" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L148" s="1"/>
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1">
@@ -6982,9 +6908,7 @@
       <c r="K149" s="1">
         <v>13333.333000000001</v>
       </c>
-      <c r="L149" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L149" s="1"/>
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1">
@@ -7026,9 +6950,7 @@
       <c r="K150" s="1">
         <v>12000</v>
       </c>
-      <c r="L150" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L150" s="1"/>
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1">
@@ -7070,9 +6992,7 @@
       <c r="K151" s="1">
         <v>10500</v>
       </c>
-      <c r="L151" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L151" s="1"/>
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1">
@@ -7114,9 +7034,7 @@
       <c r="K152" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L152" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L152" s="1"/>
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1">
@@ -7158,9 +7076,7 @@
       <c r="K153" s="1">
         <v>1100</v>
       </c>
-      <c r="L153" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L153" s="1"/>
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1">
@@ -7202,9 +7118,7 @@
       <c r="K154" s="1">
         <v>10500</v>
       </c>
-      <c r="L154" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L154" s="1"/>
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1">
@@ -7246,9 +7160,7 @@
       <c r="K155" s="1">
         <v>10000</v>
       </c>
-      <c r="L155" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L155" s="1"/>
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1">
@@ -7290,9 +7202,7 @@
       <c r="K156" s="1">
         <v>10500</v>
       </c>
-      <c r="L156" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L156" s="1"/>
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1">
@@ -7334,9 +7244,7 @@
       <c r="K157" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L157" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L157" s="1"/>
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1">
@@ -7378,9 +7286,7 @@
       <c r="K158" s="1">
         <v>5250</v>
       </c>
-      <c r="L158" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L158" s="1"/>
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1">
@@ -7422,9 +7328,7 @@
       <c r="K159" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L159" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L159" s="1"/>
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1">
@@ -7466,9 +7370,7 @@
       <c r="K160" s="1">
         <v>1100</v>
       </c>
-      <c r="L160" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L160" s="1"/>
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1">
@@ -7510,9 +7412,7 @@
       <c r="K161" s="1">
         <v>5250</v>
       </c>
-      <c r="L161" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L161" s="1"/>
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1">
@@ -8740,9 +8640,7 @@
       <c r="K192" s="1">
         <v>10500</v>
       </c>
-      <c r="L192" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L192" s="1"/>
       <c r="M192" s="1"/>
       <c r="N192" s="1"/>
       <c r="O192" s="1">
@@ -8784,9 +8682,7 @@
       <c r="K193" s="1">
         <v>10000</v>
       </c>
-      <c r="L193" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L193" s="1"/>
       <c r="M193" s="1"/>
       <c r="N193" s="1"/>
       <c r="O193" s="1">
@@ -8828,9 +8724,7 @@
       <c r="K194" s="1">
         <v>1875</v>
       </c>
-      <c r="L194" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L194" s="1"/>
       <c r="M194" s="1"/>
       <c r="N194" s="1"/>
       <c r="O194" s="1">
@@ -8872,9 +8766,7 @@
       <c r="K195" s="1">
         <v>750</v>
       </c>
-      <c r="L195" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L195" s="1"/>
       <c r="M195" s="1"/>
       <c r="N195" s="1"/>
       <c r="O195" s="1">
@@ -8916,9 +8808,7 @@
       <c r="K196" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L196" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L196" s="1"/>
       <c r="M196" s="1"/>
       <c r="N196" s="1"/>
       <c r="O196" s="1">
@@ -8960,9 +8850,7 @@
       <c r="K197" s="1">
         <v>6000</v>
       </c>
-      <c r="L197" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L197" s="1"/>
       <c r="M197" s="1"/>
       <c r="N197" s="1"/>
       <c r="O197" s="1">
@@ -9004,9 +8892,7 @@
       <c r="K198" s="1">
         <v>12000</v>
       </c>
-      <c r="L198" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L198" s="1"/>
       <c r="M198" s="1"/>
       <c r="N198" s="1"/>
       <c r="O198" s="1">
@@ -9048,9 +8934,7 @@
       <c r="K199" s="1">
         <v>5250</v>
       </c>
-      <c r="L199" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L199" s="1"/>
       <c r="M199" s="1"/>
       <c r="N199" s="1"/>
       <c r="O199" s="1">
@@ -9092,9 +8976,7 @@
       <c r="K200" s="1">
         <v>6000</v>
       </c>
-      <c r="L200" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L200" s="1"/>
       <c r="M200" s="1"/>
       <c r="N200" s="1"/>
       <c r="O200" s="1">
@@ -9136,9 +9018,7 @@
       <c r="K201" s="1">
         <v>1100</v>
       </c>
-      <c r="L201" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L201" s="1"/>
       <c r="M201" s="1"/>
       <c r="N201" s="1"/>
       <c r="O201" s="1">
@@ -9180,9 +9060,7 @@
       <c r="K202" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L202" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L202" s="1"/>
       <c r="M202" s="1"/>
       <c r="N202" s="1"/>
       <c r="O202" s="1">
@@ -9224,9 +9102,7 @@
       <c r="K203" s="1">
         <v>21000</v>
       </c>
-      <c r="L203" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L203" s="1"/>
       <c r="M203" s="1"/>
       <c r="N203" s="1"/>
       <c r="O203" s="1">
@@ -9268,9 +9144,7 @@
       <c r="K204" s="1">
         <v>4187.5</v>
       </c>
-      <c r="L204" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L204" s="1"/>
       <c r="M204" s="1"/>
       <c r="N204" s="1"/>
       <c r="O204" s="1">
@@ -9312,9 +9186,7 @@
       <c r="K205" s="1">
         <v>1100</v>
       </c>
-      <c r="L205" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L205" s="1"/>
       <c r="M205" s="1"/>
       <c r="N205" s="1"/>
       <c r="O205" s="1">
@@ -9356,9 +9228,7 @@
       <c r="K206" s="1">
         <v>1100</v>
       </c>
-      <c r="L206" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L206" s="1"/>
       <c r="M206" s="1"/>
       <c r="N206" s="1"/>
       <c r="O206" s="1">
@@ -9400,9 +9270,7 @@
       <c r="K207" s="1">
         <v>10500</v>
       </c>
-      <c r="L207" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L207" s="1"/>
       <c r="M207" s="1"/>
       <c r="N207" s="1"/>
       <c r="O207" s="1">
@@ -9444,9 +9312,7 @@
       <c r="K208" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L208" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L208" s="1"/>
       <c r="M208" s="1"/>
       <c r="N208" s="1"/>
       <c r="O208" s="1">
@@ -9488,9 +9354,7 @@
       <c r="K209" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L209" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L209" s="1"/>
       <c r="M209" s="1"/>
       <c r="N209" s="1"/>
       <c r="O209" s="1">
@@ -9532,9 +9396,7 @@
       <c r="K210" s="1">
         <v>16750</v>
       </c>
-      <c r="L210" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L210" s="1"/>
       <c r="M210" s="1"/>
       <c r="N210" s="1"/>
       <c r="O210" s="1">
@@ -9576,9 +9438,7 @@
       <c r="K211" s="1">
         <v>12000</v>
       </c>
-      <c r="L211" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L211" s="1"/>
       <c r="M211" s="1"/>
       <c r="N211" s="1"/>
       <c r="O211" s="1">
@@ -9620,9 +9480,7 @@
       <c r="K212" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L212" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L212" s="1"/>
       <c r="M212" s="1"/>
       <c r="N212" s="1"/>
       <c r="O212" s="1">
@@ -9664,9 +9522,7 @@
       <c r="K213" s="1">
         <v>15750</v>
       </c>
-      <c r="L213" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L213" s="1"/>
       <c r="M213" s="1"/>
       <c r="N213" s="1"/>
       <c r="O213" s="1">
@@ -9708,9 +9564,7 @@
       <c r="K214" s="1">
         <v>16750</v>
       </c>
-      <c r="L214" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L214" s="1"/>
       <c r="M214" s="1"/>
       <c r="N214" s="1"/>
       <c r="O214" s="1">
@@ -9752,9 +9606,7 @@
       <c r="K215" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L215" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L215" s="1"/>
       <c r="M215" s="1"/>
       <c r="N215" s="1"/>
       <c r="O215" s="1">
@@ -9796,9 +9648,7 @@
       <c r="K216" s="1">
         <v>10000</v>
       </c>
-      <c r="L216" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L216" s="1"/>
       <c r="M216" s="1"/>
       <c r="N216" s="1"/>
       <c r="O216" s="1">
@@ -9840,9 +9690,7 @@
       <c r="K217" s="1">
         <v>5250</v>
       </c>
-      <c r="L217" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L217" s="1"/>
       <c r="M217" s="1"/>
       <c r="N217" s="1"/>
       <c r="O217" s="1">
@@ -9884,9 +9732,7 @@
       <c r="K218" s="1">
         <v>16750</v>
       </c>
-      <c r="L218" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L218" s="1"/>
       <c r="M218" s="1"/>
       <c r="N218" s="1"/>
       <c r="O218" s="1">
@@ -9928,9 +9774,7 @@
       <c r="K219" s="1">
         <v>21000</v>
       </c>
-      <c r="L219" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L219" s="1"/>
       <c r="M219" s="1"/>
       <c r="N219" s="1"/>
       <c r="O219" s="1">
@@ -9972,9 +9816,7 @@
       <c r="K220" s="1">
         <v>6000</v>
       </c>
-      <c r="L220" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L220" s="1"/>
       <c r="M220" s="1"/>
       <c r="N220" s="1"/>
       <c r="O220" s="1">
@@ -10016,9 +9858,7 @@
       <c r="K221" s="1">
         <v>48000</v>
       </c>
-      <c r="L221" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L221" s="1"/>
       <c r="M221" s="1"/>
       <c r="N221" s="1"/>
       <c r="O221" s="1">
@@ -10062,9 +9902,7 @@
       <c r="K222" s="1">
         <v>24000</v>
       </c>
-      <c r="L222" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L222" s="1"/>
       <c r="M222" s="1"/>
       <c r="N222" s="1"/>
       <c r="O222" s="1">
@@ -10108,9 +9946,7 @@
       <c r="K223" s="1">
         <v>36000</v>
       </c>
-      <c r="L223" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L223" s="1"/>
       <c r="M223" s="1"/>
       <c r="N223" s="1"/>
       <c r="O223" s="1">
@@ -10154,9 +9990,7 @@
       <c r="K224" s="1">
         <v>7500</v>
       </c>
-      <c r="L224" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L224" s="1"/>
       <c r="M224" s="1"/>
       <c r="N224" s="1"/>
       <c r="O224" s="1">
@@ -10242,9 +10076,7 @@
       <c r="K226" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L226" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L226" s="1"/>
       <c r="M226" s="1"/>
       <c r="N226" s="1"/>
       <c r="O226" s="1">
@@ -10286,9 +10118,7 @@
       <c r="K227" s="1">
         <v>12000</v>
       </c>
-      <c r="L227" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L227" s="1"/>
       <c r="M227" s="1"/>
       <c r="N227" s="1"/>
       <c r="O227" s="1">
@@ -10330,9 +10160,7 @@
       <c r="K228" s="1">
         <v>23333.333999999999</v>
       </c>
-      <c r="L228" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L228" s="1"/>
       <c r="M228" s="1"/>
       <c r="N228" s="1"/>
       <c r="O228" s="1">
@@ -10374,9 +10202,7 @@
       <c r="K229" s="1">
         <v>1100</v>
       </c>
-      <c r="L229" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L229" s="1"/>
       <c r="M229" s="1"/>
       <c r="N229" s="1"/>
       <c r="O229" s="1">
@@ -10418,9 +10244,7 @@
       <c r="K230" s="1">
         <v>40000</v>
       </c>
-      <c r="L230" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L230" s="1"/>
       <c r="M230" s="1"/>
       <c r="N230" s="1"/>
       <c r="O230" s="1">
@@ -10462,9 +10286,7 @@
       <c r="K231" s="1">
         <v>1100</v>
       </c>
-      <c r="L231" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L231" s="1"/>
       <c r="M231" s="1"/>
       <c r="N231" s="1"/>
       <c r="O231" s="1">
@@ -10506,9 +10328,7 @@
       <c r="K232" s="1">
         <v>21000</v>
       </c>
-      <c r="L232" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L232" s="1"/>
       <c r="M232" s="1"/>
       <c r="N232" s="1"/>
       <c r="O232" s="1">
@@ -10550,9 +10370,7 @@
       <c r="K233" s="1">
         <v>20000</v>
       </c>
-      <c r="L233" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L233" s="1"/>
       <c r="M233" s="1"/>
       <c r="N233" s="1"/>
       <c r="O233" s="1">
@@ -10594,9 +10412,7 @@
       <c r="K234" s="1">
         <v>10500</v>
       </c>
-      <c r="L234" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L234" s="1"/>
       <c r="M234" s="1"/>
       <c r="N234" s="1"/>
       <c r="O234" s="1">
@@ -10638,9 +10454,7 @@
       <c r="K235" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L235" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L235" s="1"/>
       <c r="M235" s="1"/>
       <c r="N235" s="1"/>
       <c r="O235" s="1">
@@ -10682,9 +10496,7 @@
       <c r="K236" s="1">
         <v>31500</v>
       </c>
-      <c r="L236" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L236" s="1"/>
       <c r="M236" s="1"/>
       <c r="N236" s="1"/>
       <c r="O236" s="1">
@@ -10726,9 +10538,7 @@
       <c r="K237" s="1">
         <v>33333.332000000002</v>
       </c>
-      <c r="L237" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L237" s="1"/>
       <c r="M237" s="1"/>
       <c r="N237" s="1"/>
       <c r="O237" s="1">
@@ -10770,9 +10580,7 @@
       <c r="K238" s="1">
         <v>15750</v>
       </c>
-      <c r="L238" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L238" s="1"/>
       <c r="M238" s="1"/>
       <c r="N238" s="1"/>
       <c r="O238" s="1">
@@ -10814,9 +10622,7 @@
       <c r="K239" s="1">
         <v>37500</v>
       </c>
-      <c r="L239" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L239" s="1"/>
       <c r="M239" s="1"/>
       <c r="N239" s="1"/>
       <c r="O239" s="1">
@@ -10858,9 +10664,7 @@
       <c r="K240" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L240" s="1">
-        <v>2700</v>
-      </c>
+      <c r="L240" s="1"/>
       <c r="M240" s="1"/>
       <c r="N240" s="1"/>
       <c r="O240" s="1">
@@ -11668,9 +11472,7 @@
       <c r="K261" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L261" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L261" s="1"/>
       <c r="M261" s="1"/>
       <c r="N261" s="1"/>
       <c r="O261" s="1">
@@ -11712,9 +11514,7 @@
       <c r="K262" s="1">
         <v>1100</v>
       </c>
-      <c r="L262" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L262" s="1"/>
       <c r="M262" s="1"/>
       <c r="N262" s="1"/>
       <c r="O262" s="1">
@@ -11756,9 +11556,7 @@
       <c r="K263" s="1">
         <v>5250</v>
       </c>
-      <c r="L263" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L263" s="1"/>
       <c r="M263" s="1"/>
       <c r="N263" s="1"/>
       <c r="O263" s="1">
@@ -11800,9 +11598,7 @@
       <c r="K264" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L264" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L264" s="1"/>
       <c r="M264" s="1"/>
       <c r="N264" s="1"/>
       <c r="O264" s="1">
@@ -11844,9 +11640,7 @@
       <c r="K265" s="1">
         <v>1100</v>
       </c>
-      <c r="L265" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L265" s="1"/>
       <c r="M265" s="1"/>
       <c r="N265" s="1"/>
       <c r="O265" s="1">
@@ -11888,9 +11682,7 @@
       <c r="K266" s="1">
         <v>5250</v>
       </c>
-      <c r="L266" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L266" s="1"/>
       <c r="M266" s="1"/>
       <c r="N266" s="1"/>
       <c r="O266" s="1">
@@ -11932,9 +11724,7 @@
       <c r="K267" s="1">
         <v>8750</v>
       </c>
-      <c r="L267" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L267" s="1"/>
       <c r="M267" s="1"/>
       <c r="N267" s="1"/>
       <c r="O267" s="1">
@@ -11976,9 +11766,7 @@
       <c r="K268" s="1">
         <v>15000</v>
       </c>
-      <c r="L268" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L268" s="1"/>
       <c r="M268" s="1"/>
       <c r="N268" s="1"/>
       <c r="O268" s="1">
@@ -12020,9 +11808,7 @@
       <c r="K269" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L269" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L269" s="1"/>
       <c r="M269" s="1"/>
       <c r="N269" s="1"/>
       <c r="O269" s="1">
@@ -12064,9 +11850,7 @@
       <c r="K270" s="1">
         <v>16750</v>
       </c>
-      <c r="L270" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L270" s="1"/>
       <c r="M270" s="1"/>
       <c r="N270" s="1"/>
       <c r="O270" s="1">
@@ -12108,9 +11892,7 @@
       <c r="K271" s="1">
         <v>10500</v>
       </c>
-      <c r="L271" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L271" s="1"/>
       <c r="M271" s="1"/>
       <c r="N271" s="1"/>
       <c r="O271" s="1">
@@ -12152,9 +11934,7 @@
       <c r="K272" s="1">
         <v>1100</v>
       </c>
-      <c r="L272" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L272" s="1"/>
       <c r="M272" s="1"/>
       <c r="N272" s="1"/>
       <c r="O272" s="1">
@@ -12196,9 +11976,7 @@
       <c r="K273" s="1">
         <v>6000</v>
       </c>
-      <c r="L273" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L273" s="1"/>
       <c r="M273" s="1"/>
       <c r="N273" s="1"/>
       <c r="O273" s="1">
@@ -12240,9 +12018,7 @@
       <c r="K274" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L274" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L274" s="1"/>
       <c r="M274" s="1"/>
       <c r="N274" s="1"/>
       <c r="O274" s="1">
@@ -12284,9 +12060,7 @@
       <c r="K275" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L275" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L275" s="1"/>
       <c r="M275" s="1"/>
       <c r="N275" s="1"/>
       <c r="O275" s="1">
@@ -12328,9 +12102,7 @@
       <c r="K276" s="1">
         <v>1100</v>
       </c>
-      <c r="L276" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L276" s="1"/>
       <c r="M276" s="1"/>
       <c r="N276" s="1"/>
       <c r="O276" s="1">
@@ -12372,9 +12144,7 @@
       <c r="K277" s="1">
         <v>6000</v>
       </c>
-      <c r="L277" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L277" s="1"/>
       <c r="M277" s="1"/>
       <c r="N277" s="1"/>
       <c r="O277" s="1">
@@ -12416,9 +12186,7 @@
       <c r="K278" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L278" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L278" s="1"/>
       <c r="M278" s="1"/>
       <c r="N278" s="1"/>
       <c r="O278" s="1">
@@ -12460,9 +12228,7 @@
       <c r="K279" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L279" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L279" s="1"/>
       <c r="M279" s="1"/>
       <c r="N279" s="1"/>
       <c r="O279" s="1">
@@ -12504,9 +12270,7 @@
       <c r="K280" s="1">
         <v>16750</v>
       </c>
-      <c r="L280" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L280" s="1"/>
       <c r="M280" s="1"/>
       <c r="N280" s="1"/>
       <c r="O280" s="1">
@@ -12548,9 +12312,7 @@
       <c r="K281" s="1">
         <v>8750</v>
       </c>
-      <c r="L281" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L281" s="1"/>
       <c r="M281" s="1"/>
       <c r="N281" s="1"/>
       <c r="O281" s="1">
@@ -12592,9 +12354,7 @@
       <c r="K282" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L282" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L282" s="1"/>
       <c r="M282" s="1"/>
       <c r="N282" s="1"/>
       <c r="O282" s="1">
@@ -12636,9 +12396,7 @@
       <c r="K283" s="1">
         <v>10000</v>
       </c>
-      <c r="L283" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L283" s="1"/>
       <c r="M283" s="1"/>
       <c r="N283" s="1"/>
       <c r="O283" s="1">
@@ -12680,9 +12438,7 @@
       <c r="K284" s="1">
         <v>8750</v>
       </c>
-      <c r="L284" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L284" s="1"/>
       <c r="M284" s="1"/>
       <c r="N284" s="1"/>
       <c r="O284" s="1">
@@ -12724,9 +12480,7 @@
       <c r="K285" s="1">
         <v>20000</v>
       </c>
-      <c r="L285" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L285" s="1"/>
       <c r="M285" s="1"/>
       <c r="N285" s="1"/>
       <c r="O285" s="1">
@@ -12768,9 +12522,7 @@
       <c r="K286" s="1">
         <v>10500</v>
       </c>
-      <c r="L286" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L286" s="1"/>
       <c r="M286" s="1"/>
       <c r="N286" s="1"/>
       <c r="O286" s="1">
@@ -12812,9 +12564,7 @@
       <c r="K287" s="1">
         <v>1100</v>
       </c>
-      <c r="L287" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L287" s="1"/>
       <c r="M287" s="1"/>
       <c r="N287" s="1"/>
       <c r="O287" s="1">
@@ -12856,9 +12606,7 @@
       <c r="K288" s="1">
         <v>15000</v>
       </c>
-      <c r="L288" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L288" s="1"/>
       <c r="M288" s="1"/>
       <c r="N288" s="1"/>
       <c r="O288" s="1">
@@ -12900,9 +12648,7 @@
       <c r="K289" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L289" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L289" s="1"/>
       <c r="M289" s="1"/>
       <c r="N289" s="1"/>
       <c r="O289" s="1">
@@ -12944,9 +12690,7 @@
       <c r="K290" s="1">
         <v>21000</v>
       </c>
-      <c r="L290" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L290" s="1"/>
       <c r="M290" s="1"/>
       <c r="N290" s="1"/>
       <c r="O290" s="1">
@@ -12988,9 +12732,7 @@
       <c r="K291" s="1">
         <v>48000</v>
       </c>
-      <c r="L291" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L291" s="1"/>
       <c r="M291" s="1"/>
       <c r="N291" s="1"/>
       <c r="O291" s="1">
@@ -13034,9 +12776,7 @@
       <c r="K292" s="1">
         <v>36000</v>
       </c>
-      <c r="L292" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L292" s="1"/>
       <c r="M292" s="1"/>
       <c r="N292" s="1"/>
       <c r="O292" s="1">
@@ -13080,9 +12820,7 @@
       <c r="K293" s="1">
         <v>18000</v>
       </c>
-      <c r="L293" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L293" s="1"/>
       <c r="M293" s="1"/>
       <c r="N293" s="1"/>
       <c r="O293" s="1">
@@ -13126,9 +12864,7 @@
       <c r="K294" s="1">
         <v>6000</v>
       </c>
-      <c r="L294" s="1">
-        <v>7000</v>
-      </c>
+      <c r="L294" s="1"/>
       <c r="M294" s="1"/>
       <c r="N294" s="1"/>
       <c r="O294" s="1">
@@ -13214,9 +12950,7 @@
       <c r="K296" s="1">
         <v>10500</v>
       </c>
-      <c r="L296" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L296" s="1"/>
       <c r="M296" s="1"/>
       <c r="N296" s="1"/>
       <c r="O296" s="1">
@@ -13258,9 +12992,7 @@
       <c r="K297" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L297" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L297" s="1"/>
       <c r="M297" s="1"/>
       <c r="N297" s="1"/>
       <c r="O297" s="1">
@@ -13302,9 +13034,7 @@
       <c r="K298" s="1">
         <v>1100</v>
       </c>
-      <c r="L298" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L298" s="1"/>
       <c r="M298" s="1"/>
       <c r="N298" s="1"/>
       <c r="O298" s="1">
@@ -13346,9 +13076,7 @@
       <c r="K299" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L299" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L299" s="1"/>
       <c r="M299" s="1"/>
       <c r="N299" s="1"/>
       <c r="O299" s="1">
@@ -13390,9 +13118,7 @@
       <c r="K300" s="1">
         <v>1100</v>
       </c>
-      <c r="L300" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L300" s="1"/>
       <c r="M300" s="1"/>
       <c r="N300" s="1"/>
       <c r="O300" s="1">
@@ -13434,9 +13160,7 @@
       <c r="K301" s="1">
         <v>36750</v>
       </c>
-      <c r="L301" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L301" s="1"/>
       <c r="M301" s="1"/>
       <c r="N301" s="1"/>
       <c r="O301" s="1">
@@ -13478,9 +13202,7 @@
       <c r="K302" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L302" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L302" s="1"/>
       <c r="M302" s="1"/>
       <c r="N302" s="1"/>
       <c r="O302" s="1">
@@ -13522,9 +13244,7 @@
       <c r="K303" s="1">
         <v>33333.332000000002</v>
       </c>
-      <c r="L303" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L303" s="1"/>
       <c r="M303" s="1"/>
       <c r="N303" s="1"/>
       <c r="O303" s="1">
@@ -13566,9 +13286,7 @@
       <c r="K304" s="1">
         <v>10500</v>
       </c>
-      <c r="L304" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L304" s="1"/>
       <c r="M304" s="1"/>
       <c r="N304" s="1"/>
       <c r="O304" s="1">
@@ -13610,9 +13328,7 @@
       <c r="K305" s="1">
         <v>26250</v>
       </c>
-      <c r="L305" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L305" s="1"/>
       <c r="M305" s="1"/>
       <c r="N305" s="1"/>
       <c r="O305" s="1">
@@ -13654,9 +13370,7 @@
       <c r="K306" s="1">
         <v>5000</v>
       </c>
-      <c r="L306" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L306" s="1"/>
       <c r="M306" s="1"/>
       <c r="N306" s="1"/>
       <c r="O306" s="1">
@@ -13698,9 +13412,7 @@
       <c r="K307" s="1">
         <v>21000</v>
       </c>
-      <c r="L307" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L307" s="1"/>
       <c r="M307" s="1"/>
       <c r="N307" s="1"/>
       <c r="O307" s="1">
@@ -13742,9 +13454,7 @@
       <c r="K308" s="1">
         <v>16750</v>
       </c>
-      <c r="L308" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L308" s="1"/>
       <c r="M308" s="1"/>
       <c r="N308" s="1"/>
       <c r="O308" s="1">
@@ -13786,9 +13496,7 @@
       <c r="K309" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L309" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L309" s="1"/>
       <c r="M309" s="1"/>
       <c r="N309" s="1"/>
       <c r="O309" s="1">
@@ -13830,9 +13538,7 @@
       <c r="K310" s="1">
         <v>21000</v>
       </c>
-      <c r="L310" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L310" s="1"/>
       <c r="M310" s="1"/>
       <c r="N310" s="1"/>
       <c r="O310" s="1">
@@ -13874,9 +13580,7 @@
       <c r="K311" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L311" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L311" s="1"/>
       <c r="M311" s="1"/>
       <c r="N311" s="1"/>
       <c r="O311" s="1">
@@ -13918,9 +13622,7 @@
       <c r="K312" s="1">
         <v>1100</v>
       </c>
-      <c r="L312" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L312" s="1"/>
       <c r="M312" s="1"/>
       <c r="N312" s="1"/>
       <c r="O312" s="1">
@@ -13962,9 +13664,7 @@
       <c r="K313" s="1">
         <v>10500</v>
       </c>
-      <c r="L313" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L313" s="1"/>
       <c r="M313" s="1"/>
       <c r="N313" s="1"/>
       <c r="O313" s="1">
@@ -14006,9 +13706,7 @@
       <c r="K314" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L314" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L314" s="1"/>
       <c r="M314" s="1"/>
       <c r="N314" s="1"/>
       <c r="O314" s="1">
@@ -14050,9 +13748,7 @@
       <c r="K315" s="1">
         <v>25000</v>
       </c>
-      <c r="L315" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L315" s="1"/>
       <c r="M315" s="1"/>
       <c r="N315" s="1"/>
       <c r="O315" s="1">
@@ -14094,9 +13790,7 @@
       <c r="K316" s="1">
         <v>15500</v>
       </c>
-      <c r="L316" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L316" s="1"/>
       <c r="M316" s="1"/>
       <c r="N316" s="1"/>
       <c r="O316" s="1">
@@ -14138,9 +13832,7 @@
       <c r="K317" s="1">
         <v>10500</v>
       </c>
-      <c r="L317" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L317" s="1"/>
       <c r="M317" s="1"/>
       <c r="N317" s="1"/>
       <c r="O317" s="1">
@@ -14182,9 +13874,7 @@
       <c r="K318" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L318" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L318" s="1"/>
       <c r="M318" s="1"/>
       <c r="N318" s="1"/>
       <c r="O318" s="1">
@@ -14226,9 +13916,7 @@
       <c r="K319" s="1">
         <v>10500</v>
       </c>
-      <c r="L319" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L319" s="1"/>
       <c r="M319" s="1"/>
       <c r="N319" s="1"/>
       <c r="O319" s="1">
@@ -14270,9 +13958,7 @@
       <c r="K320" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L320" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L320" s="1"/>
       <c r="M320" s="1"/>
       <c r="N320" s="1"/>
       <c r="O320" s="1">
@@ -14314,9 +14000,7 @@
       <c r="K321" s="1">
         <v>1100</v>
       </c>
-      <c r="L321" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L321" s="1"/>
       <c r="M321" s="1"/>
       <c r="N321" s="1"/>
       <c r="O321" s="1">
@@ -14358,9 +14042,7 @@
       <c r="K322" s="1">
         <v>5250</v>
       </c>
-      <c r="L322" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L322" s="1"/>
       <c r="M322" s="1"/>
       <c r="N322" s="1"/>
       <c r="O322" s="1">
@@ -14858,9 +14540,7 @@
       <c r="K334" s="1">
         <v>10500</v>
       </c>
-      <c r="L334" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L334" s="1"/>
       <c r="M334" s="1"/>
       <c r="N334" s="1"/>
       <c r="O334" s="1">
@@ -14902,9 +14582,7 @@
       <c r="K335" s="1">
         <v>30000</v>
       </c>
-      <c r="L335" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L335" s="1"/>
       <c r="M335" s="1"/>
       <c r="N335" s="1"/>
       <c r="O335" s="1">
@@ -14946,9 +14624,7 @@
       <c r="K336" s="1">
         <v>15500</v>
       </c>
-      <c r="L336" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L336" s="1"/>
       <c r="M336" s="1"/>
       <c r="N336" s="1"/>
       <c r="O336" s="1">
@@ -14990,9 +14666,7 @@
       <c r="K337" s="1">
         <v>16750</v>
       </c>
-      <c r="L337" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L337" s="1"/>
       <c r="M337" s="1"/>
       <c r="N337" s="1"/>
       <c r="O337" s="1">
@@ -15034,9 +14708,7 @@
       <c r="K338" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L338" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L338" s="1"/>
       <c r="M338" s="1"/>
       <c r="N338" s="1"/>
       <c r="O338" s="1">
@@ -15078,9 +14750,7 @@
       <c r="K339" s="1">
         <v>10500</v>
       </c>
-      <c r="L339" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L339" s="1"/>
       <c r="M339" s="1"/>
       <c r="N339" s="1"/>
       <c r="O339" s="1">
@@ -15122,9 +14792,7 @@
       <c r="K340" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L340" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L340" s="1"/>
       <c r="M340" s="1"/>
       <c r="N340" s="1"/>
       <c r="O340" s="1">
@@ -15166,9 +14834,7 @@
       <c r="K341" s="1">
         <v>21000</v>
       </c>
-      <c r="L341" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L341" s="1"/>
       <c r="M341" s="1"/>
       <c r="N341" s="1"/>
       <c r="O341" s="1">
@@ -15210,9 +14876,7 @@
       <c r="K342" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L342" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L342" s="1"/>
       <c r="M342" s="1"/>
       <c r="N342" s="1"/>
       <c r="O342" s="1">
@@ -15254,9 +14918,7 @@
       <c r="K343" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L343" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L343" s="1"/>
       <c r="M343" s="1"/>
       <c r="N343" s="1"/>
       <c r="O343" s="1">
@@ -15298,9 +14960,7 @@
       <c r="K344" s="1">
         <v>26250</v>
       </c>
-      <c r="L344" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L344" s="1"/>
       <c r="M344" s="1"/>
       <c r="N344" s="1"/>
       <c r="O344" s="1">
@@ -15342,9 +15002,7 @@
       <c r="K345" s="1">
         <v>16666.666000000001</v>
       </c>
-      <c r="L345" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L345" s="1"/>
       <c r="M345" s="1"/>
       <c r="N345" s="1"/>
       <c r="O345" s="1">
@@ -15386,9 +15044,7 @@
       <c r="K346" s="1">
         <v>12000</v>
       </c>
-      <c r="L346" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L346" s="1"/>
       <c r="M346" s="1"/>
       <c r="N346" s="1"/>
       <c r="O346" s="1">
@@ -15430,9 +15086,7 @@
       <c r="K347" s="1">
         <v>15750</v>
       </c>
-      <c r="L347" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L347" s="1"/>
       <c r="M347" s="1"/>
       <c r="N347" s="1"/>
       <c r="O347" s="1">
@@ -15474,9 +15128,7 @@
       <c r="K348" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L348" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L348" s="1"/>
       <c r="M348" s="1"/>
       <c r="N348" s="1"/>
       <c r="O348" s="1">
@@ -15518,9 +15170,7 @@
       <c r="K349" s="1">
         <v>17500</v>
       </c>
-      <c r="L349" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L349" s="1"/>
       <c r="M349" s="1"/>
       <c r="N349" s="1"/>
       <c r="O349" s="1">
@@ -15562,9 +15212,7 @@
       <c r="K350" s="1">
         <v>7500</v>
       </c>
-      <c r="L350" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L350" s="1"/>
       <c r="M350" s="1"/>
       <c r="N350" s="1"/>
       <c r="O350" s="1">
@@ -15606,9 +15254,7 @@
       <c r="K351" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L351" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L351" s="1"/>
       <c r="M351" s="1"/>
       <c r="N351" s="1"/>
       <c r="O351" s="1">
@@ -15650,9 +15296,7 @@
       <c r="K352" s="1">
         <v>1395.8334</v>
       </c>
-      <c r="L352" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L352" s="1"/>
       <c r="M352" s="1"/>
       <c r="N352" s="1"/>
       <c r="O352" s="1">
@@ -15694,9 +15338,7 @@
       <c r="K353" s="1">
         <v>15750</v>
       </c>
-      <c r="L353" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L353" s="1"/>
       <c r="M353" s="1"/>
       <c r="N353" s="1"/>
       <c r="O353" s="1">
@@ -15738,9 +15380,7 @@
       <c r="K354" s="1">
         <v>26250</v>
       </c>
-      <c r="L354" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L354" s="1"/>
       <c r="M354" s="1"/>
       <c r="N354" s="1"/>
       <c r="O354" s="1">
@@ -15782,9 +15422,7 @@
       <c r="K355" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L355" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L355" s="1"/>
       <c r="M355" s="1"/>
       <c r="N355" s="1"/>
       <c r="O355" s="1">
@@ -15826,9 +15464,7 @@
       <c r="K356" s="1">
         <v>15500</v>
       </c>
-      <c r="L356" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L356" s="1"/>
       <c r="M356" s="1"/>
       <c r="N356" s="1"/>
       <c r="O356" s="1">
@@ -15870,9 +15506,7 @@
       <c r="K357" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L357" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L357" s="1"/>
       <c r="M357" s="1"/>
       <c r="N357" s="1"/>
       <c r="O357" s="1">
@@ -15914,9 +15548,7 @@
       <c r="K358" s="1">
         <v>1875</v>
       </c>
-      <c r="L358" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L358" s="1"/>
       <c r="M358" s="1"/>
       <c r="N358" s="1"/>
       <c r="O358" s="1">
@@ -15958,9 +15590,7 @@
       <c r="K359" s="1">
         <v>1875</v>
       </c>
-      <c r="L359" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L359" s="1"/>
       <c r="M359" s="1"/>
       <c r="N359" s="1"/>
       <c r="O359" s="1">
@@ -16002,9 +15632,7 @@
       <c r="K360" s="1">
         <v>5000</v>
       </c>
-      <c r="L360" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L360" s="1"/>
       <c r="M360" s="1"/>
       <c r="N360" s="1"/>
       <c r="O360" s="1">
@@ -16046,9 +15674,7 @@
       <c r="K361" s="1">
         <v>21000</v>
       </c>
-      <c r="L361" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L361" s="1"/>
       <c r="M361" s="1"/>
       <c r="N361" s="1"/>
       <c r="O361" s="1">
@@ -16090,9 +15716,7 @@
       <c r="K362" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L362" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L362" s="1"/>
       <c r="M362" s="1"/>
       <c r="N362" s="1"/>
       <c r="O362" s="1">
@@ -16938,9 +16562,7 @@
       <c r="K384" s="1">
         <v>2400</v>
       </c>
-      <c r="L384" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L384" s="1"/>
       <c r="M384" s="1"/>
       <c r="N384" s="1"/>
       <c r="O384" s="1">
@@ -16982,9 +16604,7 @@
       <c r="K385" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L385" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L385" s="1"/>
       <c r="M385" s="1"/>
       <c r="N385" s="1"/>
       <c r="O385" s="1">
@@ -17026,9 +16646,7 @@
       <c r="K386" s="1">
         <v>10500</v>
       </c>
-      <c r="L386" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L386" s="1"/>
       <c r="M386" s="1"/>
       <c r="N386" s="1"/>
       <c r="O386" s="1">
@@ -17070,9 +16688,7 @@
       <c r="K387" s="1">
         <v>5000</v>
       </c>
-      <c r="L387" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L387" s="1"/>
       <c r="M387" s="1"/>
       <c r="N387" s="1"/>
       <c r="O387" s="1">
@@ -17114,9 +16730,7 @@
       <c r="K388" s="1">
         <v>16666.666000000001</v>
       </c>
-      <c r="L388" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L388" s="1"/>
       <c r="M388" s="1"/>
       <c r="N388" s="1"/>
       <c r="O388" s="1">
@@ -17158,9 +16772,7 @@
       <c r="K389" s="1">
         <v>10500</v>
       </c>
-      <c r="L389" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L389" s="1"/>
       <c r="M389" s="1"/>
       <c r="N389" s="1"/>
       <c r="O389" s="1">
@@ -17202,9 +16814,7 @@
       <c r="K390" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L390" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L390" s="1"/>
       <c r="M390" s="1"/>
       <c r="N390" s="1"/>
       <c r="O390" s="1">
@@ -17246,9 +16856,7 @@
       <c r="K391" s="1">
         <v>3750</v>
       </c>
-      <c r="L391" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L391" s="1"/>
       <c r="M391" s="1"/>
       <c r="N391" s="1"/>
       <c r="O391" s="1">
@@ -17290,9 +16898,7 @@
       <c r="K392" s="1">
         <v>3750</v>
       </c>
-      <c r="L392" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L392" s="1"/>
       <c r="M392" s="1"/>
       <c r="N392" s="1"/>
       <c r="O392" s="1">
@@ -17334,9 +16940,7 @@
       <c r="K393" s="1">
         <v>10500</v>
       </c>
-      <c r="L393" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L393" s="1"/>
       <c r="M393" s="1"/>
       <c r="N393" s="1"/>
       <c r="O393" s="1">
@@ -17378,9 +16982,7 @@
       <c r="K394" s="1">
         <v>5000</v>
       </c>
-      <c r="L394" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L394" s="1"/>
       <c r="M394" s="1"/>
       <c r="N394" s="1"/>
       <c r="O394" s="1">
@@ -17422,9 +17024,7 @@
       <c r="K395" s="1">
         <v>1875</v>
       </c>
-      <c r="L395" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L395" s="1"/>
       <c r="M395" s="1"/>
       <c r="N395" s="1"/>
       <c r="O395" s="1">
@@ -17466,9 +17066,7 @@
       <c r="K396" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L396" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L396" s="1"/>
       <c r="M396" s="1"/>
       <c r="N396" s="1"/>
       <c r="O396" s="1">
@@ -17510,9 +17108,7 @@
       <c r="K397" s="1">
         <v>15750</v>
       </c>
-      <c r="L397" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L397" s="1"/>
       <c r="M397" s="1"/>
       <c r="N397" s="1"/>
       <c r="O397" s="1">
@@ -17554,9 +17150,7 @@
       <c r="K398" s="1">
         <v>8750</v>
       </c>
-      <c r="L398" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L398" s="1"/>
       <c r="M398" s="1"/>
       <c r="N398" s="1"/>
       <c r="O398" s="1">
@@ -17598,9 +17192,7 @@
       <c r="K399" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L399" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L399" s="1"/>
       <c r="M399" s="1"/>
       <c r="N399" s="1"/>
       <c r="O399" s="1">
@@ -17642,9 +17234,7 @@
       <c r="K400" s="1">
         <v>10000</v>
       </c>
-      <c r="L400" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L400" s="1"/>
       <c r="M400" s="1"/>
       <c r="N400" s="1"/>
       <c r="O400" s="1">
@@ -17686,9 +17276,7 @@
       <c r="K401" s="1">
         <v>2791.6667000000002</v>
       </c>
-      <c r="L401" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L401" s="1"/>
       <c r="M401" s="1"/>
       <c r="N401" s="1"/>
       <c r="O401" s="1">
@@ -17730,9 +17318,7 @@
       <c r="K402" s="1">
         <v>2791.6667000000002</v>
       </c>
-      <c r="L402" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L402" s="1"/>
       <c r="M402" s="1"/>
       <c r="N402" s="1"/>
       <c r="O402" s="1">
@@ -17774,9 +17360,7 @@
       <c r="K403" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L403" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L403" s="1"/>
       <c r="M403" s="1"/>
       <c r="N403" s="1"/>
       <c r="O403" s="1">
@@ -17818,9 +17402,7 @@
       <c r="K404" s="1">
         <v>1200</v>
       </c>
-      <c r="L404" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L404" s="1"/>
       <c r="M404" s="1"/>
       <c r="N404" s="1"/>
       <c r="O404" s="1">
@@ -17862,9 +17444,7 @@
       <c r="K405" s="1">
         <v>600</v>
       </c>
-      <c r="L405" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L405" s="1"/>
       <c r="M405" s="1"/>
       <c r="N405" s="1"/>
       <c r="O405" s="1">
@@ -17906,9 +17486,7 @@
       <c r="K406" s="1">
         <v>750</v>
       </c>
-      <c r="L406" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L406" s="1"/>
       <c r="M406" s="1"/>
       <c r="N406" s="1"/>
       <c r="O406" s="1">
@@ -17950,9 +17528,7 @@
       <c r="K407" s="1">
         <v>1666.6666</v>
       </c>
-      <c r="L407" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L407" s="1"/>
       <c r="M407" s="1"/>
       <c r="N407" s="1"/>
       <c r="O407" s="1">
@@ -17994,9 +17570,7 @@
       <c r="K408" s="1">
         <v>2000</v>
       </c>
-      <c r="L408" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L408" s="1"/>
       <c r="M408" s="1"/>
       <c r="N408" s="1"/>
       <c r="O408" s="1">
@@ -18038,9 +17612,7 @@
       <c r="K409" s="1">
         <v>15750</v>
       </c>
-      <c r="L409" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L409" s="1"/>
       <c r="M409" s="1"/>
       <c r="N409" s="1"/>
       <c r="O409" s="1">
@@ -18082,9 +17654,7 @@
       <c r="K410" s="1">
         <v>13333.333000000001</v>
       </c>
-      <c r="L410" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L410" s="1"/>
       <c r="M410" s="1"/>
       <c r="N410" s="1"/>
       <c r="O410" s="1">
@@ -18126,9 +17696,7 @@
       <c r="K411" s="1">
         <v>3750</v>
       </c>
-      <c r="L411" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L411" s="1"/>
       <c r="M411" s="1"/>
       <c r="N411" s="1"/>
       <c r="O411" s="1">
@@ -18170,9 +17738,7 @@
       <c r="K412" s="1">
         <v>3750</v>
       </c>
-      <c r="L412" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L412" s="1"/>
       <c r="M412" s="1"/>
       <c r="N412" s="1"/>
       <c r="O412" s="1">
@@ -18214,9 +17780,7 @@
       <c r="K413" s="1">
         <v>15000</v>
       </c>
-      <c r="L413" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L413" s="1"/>
       <c r="M413" s="1"/>
       <c r="N413" s="1"/>
       <c r="O413" s="1">
@@ -18258,9 +17822,7 @@
       <c r="K414" s="1">
         <v>10000</v>
       </c>
-      <c r="L414" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L414" s="1"/>
       <c r="M414" s="1"/>
       <c r="N414" s="1"/>
       <c r="O414" s="1">
@@ -18302,9 +17864,7 @@
       <c r="K415" s="1">
         <v>16750</v>
       </c>
-      <c r="L415" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L415" s="1"/>
       <c r="M415" s="1"/>
       <c r="N415" s="1"/>
       <c r="O415" s="1">
@@ -18346,9 +17906,7 @@
       <c r="K416" s="1">
         <v>5250</v>
       </c>
-      <c r="L416" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L416" s="1"/>
       <c r="M416" s="1"/>
       <c r="N416" s="1"/>
       <c r="O416" s="1">
@@ -18390,9 +17948,7 @@
       <c r="K417" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L417" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L417" s="1"/>
       <c r="M417" s="1"/>
       <c r="N417" s="1"/>
       <c r="O417" s="1">
@@ -18434,9 +17990,7 @@
       <c r="K418" s="1">
         <v>26250</v>
       </c>
-      <c r="L418" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L418" s="1"/>
       <c r="M418" s="1"/>
       <c r="N418" s="1"/>
       <c r="O418" s="1">
@@ -18478,9 +18032,7 @@
       <c r="K419" s="1">
         <v>5000</v>
       </c>
-      <c r="L419" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L419" s="1"/>
       <c r="M419" s="1"/>
       <c r="N419" s="1"/>
       <c r="O419" s="1">
@@ -18522,9 +18074,7 @@
       <c r="K420" s="1">
         <v>24000</v>
       </c>
-      <c r="L420" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L420" s="1"/>
       <c r="M420" s="1"/>
       <c r="N420" s="1"/>
       <c r="O420" s="1">
@@ -18568,9 +18118,7 @@
       <c r="K421" s="1">
         <v>21600</v>
       </c>
-      <c r="L421" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L421" s="1"/>
       <c r="M421" s="1"/>
       <c r="N421" s="1"/>
       <c r="O421" s="1">
@@ -18614,9 +18162,7 @@
       <c r="K422" s="1">
         <v>4800</v>
       </c>
-      <c r="L422" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L422" s="1"/>
       <c r="M422" s="1"/>
       <c r="N422" s="1"/>
       <c r="O422" s="1">
@@ -18660,9 +18206,7 @@
       <c r="K423" s="1">
         <v>6000</v>
       </c>
-      <c r="L423" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L423" s="1"/>
       <c r="M423" s="1"/>
       <c r="N423" s="1"/>
       <c r="O423" s="1">
@@ -18706,9 +18250,7 @@
       <c r="K424" s="1">
         <v>7500</v>
       </c>
-      <c r="L424" s="1">
-        <v>2500</v>
-      </c>
+      <c r="L424" s="1"/>
       <c r="M424" s="1"/>
       <c r="N424" s="1"/>
       <c r="O424" s="1">
@@ -20076,9 +19618,7 @@
       <c r="K459" s="1">
         <v>5250</v>
       </c>
-      <c r="L459" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L459" s="1"/>
       <c r="M459" s="1"/>
       <c r="N459" s="1"/>
       <c r="O459" s="1">
@@ -20120,9 +19660,7 @@
       <c r="K460" s="1">
         <v>1500</v>
       </c>
-      <c r="L460" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L460" s="1"/>
       <c r="M460" s="1"/>
       <c r="N460" s="1"/>
       <c r="O460" s="1">
@@ -20164,9 +19702,7 @@
       <c r="K461" s="1">
         <v>2000</v>
       </c>
-      <c r="L461" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L461" s="1"/>
       <c r="M461" s="1"/>
       <c r="N461" s="1"/>
       <c r="O461" s="1">
@@ -20208,9 +19744,7 @@
       <c r="K462" s="1">
         <v>10500</v>
       </c>
-      <c r="L462" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L462" s="1"/>
       <c r="M462" s="1"/>
       <c r="N462" s="1"/>
       <c r="O462" s="1">
@@ -20252,9 +19786,7 @@
       <c r="K463" s="1">
         <v>21000</v>
       </c>
-      <c r="L463" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L463" s="1"/>
       <c r="M463" s="1"/>
       <c r="N463" s="1"/>
       <c r="O463" s="1">
@@ -20296,9 +19828,7 @@
       <c r="K464" s="1">
         <v>10500</v>
       </c>
-      <c r="L464" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L464" s="1"/>
       <c r="M464" s="1"/>
       <c r="N464" s="1"/>
       <c r="O464" s="1">
@@ -20340,9 +19870,7 @@
       <c r="K465" s="1">
         <v>18000</v>
       </c>
-      <c r="L465" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L465" s="1"/>
       <c r="M465" s="1"/>
       <c r="N465" s="1"/>
       <c r="O465" s="1">
@@ -20384,9 +19912,7 @@
       <c r="K466" s="1">
         <v>10500</v>
       </c>
-      <c r="L466" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L466" s="1"/>
       <c r="M466" s="1"/>
       <c r="N466" s="1"/>
       <c r="O466" s="1">
@@ -20428,9 +19954,7 @@
       <c r="K467" s="1">
         <v>10500</v>
       </c>
-      <c r="L467" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L467" s="1"/>
       <c r="M467" s="1"/>
       <c r="N467" s="1"/>
       <c r="O467" s="1">
@@ -20472,9 +19996,7 @@
       <c r="K468" s="1">
         <v>10500</v>
       </c>
-      <c r="L468" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L468" s="1"/>
       <c r="M468" s="1"/>
       <c r="N468" s="1"/>
       <c r="O468" s="1">
@@ -20516,9 +20038,7 @@
       <c r="K469" s="1">
         <v>31500</v>
       </c>
-      <c r="L469" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L469" s="1"/>
       <c r="M469" s="1"/>
       <c r="N469" s="1"/>
       <c r="O469" s="1">
@@ -20560,9 +20080,7 @@
       <c r="K470" s="1">
         <v>750</v>
       </c>
-      <c r="L470" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L470" s="1"/>
       <c r="M470" s="1"/>
       <c r="N470" s="1"/>
       <c r="O470" s="1">
@@ -20604,9 +20122,7 @@
       <c r="K471" s="1">
         <v>2791.6667000000002</v>
       </c>
-      <c r="L471" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L471" s="1"/>
       <c r="M471" s="1"/>
       <c r="N471" s="1"/>
       <c r="O471" s="1">
@@ -20648,9 +20164,7 @@
       <c r="K472" s="1">
         <v>729.16669999999999</v>
       </c>
-      <c r="L472" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L472" s="1"/>
       <c r="M472" s="1"/>
       <c r="N472" s="1"/>
       <c r="O472" s="1">
@@ -20692,9 +20206,7 @@
       <c r="K473" s="1">
         <v>10500</v>
       </c>
-      <c r="L473" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L473" s="1"/>
       <c r="M473" s="1"/>
       <c r="N473" s="1"/>
       <c r="O473" s="1">
@@ -20736,9 +20248,7 @@
       <c r="K474" s="1">
         <v>5625</v>
       </c>
-      <c r="L474" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L474" s="1"/>
       <c r="M474" s="1"/>
       <c r="N474" s="1"/>
       <c r="O474" s="1">
@@ -20780,9 +20290,7 @@
       <c r="K475" s="1">
         <v>15000</v>
       </c>
-      <c r="L475" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L475" s="1"/>
       <c r="M475" s="1"/>
       <c r="N475" s="1"/>
       <c r="O475" s="1">
@@ -20824,9 +20332,7 @@
       <c r="K476" s="1">
         <v>26250</v>
       </c>
-      <c r="L476" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L476" s="1"/>
       <c r="M476" s="1"/>
       <c r="N476" s="1"/>
       <c r="O476" s="1">
@@ -20868,9 +20374,7 @@
       <c r="K477" s="1">
         <v>8750</v>
       </c>
-      <c r="L477" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L477" s="1"/>
       <c r="M477" s="1"/>
       <c r="N477" s="1"/>
       <c r="O477" s="1">
@@ -20912,9 +20416,7 @@
       <c r="K478" s="1">
         <v>21000</v>
       </c>
-      <c r="L478" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L478" s="1"/>
       <c r="M478" s="1"/>
       <c r="N478" s="1"/>
       <c r="O478" s="1">
@@ -20956,9 +20458,7 @@
       <c r="K479" s="1">
         <v>8750</v>
       </c>
-      <c r="L479" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L479" s="1"/>
       <c r="M479" s="1"/>
       <c r="N479" s="1"/>
       <c r="O479" s="1">
@@ -21000,9 +20500,7 @@
       <c r="K480" s="1">
         <v>7750</v>
       </c>
-      <c r="L480" s="1">
-        <v>3000</v>
-      </c>
+      <c r="L480" s="1"/>
       <c r="M480" s="1"/>
       <c r="N480" s="1"/>
       <c r="O480" s="1">
@@ -23444,9 +22942,7 @@
       <c r="K544" s="1">
         <v>6000</v>
       </c>
-      <c r="L544" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L544" s="1"/>
       <c r="M544" s="1"/>
       <c r="N544" s="1"/>
       <c r="O544" s="1">
@@ -23488,9 +22984,7 @@
       <c r="K545" s="1">
         <v>1666.6666</v>
       </c>
-      <c r="L545" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L545" s="1"/>
       <c r="M545" s="1"/>
       <c r="N545" s="1"/>
       <c r="O545" s="1">
@@ -23532,9 +23026,7 @@
       <c r="K546" s="1">
         <v>30000</v>
       </c>
-      <c r="L546" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L546" s="1"/>
       <c r="M546" s="1"/>
       <c r="N546" s="1"/>
       <c r="O546" s="1">
@@ -23576,9 +23068,7 @@
       <c r="K547" s="1">
         <v>26250</v>
       </c>
-      <c r="L547" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L547" s="1"/>
       <c r="M547" s="1"/>
       <c r="N547" s="1"/>
       <c r="O547" s="1">
@@ -23620,9 +23110,7 @@
       <c r="K548" s="1">
         <v>4800</v>
       </c>
-      <c r="L548" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L548" s="1"/>
       <c r="M548" s="1"/>
       <c r="N548" s="1"/>
       <c r="O548" s="1">
@@ -23664,9 +23152,7 @@
       <c r="K549" s="1">
         <v>10000</v>
       </c>
-      <c r="L549" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L549" s="1"/>
       <c r="M549" s="1"/>
       <c r="N549" s="1"/>
       <c r="O549" s="1">
@@ -23708,9 +23194,7 @@
       <c r="K550" s="1">
         <v>3750</v>
       </c>
-      <c r="L550" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L550" s="1"/>
       <c r="M550" s="1"/>
       <c r="N550" s="1"/>
       <c r="O550" s="1">
@@ -23752,9 +23236,7 @@
       <c r="K551" s="1">
         <v>3750</v>
       </c>
-      <c r="L551" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L551" s="1"/>
       <c r="M551" s="1"/>
       <c r="N551" s="1"/>
       <c r="O551" s="1">
@@ -23796,9 +23278,7 @@
       <c r="K552" s="1">
         <v>31500</v>
       </c>
-      <c r="L552" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L552" s="1"/>
       <c r="M552" s="1"/>
       <c r="N552" s="1"/>
       <c r="O552" s="1">
@@ -23840,9 +23320,7 @@
       <c r="K553" s="1">
         <v>5000</v>
       </c>
-      <c r="L553" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L553" s="1"/>
       <c r="M553" s="1"/>
       <c r="N553" s="1"/>
       <c r="O553" s="1">
@@ -23884,9 +23362,7 @@
       <c r="K554" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L554" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L554" s="1"/>
       <c r="M554" s="1"/>
       <c r="N554" s="1"/>
       <c r="O554" s="1">
@@ -23928,9 +23404,7 @@
       <c r="K555" s="1">
         <v>3750</v>
       </c>
-      <c r="L555" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L555" s="1"/>
       <c r="M555" s="1"/>
       <c r="N555" s="1"/>
       <c r="O555" s="1">
@@ -23972,9 +23446,7 @@
       <c r="K556" s="1">
         <v>12000</v>
       </c>
-      <c r="L556" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L556" s="1"/>
       <c r="M556" s="1"/>
       <c r="N556" s="1"/>
       <c r="O556" s="1">
@@ -24016,9 +23488,7 @@
       <c r="K557" s="1">
         <v>10500</v>
       </c>
-      <c r="L557" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L557" s="1"/>
       <c r="M557" s="1"/>
       <c r="N557" s="1"/>
       <c r="O557" s="1">
@@ -24060,9 +23530,7 @@
       <c r="K558" s="1">
         <v>17500</v>
       </c>
-      <c r="L558" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L558" s="1"/>
       <c r="M558" s="1"/>
       <c r="N558" s="1"/>
       <c r="O558" s="1">
@@ -24104,9 +23572,7 @@
       <c r="K559" s="1">
         <v>42000</v>
       </c>
-      <c r="L559" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L559" s="1"/>
       <c r="M559" s="1"/>
       <c r="N559" s="1"/>
       <c r="O559" s="1">
@@ -24148,9 +23614,7 @@
       <c r="K560" s="1">
         <v>10500</v>
       </c>
-      <c r="L560" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L560" s="1"/>
       <c r="M560" s="1"/>
       <c r="N560" s="1"/>
       <c r="O560" s="1">
@@ -24192,9 +23656,7 @@
       <c r="K561" s="1">
         <v>5000</v>
       </c>
-      <c r="L561" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L561" s="1"/>
       <c r="M561" s="1"/>
       <c r="N561" s="1"/>
       <c r="O561" s="1">
@@ -24236,9 +23698,7 @@
       <c r="K562" s="1">
         <v>21000</v>
       </c>
-      <c r="L562" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L562" s="1"/>
       <c r="M562" s="1"/>
       <c r="N562" s="1"/>
       <c r="O562" s="1">
@@ -24280,9 +23740,7 @@
       <c r="K563" s="1">
         <v>21000</v>
       </c>
-      <c r="L563" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L563" s="1"/>
       <c r="M563" s="1"/>
       <c r="N563" s="1"/>
       <c r="O563" s="1">
@@ -24324,9 +23782,7 @@
       <c r="K564" s="1">
         <v>21000</v>
       </c>
-      <c r="L564" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L564" s="1"/>
       <c r="M564" s="1"/>
       <c r="N564" s="1"/>
       <c r="O564" s="1">
@@ -24368,9 +23824,7 @@
       <c r="K565" s="1">
         <v>31000</v>
       </c>
-      <c r="L565" s="1">
-        <v>2000</v>
-      </c>
+      <c r="L565" s="1"/>
       <c r="M565" s="1"/>
       <c r="N565" s="1"/>
       <c r="O565" s="1">
@@ -24458,12 +23912,8 @@
       <c r="K567" s="1">
         <v>30000</v>
       </c>
-      <c r="L567" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M567" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L567" s="1"/>
+      <c r="M567" s="1"/>
       <c r="N567" s="1"/>
       <c r="O567" s="1">
         <v>1511</v>
@@ -24504,12 +23954,8 @@
       <c r="K568" s="1">
         <v>8750</v>
       </c>
-      <c r="L568" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M568" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L568" s="1"/>
+      <c r="M568" s="1"/>
       <c r="N568" s="1"/>
       <c r="O568" s="1">
         <v>1512</v>
@@ -24550,12 +23996,8 @@
       <c r="K569" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L569" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M569" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L569" s="1"/>
+      <c r="M569" s="1"/>
       <c r="N569" s="1"/>
       <c r="O569" s="1">
         <v>1513</v>
@@ -24596,12 +24038,8 @@
       <c r="K570" s="1">
         <v>10500</v>
       </c>
-      <c r="L570" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M570" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L570" s="1"/>
+      <c r="M570" s="1"/>
       <c r="N570" s="1"/>
       <c r="O570" s="1">
         <v>1514</v>
@@ -24642,12 +24080,8 @@
       <c r="K571" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L571" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M571" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L571" s="1"/>
+      <c r="M571" s="1"/>
       <c r="N571" s="1"/>
       <c r="O571" s="1">
         <v>1515</v>
@@ -24688,12 +24122,8 @@
       <c r="K572" s="1">
         <v>5250</v>
       </c>
-      <c r="L572" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M572" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L572" s="1"/>
+      <c r="M572" s="1"/>
       <c r="N572" s="1"/>
       <c r="O572" s="1">
         <v>1516</v>
@@ -24734,12 +24164,8 @@
       <c r="K573" s="1">
         <v>6666.6665000000003</v>
       </c>
-      <c r="L573" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M573" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L573" s="1"/>
+      <c r="M573" s="1"/>
       <c r="N573" s="1"/>
       <c r="O573" s="1">
         <v>1517</v>
@@ -24780,12 +24206,8 @@
       <c r="K574" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L574" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M574" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L574" s="1"/>
+      <c r="M574" s="1"/>
       <c r="N574" s="1"/>
       <c r="O574" s="1">
         <v>1518</v>
@@ -24826,12 +24248,8 @@
       <c r="K575" s="1">
         <v>10500</v>
       </c>
-      <c r="L575" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M575" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L575" s="1"/>
+      <c r="M575" s="1"/>
       <c r="N575" s="1"/>
       <c r="O575" s="1">
         <v>1519</v>
@@ -24872,12 +24290,8 @@
       <c r="K576" s="1">
         <v>31500</v>
       </c>
-      <c r="L576" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M576" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L576" s="1"/>
+      <c r="M576" s="1"/>
       <c r="N576" s="1"/>
       <c r="O576" s="1">
         <v>1520</v>
@@ -24918,12 +24332,8 @@
       <c r="K577" s="1">
         <v>7500</v>
       </c>
-      <c r="L577" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M577" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L577" s="1"/>
+      <c r="M577" s="1"/>
       <c r="N577" s="1"/>
       <c r="O577" s="1">
         <v>1521</v>
@@ -24964,12 +24374,8 @@
       <c r="K578" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L578" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M578" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L578" s="1"/>
+      <c r="M578" s="1"/>
       <c r="N578" s="1"/>
       <c r="O578" s="1">
         <v>1522</v>
@@ -25010,12 +24416,8 @@
       <c r="K579" s="1">
         <v>10500</v>
       </c>
-      <c r="L579" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M579" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L579" s="1"/>
+      <c r="M579" s="1"/>
       <c r="N579" s="1"/>
       <c r="O579" s="1">
         <v>1523</v>
@@ -25056,12 +24458,8 @@
       <c r="K580" s="1">
         <v>10000</v>
       </c>
-      <c r="L580" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M580" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L580" s="1"/>
+      <c r="M580" s="1"/>
       <c r="N580" s="1"/>
       <c r="O580" s="1">
         <v>1524</v>
@@ -25102,12 +24500,8 @@
       <c r="K581" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L581" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M581" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L581" s="1"/>
+      <c r="M581" s="1"/>
       <c r="N581" s="1"/>
       <c r="O581" s="1">
         <v>1525</v>
@@ -25148,12 +24542,8 @@
       <c r="K582" s="1">
         <v>10500</v>
       </c>
-      <c r="L582" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M582" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L582" s="1"/>
+      <c r="M582" s="1"/>
       <c r="N582" s="1"/>
       <c r="O582" s="1">
         <v>1526</v>
@@ -25194,12 +24584,8 @@
       <c r="K583" s="1">
         <v>16666.666000000001</v>
       </c>
-      <c r="L583" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M583" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L583" s="1"/>
+      <c r="M583" s="1"/>
       <c r="N583" s="1"/>
       <c r="O583" s="1">
         <v>1527</v>
@@ -25240,12 +24626,8 @@
       <c r="K584" s="1">
         <v>16750</v>
       </c>
-      <c r="L584" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M584" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L584" s="1"/>
+      <c r="M584" s="1"/>
       <c r="N584" s="1"/>
       <c r="O584" s="1">
         <v>1528</v>
@@ -25286,12 +24668,8 @@
       <c r="K585" s="1">
         <v>5250</v>
       </c>
-      <c r="L585" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M585" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L585" s="1"/>
+      <c r="M585" s="1"/>
       <c r="N585" s="1"/>
       <c r="O585" s="1">
         <v>1529</v>
@@ -25332,12 +24710,8 @@
       <c r="K586" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L586" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M586" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L586" s="1"/>
+      <c r="M586" s="1"/>
       <c r="N586" s="1"/>
       <c r="O586" s="1">
         <v>1530</v>
@@ -25378,12 +24752,8 @@
       <c r="K587" s="1">
         <v>10500</v>
       </c>
-      <c r="L587" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M587" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L587" s="1"/>
+      <c r="M587" s="1"/>
       <c r="N587" s="1"/>
       <c r="O587" s="1">
         <v>1531</v>
@@ -25424,12 +24794,8 @@
       <c r="K588" s="1">
         <v>3333.3332999999998</v>
       </c>
-      <c r="L588" s="1">
-        <v>10500</v>
-      </c>
-      <c r="M588" s="1">
-        <v>6000</v>
-      </c>
+      <c r="L588" s="1"/>
+      <c r="M588" s="1"/>
       <c r="N588" s="1"/>
       <c r="O588" s="1">
         <v>1532</v>

</xml_diff>